<commit_message>
nouveau ajout derniere fonction chcab att j
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B5D026-C468-7F42-9B0D-D9A7E658636E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16270FC1-9EC2-CA4B-96B5-AFC4D23B2327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ETPT Format DDG'!$A$2:$DT$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$80</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="378">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -2494,6 +2494,18 @@
   </si>
   <si>
     <t>ajouter ? JA Pôle Social,JA Parquet,JA JP,JA VIF</t>
+  </si>
+  <si>
+    <t>A GREFFIER</t>
+  </si>
+  <si>
+    <t>à valider</t>
+  </si>
+  <si>
+    <t>Att. J</t>
+  </si>
+  <si>
+    <t>ATTACHÉ DE JUSTICE</t>
   </si>
 </sst>
 </file>
@@ -2847,7 +2859,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2989,6 +3001,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3389,7 +3407,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3926,6 +3944,21 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -6851,10 +6884,10 @@
   <sheetPr codeName="Feuil14">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
     <sheetView zoomScale="118" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7187,7 +7220,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="137" t="s">
         <v>79</v>
       </c>
@@ -7207,7 +7240,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="137" t="s">
         <v>79</v>
       </c>
@@ -7227,35 +7260,38 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="137" t="s">
+    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="181" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="132" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="B19" s="182" t="s">
+        <v>374</v>
+      </c>
+      <c r="C19" s="183" t="s">
+        <v>374</v>
+      </c>
+      <c r="D19" s="183" t="s">
         <v>88</v>
       </c>
-      <c r="E19" s="136" t="s">
+      <c r="E19" s="184" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="134" t="s">
+      <c r="F19" s="185" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="G19" s="35" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="137" t="s">
         <v>79</v>
       </c>
       <c r="B20" s="132" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>88</v>
@@ -7267,15 +7303,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="137" t="s">
         <v>79</v>
       </c>
       <c r="B21" s="132" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>88</v>
@@ -7287,15 +7323,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="137" t="s">
         <v>79</v>
       </c>
       <c r="B22" s="132" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>88</v>
@@ -7307,15 +7343,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="137" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="132" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>88</v>
@@ -7324,30 +7360,30 @@
         <v>45</v>
       </c>
       <c r="F23" s="134" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="137" t="s">
         <v>79</v>
       </c>
       <c r="B24" s="132" t="s">
-        <v>327</v>
+        <v>51</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>327</v>
+        <v>51</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="138" t="s">
-        <v>53</v>
+        <v>88</v>
+      </c>
+      <c r="E24" s="136" t="s">
+        <v>45</v>
       </c>
       <c r="F24" s="134" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="137" t="s">
         <v>79</v>
       </c>
@@ -7355,7 +7391,7 @@
         <v>327</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>358</v>
+        <v>327</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>87</v>
@@ -7367,7 +7403,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="137" t="s">
         <v>79</v>
       </c>
@@ -7375,39 +7411,39 @@
         <v>327</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E26" s="138" t="s">
-        <v>360</v>
+        <v>53</v>
       </c>
       <c r="F26" s="134" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="137" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="132" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>329</v>
+        <v>359</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E27" s="138" t="s">
-        <v>53</v>
+        <v>360</v>
       </c>
       <c r="F27" s="134" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="137" t="s">
         <v>79</v>
       </c>
@@ -7415,7 +7451,7 @@
         <v>328</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>362</v>
+        <v>329</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>87</v>
@@ -7427,7 +7463,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="137" t="s">
         <v>79</v>
       </c>
@@ -7435,39 +7471,39 @@
         <v>328</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E29" s="138" t="s">
-        <v>360</v>
+        <v>53</v>
       </c>
       <c r="F29" s="134" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="137" t="s">
         <v>79</v>
       </c>
       <c r="B30" s="132" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>330</v>
+        <v>363</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E30" s="138" t="s">
-        <v>53</v>
+        <v>360</v>
       </c>
       <c r="F30" s="134" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="137" t="s">
         <v>79</v>
       </c>
@@ -7475,7 +7511,7 @@
         <v>330</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>364</v>
+        <v>330</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>87</v>
@@ -7487,7 +7523,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="137" t="s">
         <v>79</v>
       </c>
@@ -7495,16 +7531,16 @@
         <v>330</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E32" s="138" t="s">
-        <v>360</v>
+        <v>53</v>
       </c>
       <c r="F32" s="134" t="s">
-        <v>361</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7512,19 +7548,19 @@
         <v>79</v>
       </c>
       <c r="B33" s="132" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>331</v>
+        <v>365</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E33" s="138" t="s">
-        <v>53</v>
+        <v>360</v>
       </c>
       <c r="F33" s="134" t="s">
-        <v>54</v>
+        <v>361</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7535,7 +7571,7 @@
         <v>331</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>366</v>
+        <v>331</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>87</v>
@@ -7555,16 +7591,16 @@
         <v>331</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E35" s="138" t="s">
-        <v>360</v>
+        <v>53</v>
       </c>
       <c r="F35" s="134" t="s">
-        <v>361</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7572,19 +7608,19 @@
         <v>79</v>
       </c>
       <c r="B36" s="132" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>332</v>
+        <v>367</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E36" s="138" t="s">
-        <v>53</v>
+        <v>360</v>
       </c>
       <c r="F36" s="134" t="s">
-        <v>55</v>
+        <v>361</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7595,7 +7631,7 @@
         <v>332</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>368</v>
+        <v>332</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>87</v>
@@ -7615,16 +7651,16 @@
         <v>332</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E38" s="138" t="s">
-        <v>360</v>
+        <v>53</v>
       </c>
       <c r="F38" s="134" t="s">
-        <v>370</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7632,28 +7668,30 @@
         <v>79</v>
       </c>
       <c r="B39" s="132" t="s">
-        <v>86</v>
+        <v>332</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>56</v>
+        <v>369</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E39" s="136" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" s="134"/>
+        <v>87</v>
+      </c>
+      <c r="E39" s="138" t="s">
+        <v>360</v>
+      </c>
+      <c r="F39" s="134" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="137" t="s">
         <v>79</v>
       </c>
       <c r="B40" s="132" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>73</v>
@@ -7668,10 +7706,10 @@
         <v>79</v>
       </c>
       <c r="B41" s="132" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>73</v>
@@ -7686,10 +7724,10 @@
         <v>79</v>
       </c>
       <c r="B42" s="132" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>73</v>
@@ -7704,10 +7742,10 @@
         <v>79</v>
       </c>
       <c r="B43" s="132" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>73</v>
@@ -7722,10 +7760,10 @@
         <v>79</v>
       </c>
       <c r="B44" s="132" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>73</v>
@@ -7740,10 +7778,10 @@
         <v>79</v>
       </c>
       <c r="B45" s="132" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>73</v>
@@ -7758,10 +7796,10 @@
         <v>79</v>
       </c>
       <c r="B46" s="132" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>73</v>
@@ -7776,10 +7814,10 @@
         <v>79</v>
       </c>
       <c r="B47" s="132" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>73</v>
@@ -7794,10 +7832,10 @@
         <v>79</v>
       </c>
       <c r="B48" s="132" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>73</v>
@@ -7809,16 +7847,16 @@
     </row>
     <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="137" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B49" s="132" t="s">
-        <v>333</v>
+        <v>80</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D49" s="139" t="s">
-        <v>334</v>
+        <v>63</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="E49" s="136" t="s">
         <v>57</v>
@@ -7826,26 +7864,24 @@
       <c r="F49" s="134"/>
     </row>
     <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="137" t="s">
+      <c r="A50" s="181" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="132" t="s">
-        <v>335</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E50" s="136" t="s">
+      <c r="B50" s="182" t="s">
+        <v>377</v>
+      </c>
+      <c r="C50" s="183" t="s">
+        <v>376</v>
+      </c>
+      <c r="D50" s="183" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" s="184" t="s">
         <v>57</v>
       </c>
-      <c r="F50" s="134" t="s">
-        <v>69</v>
-      </c>
+      <c r="F50" s="185"/>
       <c r="G50" s="35" t="s">
-        <v>353</v>
+        <v>375</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -7853,72 +7889,74 @@
         <v>75</v>
       </c>
       <c r="B51" s="132" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>88</v>
+        <v>67</v>
+      </c>
+      <c r="D51" s="139" t="s">
+        <v>334</v>
       </c>
       <c r="E51" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F51" s="134" t="s">
-        <v>69</v>
-      </c>
-      <c r="G51" s="35" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F51" s="134"/>
+    </row>
+    <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="137" t="s">
         <v>75</v>
       </c>
       <c r="B52" s="132" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="139" t="s">
-        <v>73</v>
+        <v>336</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="E52" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F52" s="134"/>
+      <c r="F52" s="134" t="s">
+        <v>69</v>
+      </c>
       <c r="G52" s="35" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="137" t="s">
         <v>75</v>
       </c>
       <c r="B53" s="132" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" s="139" t="s">
-        <v>73</v>
+        <v>372</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="E53" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F53" s="134"/>
+      <c r="F53" s="134" t="s">
+        <v>69</v>
+      </c>
+      <c r="G53" s="35" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="137" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="132" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D54" s="139" t="s">
         <v>73</v>
@@ -7927,16 +7965,19 @@
         <v>57</v>
       </c>
       <c r="F54" s="134"/>
+      <c r="G54" s="35" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="137" t="s">
         <v>75</v>
       </c>
       <c r="B55" s="132" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D55" s="139" t="s">
         <v>73</v>
@@ -7947,37 +7988,58 @@
       <c r="F55" s="134"/>
     </row>
     <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="140" t="s">
+      <c r="A56" s="137" t="s">
         <v>75</v>
       </c>
-      <c r="B56" s="141" t="s">
-        <v>341</v>
-      </c>
-      <c r="C56" s="142" t="s">
-        <v>70</v>
+      <c r="B56" s="132" t="s">
+        <v>339</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="D56" s="139" t="s">
         <v>73</v>
       </c>
-      <c r="E56" s="143" t="s">
+      <c r="E56" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F56" s="144"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="43"/>
-      <c r="B57" s="42"/>
-      <c r="C57" s="42"/>
-      <c r="D57" s="42"/>
-      <c r="E57" s="42"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="43"/>
-      <c r="B58" s="42"/>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="42"/>
-      <c r="F58" s="40"/>
+      <c r="F56" s="134"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="137" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" s="132" t="s">
+        <v>340</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" s="136" t="s">
+        <v>57</v>
+      </c>
+      <c r="F57" s="134"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="140" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="141" t="s">
+        <v>341</v>
+      </c>
+      <c r="C58" s="142" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" s="143" t="s">
+        <v>57</v>
+      </c>
+      <c r="F58" s="144"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="43"/>
@@ -7985,7 +8047,6 @@
       <c r="C59" s="42"/>
       <c r="D59" s="42"/>
       <c r="E59" s="42"/>
-      <c r="F59" s="40"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="43"/>
@@ -8012,60 +8073,58 @@
       <c r="F62" s="40"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="44"/>
+      <c r="A63" s="43"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
       <c r="D63" s="42"/>
       <c r="E63" s="42"/>
+      <c r="F63" s="40"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="44"/>
+      <c r="A64" s="43"/>
+      <c r="B64" s="42"/>
+      <c r="C64" s="42"/>
       <c r="D64" s="42"/>
       <c r="E64" s="42"/>
-      <c r="F64" s="36"/>
+      <c r="F64" s="40"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="44"/>
       <c r="D65" s="42"/>
       <c r="E65" s="42"/>
-      <c r="F65" s="40"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="49"/>
-      <c r="B66" s="48"/>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="37"/>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="46"/>
-      <c r="B67" s="45"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
-      <c r="G67" s="36"/>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="44"/>
-    </row>
-    <row r="69" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="41"/>
+      <c r="A66" s="44"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="36"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="44"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="40"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" s="49"/>
+      <c r="B68" s="48"/>
+      <c r="C68" s="48"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="37"/>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="46"/>
+      <c r="B69" s="45"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45"/>
+      <c r="G69" s="36"/>
     </row>
     <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="43"/>
-      <c r="B70" s="42"/>
-      <c r="C70" s="42"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="42"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="36"/>
-    </row>
-    <row r="71" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="43"/>
-      <c r="B71" s="42"/>
-      <c r="C71" s="42"/>
-      <c r="D71" s="42"/>
-      <c r="E71" s="42"/>
-      <c r="F71" s="42"/>
-      <c r="G71" s="36"/>
+      <c r="A70" s="44"/>
+    </row>
+    <row r="71" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="41"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="43"/>
@@ -8077,11 +8136,11 @@
       <c r="G72" s="36"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="91"/>
-      <c r="B73" s="92"/>
-      <c r="C73" s="92"/>
-      <c r="D73" s="92"/>
-      <c r="E73" s="92"/>
+      <c r="A73" s="43"/>
+      <c r="B73" s="42"/>
+      <c r="C73" s="42"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
       <c r="F73" s="42"/>
       <c r="G73" s="36"/>
     </row>
@@ -8091,15 +8150,17 @@
       <c r="C74" s="42"/>
       <c r="D74" s="42"/>
       <c r="E74" s="42"/>
+      <c r="F74" s="42"/>
       <c r="G74" s="36"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="43"/>
-      <c r="B75" s="42"/>
-      <c r="C75" s="42"/>
-      <c r="D75" s="42"/>
-      <c r="E75" s="42"/>
+      <c r="A75" s="91"/>
+      <c r="B75" s="92"/>
+      <c r="C75" s="92"/>
+      <c r="D75" s="92"/>
+      <c r="E75" s="92"/>
       <c r="F75" s="42"/>
+      <c r="G75" s="36"/>
     </row>
     <row r="76" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="43"/>
@@ -8107,25 +8168,41 @@
       <c r="C76" s="42"/>
       <c r="D76" s="42"/>
       <c r="E76" s="42"/>
-      <c r="F76" s="42"/>
+      <c r="G76" s="36"/>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="41"/>
-      <c r="B77" s="36"/>
-      <c r="C77" s="36"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="40"/>
-      <c r="G77" s="36"/>
+      <c r="A77" s="43"/>
+      <c r="B77" s="42"/>
+      <c r="C77" s="42"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
+      <c r="F77" s="42"/>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="39"/>
-      <c r="B78" s="38"/>
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="38"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="36"/>
+      <c r="A78" s="43"/>
+      <c r="B78" s="42"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="42"/>
+      <c r="F78" s="42"/>
+    </row>
+    <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="41"/>
+      <c r="B79" s="36"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="40"/>
+      <c r="G79" s="36"/>
+    </row>
+    <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="39"/>
+      <c r="B80" s="38"/>
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="38"/>
+      <c r="F80" s="37"/>
+      <c r="G80" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
hide tab extractor CA
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC82489D-FECF-8F41-BD85-8DA2F8E9FD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896F4498-4BDF-2249-9C96-9F745064010A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="codage tribunal" sheetId="12" state="hidden" r:id="rId5"/>
     <sheet name="Juridictions" sheetId="17" state="hidden" r:id="rId6"/>
     <sheet name="Table_Fonctions" sheetId="19" state="hidden" r:id="rId7"/>
-    <sheet name="ETPT_CA_JUR" sheetId="30" r:id="rId8"/>
+    <sheet name="ETPT_CA_JUR" sheetId="30" state="hidden" r:id="rId8"/>
     <sheet name="ETPT_CA_JUR_DDG" sheetId="25" r:id="rId9"/>
     <sheet name="ETPT_CA_JUR Corresp" sheetId="38" state="hidden" r:id="rId10"/>
   </sheets>
@@ -9710,7 +9710,7 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update menu déroulant JA
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF39370-4BCF-7C41-BDA0-61B4BDD022F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15666CDA-98BA-8C4E-9634-66219B71164B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ETPT Format DDG'!$A$2:$DT$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="381">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -2433,15 +2433,6 @@
     <t>Indisponibilité des placés à reporter sur le SAR, ligne "Etpt placés absents non affectés", colonne ABC-BUR</t>
   </si>
   <si>
-    <t>manque : JURISTE AS chambres sociales</t>
-  </si>
-  <si>
-    <t>manque : JURISTE AS parquet général</t>
-  </si>
-  <si>
-    <t>manque : Magistrat placé SUB</t>
-  </si>
-  <si>
     <t xml:space="preserve">                Déclaration des ETPT CA</t>
   </si>
   <si>
@@ -2487,21 +2478,12 @@
     <t>Fonctionnaire CTECH placé SUB</t>
   </si>
   <si>
-    <t>manque : VPP add / sub et JP add / sub</t>
-  </si>
-  <si>
     <t>JA Siège autres</t>
   </si>
   <si>
-    <t>ajouter ? JA Pôle Social,JA Parquet,JA JP,JA VIF</t>
-  </si>
-  <si>
     <t>A GREFFIER</t>
   </si>
   <si>
-    <t>à valider</t>
-  </si>
-  <si>
     <t>Att. J</t>
   </si>
   <si>
@@ -2512,6 +2494,27 @@
   </si>
   <si>
     <t>Pas encore appelé dans la matrice DDG, à voir lors de la publication de la prochaine circulaire 2025/2026</t>
+  </si>
+  <si>
+    <t>JURISTE AS chambres sociales</t>
+  </si>
+  <si>
+    <t>JURISTE AS parquet général</t>
+  </si>
+  <si>
+    <t>JA Chambres Sociales</t>
+  </si>
+  <si>
+    <t>JA Siège Autres</t>
+  </si>
+  <si>
+    <t>JA Parquet Général</t>
+  </si>
+  <si>
+    <t>manque : Magistrat placé SUB en attente de retour d'Aurélie</t>
+  </si>
+  <si>
+    <t>manque : VPP add / sub et JP add / sub en attente de retour d'Aurélie</t>
   </si>
 </sst>
 </file>
@@ -4265,8 +4268,8 @@
       <xdr:rowOff>28222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1326444</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1086556</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>976232</xdr:rowOff>
     </xdr:to>
@@ -4749,7 +4752,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+      <selection activeCell="A14" sqref="A14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6482,13 +6485,13 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AKL1" sqref="K1:AKL1"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="32.5" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="38.33203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="51.83203125" customWidth="1"/>
@@ -6890,10 +6893,10 @@
   <sheetPr codeName="Feuil14">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView topLeftCell="A41" zoomScale="118" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7068,7 +7071,7 @@
         <v>38</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -7091,7 +7094,7 @@
         <v>38</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -7226,7 +7229,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="137" t="s">
         <v>79</v>
       </c>
@@ -7246,7 +7249,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="137" t="s">
         <v>79</v>
       </c>
@@ -7266,15 +7269,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="153" t="s">
         <v>79</v>
       </c>
       <c r="B19" s="154" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C19" s="155" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D19" s="155" t="s">
         <v>88</v>
@@ -7285,11 +7288,8 @@
       <c r="F19" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="G19" s="35" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="137" t="s">
         <v>79</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="137" t="s">
         <v>79</v>
       </c>
@@ -7329,7 +7329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="137" t="s">
         <v>79</v>
       </c>
@@ -7349,7 +7349,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="137" t="s">
         <v>79</v>
       </c>
@@ -7369,7 +7369,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="137" t="s">
         <v>79</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="137" t="s">
         <v>79</v>
       </c>
@@ -7409,7 +7409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="137" t="s">
         <v>79</v>
       </c>
@@ -7417,7 +7417,7 @@
         <v>327</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>87</v>
@@ -7429,7 +7429,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="137" t="s">
         <v>79</v>
       </c>
@@ -7437,19 +7437,19 @@
         <v>327</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E27" s="138" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F27" s="134" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="137" t="s">
         <v>79</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="137" t="s">
         <v>79</v>
       </c>
@@ -7477,7 +7477,7 @@
         <v>328</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>87</v>
@@ -7489,7 +7489,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="137" t="s">
         <v>79</v>
       </c>
@@ -7497,19 +7497,19 @@
         <v>328</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E30" s="138" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F30" s="134" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="137" t="s">
         <v>79</v>
       </c>
@@ -7529,7 +7529,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="137" t="s">
         <v>79</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>330</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>87</v>
@@ -7557,16 +7557,16 @@
         <v>330</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E33" s="138" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F33" s="134" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7597,7 +7597,7 @@
         <v>331</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>87</v>
@@ -7617,16 +7617,16 @@
         <v>331</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E36" s="138" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F36" s="134" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7657,7 +7657,7 @@
         <v>332</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>87</v>
@@ -7677,16 +7677,16 @@
         <v>332</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>87</v>
       </c>
       <c r="E39" s="138" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F39" s="134" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7874,10 +7874,10 @@
         <v>75</v>
       </c>
       <c r="B50" s="154" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C50" s="155" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D50" s="155" t="s">
         <v>73</v>
@@ -7886,10 +7886,10 @@
         <v>57</v>
       </c>
       <c r="F50" s="157" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="G50" s="35" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -7918,7 +7918,7 @@
         <v>335</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>336</v>
+        <v>376</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>88</v>
@@ -7927,10 +7927,7 @@
         <v>57</v>
       </c>
       <c r="F52" s="134" t="s">
-        <v>69</v>
-      </c>
-      <c r="G52" s="35" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -7941,7 +7938,7 @@
         <v>335</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>88</v>
@@ -7952,76 +7949,76 @@
       <c r="F53" s="134" t="s">
         <v>69</v>
       </c>
-      <c r="G53" s="35" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="137" t="s">
         <v>75</v>
       </c>
       <c r="B54" s="132" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D54" s="139" t="s">
-        <v>73</v>
+        <v>378</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="E54" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F54" s="134"/>
-      <c r="G54" s="35" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F54" s="134" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="137" t="s">
         <v>75</v>
       </c>
       <c r="B55" s="132" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" s="139" t="s">
-        <v>73</v>
+        <v>336</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="E55" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F55" s="134"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F55" s="134" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="137" t="s">
         <v>75</v>
       </c>
       <c r="B56" s="132" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D56" s="139" t="s">
-        <v>73</v>
+        <v>368</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="E56" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F56" s="134"/>
+      <c r="F56" s="134" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="137" t="s">
         <v>75</v>
       </c>
       <c r="B57" s="132" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D57" s="139" t="s">
         <v>73</v>
@@ -8032,45 +8029,76 @@
       <c r="F57" s="134"/>
     </row>
     <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="140" t="s">
+      <c r="A58" s="137" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="141" t="s">
-        <v>341</v>
-      </c>
-      <c r="C58" s="142" t="s">
-        <v>70</v>
+      <c r="B58" s="132" t="s">
+        <v>338</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D58" s="139" t="s">
         <v>73</v>
       </c>
-      <c r="E58" s="143" t="s">
+      <c r="E58" s="136" t="s">
         <v>57</v>
       </c>
-      <c r="F58" s="144"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="43"/>
-      <c r="B59" s="42"/>
-      <c r="C59" s="42"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="42"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="43"/>
-      <c r="B60" s="42"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="40"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="43"/>
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="40"/>
+      <c r="F58" s="134"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="137" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="132" t="s">
+        <v>339</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D59" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="136" t="s">
+        <v>57</v>
+      </c>
+      <c r="F59" s="134"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="137" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" s="132" t="s">
+        <v>340</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="E60" s="136" t="s">
+        <v>57</v>
+      </c>
+      <c r="F60" s="134"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="140" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="141" t="s">
+        <v>341</v>
+      </c>
+      <c r="C61" s="142" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" s="139" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" s="143" t="s">
+        <v>57</v>
+      </c>
+      <c r="F61" s="144"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="43"/>
@@ -8078,7 +8106,6 @@
       <c r="C62" s="42"/>
       <c r="D62" s="42"/>
       <c r="E62" s="42"/>
-      <c r="F62" s="40"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="43"/>
@@ -8097,76 +8124,73 @@
       <c r="F64" s="40"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="44"/>
+      <c r="A65" s="43"/>
+      <c r="B65" s="42"/>
+      <c r="C65" s="42"/>
       <c r="D65" s="42"/>
       <c r="E65" s="42"/>
+      <c r="F65" s="40"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="44"/>
+      <c r="A66" s="43"/>
+      <c r="B66" s="42"/>
+      <c r="C66" s="42"/>
       <c r="D66" s="42"/>
       <c r="E66" s="42"/>
-      <c r="F66" s="36"/>
+      <c r="F66" s="40"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="44"/>
+      <c r="A67" s="43"/>
+      <c r="B67" s="42"/>
+      <c r="C67" s="42"/>
       <c r="D67" s="42"/>
       <c r="E67" s="42"/>
       <c r="F67" s="40"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="49"/>
-      <c r="B68" s="48"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="37"/>
-    </row>
-    <row r="69" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="46"/>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
-      <c r="G69" s="36"/>
-    </row>
-    <row r="70" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="44"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" s="44"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="36"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="44"/>
-    </row>
-    <row r="71" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="41"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
+      <c r="F70" s="40"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="49"/>
+      <c r="B71" s="48"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="47"/>
+      <c r="F71" s="37"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="43"/>
-      <c r="B72" s="42"/>
-      <c r="C72" s="42"/>
-      <c r="D72" s="42"/>
-      <c r="E72" s="42"/>
-      <c r="F72" s="42"/>
+      <c r="A72" s="46"/>
+      <c r="B72" s="45"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="45"/>
       <c r="G72" s="36"/>
     </row>
     <row r="73" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="43"/>
-      <c r="B73" s="42"/>
-      <c r="C73" s="42"/>
-      <c r="D73" s="42"/>
-      <c r="E73" s="42"/>
-      <c r="F73" s="42"/>
-      <c r="G73" s="36"/>
-    </row>
-    <row r="74" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="43"/>
-      <c r="B74" s="42"/>
-      <c r="C74" s="42"/>
-      <c r="D74" s="42"/>
-      <c r="E74" s="42"/>
-      <c r="F74" s="42"/>
-      <c r="G74" s="36"/>
+      <c r="A73" s="44"/>
+    </row>
+    <row r="74" spans="1:7" s="36" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="41"/>
     </row>
     <row r="75" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="91"/>
-      <c r="B75" s="92"/>
-      <c r="C75" s="92"/>
-      <c r="D75" s="92"/>
-      <c r="E75" s="92"/>
+      <c r="A75" s="43"/>
+      <c r="B75" s="42"/>
+      <c r="C75" s="42"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
       <c r="F75" s="42"/>
       <c r="G75" s="36"/>
     </row>
@@ -8176,6 +8200,7 @@
       <c r="C76" s="42"/>
       <c r="D76" s="42"/>
       <c r="E76" s="42"/>
+      <c r="F76" s="42"/>
       <c r="G76" s="36"/>
     </row>
     <row r="77" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -8185,32 +8210,58 @@
       <c r="D77" s="42"/>
       <c r="E77" s="42"/>
       <c r="F77" s="42"/>
+      <c r="G77" s="36"/>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="43"/>
-      <c r="B78" s="42"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="42"/>
-      <c r="E78" s="42"/>
+      <c r="A78" s="91"/>
+      <c r="B78" s="92"/>
+      <c r="C78" s="92"/>
+      <c r="D78" s="92"/>
+      <c r="E78" s="92"/>
       <c r="F78" s="42"/>
+      <c r="G78" s="36"/>
     </row>
     <row r="79" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="41"/>
-      <c r="B79" s="36"/>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
-      <c r="F79" s="40"/>
+      <c r="A79" s="43"/>
+      <c r="B79" s="42"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
       <c r="G79" s="36"/>
     </row>
     <row r="80" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="39"/>
-      <c r="B80" s="38"/>
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="38"/>
-      <c r="F80" s="37"/>
-      <c r="G80" s="36"/>
+      <c r="A80" s="43"/>
+      <c r="B80" s="42"/>
+      <c r="C80" s="42"/>
+      <c r="D80" s="42"/>
+      <c r="E80" s="42"/>
+      <c r="F80" s="42"/>
+    </row>
+    <row r="81" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="43"/>
+      <c r="B81" s="42"/>
+      <c r="C81" s="42"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="42"/>
+      <c r="F81" s="42"/>
+    </row>
+    <row r="82" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="41"/>
+      <c r="B82" s="36"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="40"/>
+      <c r="G82" s="36"/>
+    </row>
+    <row r="83" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="39"/>
+      <c r="B83" s="38"/>
+      <c r="C83" s="38"/>
+      <c r="D83" s="38"/>
+      <c r="E83" s="38"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -8226,9 +8277,9 @@
   <dimension ref="A1:BJ19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <pane xSplit="6" topLeftCell="N1" activePane="topRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="topRight" activeCell="D14" sqref="D14"/>
+      <selection pane="topRight" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8552,7 +8603,7 @@
       <c r="B5" s="54"/>
       <c r="C5" s="54"/>
       <c r="D5" s="60" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E5" s="146" t="s">
         <v>117</v>
@@ -9744,12 +9795,12 @@
   <sheetData>
     <row r="1" spans="1:31" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>

</xml_diff>

<commit_message>
add fix agregat placé CA
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB0B10B-3D41-0E43-BFAB-7C7A4C31C851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEB85F7-B5BB-F443-95DF-E2870479884F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -5998,8 +5998,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6177,7 +6177,7 @@
         <v>138</v>
       </c>
       <c r="G6" s="19" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="H6" s="91" t="str">
@@ -6185,11 +6185,11 @@
         <v/>
       </c>
       <c r="I6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="J6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="K6" s="18" t="e">
@@ -6197,7 +6197,7 @@
 INDEX('ETPT Format DDG'!$A:$FF,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),'ETPT Format DDG'!$I:$I,"C",
+),'ETPT Format DDG'!$FG:$FG,"C",
 'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Magistrat")</f>
         <v>#N/A</v>
@@ -6217,7 +6217,7 @@
         <v/>
       </c>
       <c r="N6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="O6" s="91" t="str">
@@ -6225,15 +6225,15 @@
         <v/>
       </c>
       <c r="P6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="Q6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="R6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$I:$I,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
       <c r="S6" s="19" t="e">
@@ -6255,7 +6255,7 @@
 INDEX('ETPT Format DDG'!$A:$FF,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),'ETPT Format DDG'!$I:$I,"C",
+),'ETPT Format DDG'!$FG:$FG,"C",
 'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Autour du magistrat")</f>
         <v>#N/A</v>

</xml_diff>

<commit_message>
add contentieux mineur ca gap
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0860825-BB90-D143-A29B-F00B6CED0756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A27792-112A-FB4A-829B-B40BB5EEDBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="23880" windowHeight="17780" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
@@ -3494,27 +3494,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3654,6 +3634,16 @@
       <font>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6040,14 +6030,14 @@
   <dimension ref="A1:FG4"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
     <col min="126" max="126" width="13.5" customWidth="1"/>
     <col min="127" max="127" width="15.83203125" customWidth="1"/>
     <col min="128" max="128" width="36.1640625" customWidth="1"/>
@@ -6130,7 +6120,7 @@
     <mergeCell ref="FA1:FF1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:FF1048576">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
       <formula>AND(OR($N1&lt;&gt;"-",$O1&lt;&gt;0,$P1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6445,64 +6435,64 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L6)&lt;&gt;_xlfn.NUMBERVALUE($L7),_xlfn.NUMBERVALUE($S6)&lt;&gt;_xlfn.NUMBERVALUE($S7),_xlfn.NUMBERVALUE($U6)&lt;&gt;_xlfn.NUMBERVALUE($U7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update extractors with automation
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A27792-112A-FB4A-829B-B40BB5EEDBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE02AFD-3461-0B4A-A860-F79A1F0EC7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="23880" windowHeight="17780" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="23880" windowHeight="17780" firstSheet="2" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId2"/>
     <sheet name="ETPT Format DDG" sheetId="9" r:id="rId3"/>
     <sheet name="Agrégats DDG" sheetId="10" r:id="rId4"/>
-    <sheet name="codage tribunal" sheetId="12" state="hidden" r:id="rId5"/>
-    <sheet name="Juridictions" sheetId="17" state="hidden" r:id="rId6"/>
-    <sheet name="Table_Fonctions" sheetId="19" state="hidden" r:id="rId7"/>
-    <sheet name="ETPT_CA_JUR" sheetId="30" state="hidden" r:id="rId8"/>
+    <sheet name="codage tribunal" sheetId="12" r:id="rId5"/>
+    <sheet name="Juridictions" sheetId="17" r:id="rId6"/>
+    <sheet name="Table_Fonctions" sheetId="19" r:id="rId7"/>
+    <sheet name="ETPT_CA_JUR" sheetId="30" r:id="rId8"/>
     <sheet name="ETPT_CA_JUR_DDG" sheetId="25" r:id="rId9"/>
-    <sheet name="ETPT_CA_JUR Corresp" sheetId="38" state="hidden" r:id="rId10"/>
+    <sheet name="ETPT_CA_JUR Corresp" sheetId="38" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="263">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t xml:space="preserve">                  Extracteur de données d'effectifs</t>
-  </si>
-  <si>
-    <t>RECAPITULATIF</t>
   </si>
   <si>
     <t>CPH détachés</t>
@@ -2115,21 +2112,6 @@
     <t>Correspondance</t>
   </si>
   <si>
-    <t>Temps ventilés sur la période (contentieux sociaux civils et commerciaux)</t>
-  </si>
-  <si>
-    <t>Temps ventilés sur la période (service pénal)</t>
-  </si>
-  <si>
-    <t>Temps ventilés sur la période (hors indisponibilité)</t>
-  </si>
-  <si>
-    <t>Temps ventilés sur la période (y.c. indisponibilité)</t>
-  </si>
-  <si>
-    <t>Soutien (Hors accueil du justiciable)</t>
-  </si>
-  <si>
     <t>PARQUET_JIRS</t>
   </si>
   <si>
@@ -2173,6 +2155,12 @@
   </si>
   <si>
     <t>#! FOR_EACH f fonctions</t>
+  </si>
+  <si>
+    <t>=ETPT_CA_JUR!D5</t>
+  </si>
+  <si>
+    <t>Fonction agrégats</t>
   </si>
 </sst>
 </file>
@@ -2188,7 +2176,7 @@
     <numFmt numFmtId="169" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2366,14 +2354,6 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2520,7 +2500,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2554,12 +2534,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3028,7 +3002,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3141,67 +3115,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="9" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="19" fillId="8" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="19" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="9" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="20" fillId="8" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="22" fillId="8" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="13" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="24" fillId="12" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3210,22 +3184,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3237,7 +3211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3249,49 +3223,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="20" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="17" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="17" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="37" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="36" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="37" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="36" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="38" fillId="11" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="37" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="38" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="36" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="169" fontId="37" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="169" fontId="35" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="36" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="40" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3301,65 +3275,65 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="39" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="38" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="39" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="38" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="39" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="38" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="39" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="38" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="40" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="39" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="40" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="39" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="42" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="41" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="42" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="41" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="42" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="41" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="19" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="37" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="19" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="36" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="44" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="43" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="34" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="34" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="33" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="44" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="45" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="46" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3368,22 +3342,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3392,7 +3366,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3401,10 +3375,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3413,53 +3387,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3479,10 +3450,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="40" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="39" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3494,7 +3465,17 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4397,7 +4378,7 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="EJ1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -4416,10 +4397,10 @@
     <row r="1" spans="1:8" s="26" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50"/>
       <c r="B1" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="126" t="s">
         <v>112</v>
-      </c>
-      <c r="C1" s="126" t="s">
-        <v>113</v>
       </c>
       <c r="D1" s="126"/>
       <c r="E1" s="126"/>
@@ -4432,7 +4413,7 @@
       <c r="A2" s="53"/>
       <c r="B2" s="54"/>
       <c r="C2" s="127" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" s="127"/>
       <c r="E2" s="127"/>
@@ -4451,16 +4432,16 @@
     <row r="4" spans="1:8" s="62" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="61" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="D4" s="61" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="E4" s="133" t="s">
         <v>116</v>
-      </c>
-      <c r="E4" s="133" t="s">
-        <v>117</v>
       </c>
       <c r="F4" s="134"/>
       <c r="G4" s="68"/>
@@ -4471,16 +4452,16 @@
     <row r="5" spans="1:8" s="26" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="57"/>
       <c r="B5" s="72" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="65" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="D5" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="65" t="s">
-        <v>120</v>
-      </c>
       <c r="E5" s="135" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" s="136"/>
       <c r="G5" s="67"/>
@@ -4491,16 +4472,16 @@
     <row r="6" spans="1:8" s="26" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="57"/>
       <c r="B6" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="D6" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="66" t="s">
-        <v>123</v>
-      </c>
       <c r="E6" s="137" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F6" s="138"/>
       <c r="G6" s="67"/>
@@ -4511,16 +4492,16 @@
     <row r="7" spans="1:8" s="26" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="57"/>
       <c r="B7" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="D7" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="66" t="s">
-        <v>126</v>
-      </c>
       <c r="E7" s="137" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" s="138"/>
       <c r="G7" s="67"/>
@@ -4531,16 +4512,16 @@
     <row r="8" spans="1:8" s="26" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="57"/>
       <c r="B8" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="128" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="128" t="s">
+      <c r="D8" s="128" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="128" t="s">
-        <v>129</v>
-      </c>
       <c r="E8" s="139" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F8" s="140"/>
       <c r="G8" s="67"/>
@@ -4551,7 +4532,7 @@
     <row r="9" spans="1:8" s="26" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="57"/>
       <c r="B9" s="76" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="128"/>
       <c r="D9" s="128"/>
@@ -4565,7 +4546,7 @@
     <row r="10" spans="1:8" s="26" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="57"/>
       <c r="B10" s="77" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="129"/>
       <c r="D10" s="129"/>
@@ -4591,7 +4572,7 @@
       <c r="A12" s="57"/>
       <c r="B12" s="69"/>
       <c r="C12" s="132" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D12" s="132"/>
       <c r="E12" s="132"/>
@@ -4659,13 +4640,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="152" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" s="152"/>
-      <c r="C1" s="152"/>
-      <c r="D1" s="152"/>
-      <c r="E1" s="152"/>
+      <c r="A1" s="151" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
       <c r="F1" s="96"/>
       <c r="G1" s="78"/>
       <c r="H1" s="78"/>
@@ -4697,7 +4678,7 @@
       <c r="G2" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="153" t="s">
+      <c r="H2" s="152" t="s">
         <v>105</v>
       </c>
       <c r="I2" s="80" t="s">
@@ -4718,7 +4699,7 @@
       <c r="N2" s="80" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="153" t="s">
+      <c r="O2" s="152" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="80" t="s">
@@ -4730,7 +4711,7 @@
       <c r="R2" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="153" t="s">
+      <c r="S2" s="152" t="s">
         <v>102</v>
       </c>
       <c r="T2" s="80" t="s">
@@ -4748,7 +4729,7 @@
       <c r="X2" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="153" t="s">
+      <c r="Y2" s="152" t="s">
         <v>100</v>
       </c>
     </row>
@@ -4762,7 +4743,7 @@
       <c r="G3" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="H3" s="153"/>
+      <c r="H3" s="152"/>
       <c r="I3" s="80" t="s">
         <v>96</v>
       </c>
@@ -4773,17 +4754,17 @@
         <v>94</v>
       </c>
       <c r="L3" s="80" t="s">
+        <v>140</v>
+      </c>
+      <c r="M3" s="80" t="s">
         <v>141</v>
-      </c>
-      <c r="M3" s="80" t="s">
-        <v>142</v>
       </c>
       <c r="N3" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="O3" s="153"/>
+      <c r="O3" s="152"/>
       <c r="P3" s="80" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q3" s="80" t="s">
         <v>91</v>
@@ -4791,7 +4772,7 @@
       <c r="R3" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="S3" s="153"/>
+      <c r="S3" s="152"/>
       <c r="T3" s="80" t="s">
         <v>90</v>
       </c>
@@ -4799,15 +4780,15 @@
         <v>89</v>
       </c>
       <c r="V3" s="80" t="s">
+        <v>143</v>
+      </c>
+      <c r="W3" s="80" t="s">
         <v>144</v>
-      </c>
-      <c r="W3" s="80" t="s">
-        <v>145</v>
       </c>
       <c r="X3" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="Y3" s="153"/>
+      <c r="Y3" s="152"/>
     </row>
     <row r="4" spans="1:25" ht="84" x14ac:dyDescent="0.2">
       <c r="A4" s="98"/>
@@ -4829,7 +4810,7 @@
       <c r="G4" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="H4" s="153"/>
+      <c r="H4" s="152"/>
       <c r="I4" s="80" t="s">
         <v>78</v>
       </c>
@@ -4840,17 +4821,17 @@
         <v>76</v>
       </c>
       <c r="L4" s="80" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="80" t="s">
         <v>146</v>
-      </c>
-      <c r="M4" s="80" t="s">
-        <v>147</v>
       </c>
       <c r="N4" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="153"/>
+      <c r="O4" s="152"/>
       <c r="P4" s="80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q4" s="80" t="s">
         <v>73</v>
@@ -4858,7 +4839,7 @@
       <c r="R4" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="S4" s="153"/>
+      <c r="S4" s="152"/>
       <c r="T4" s="80" t="s">
         <v>72</v>
       </c>
@@ -4866,19 +4847,19 @@
         <v>71</v>
       </c>
       <c r="V4" s="80" t="s">
+        <v>148</v>
+      </c>
+      <c r="W4" s="80" t="s">
         <v>149</v>
-      </c>
-      <c r="W4" s="80" t="s">
-        <v>150</v>
       </c>
       <c r="X4" s="80" t="s">
         <v>70</v>
       </c>
-      <c r="Y4" s="153"/>
+      <c r="Y4" s="152"/>
     </row>
     <row r="5" spans="1:25" ht="332" x14ac:dyDescent="0.2">
       <c r="A5" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B5" s="101"/>
       <c r="C5" s="101"/>
@@ -4890,36 +4871,36 @@
         <v>64</v>
       </c>
       <c r="G5" s="81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H5" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G5:G5)</f>
         <v>0</v>
       </c>
       <c r="I5" s="81" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J5" s="83"/>
       <c r="K5" s="83"/>
       <c r="L5" s="83"/>
       <c r="M5" s="81" t="s">
+        <v>153</v>
+      </c>
+      <c r="N5" s="81" t="s">
         <v>154</v>
-      </c>
-      <c r="N5" s="81" t="s">
-        <v>155</v>
       </c>
       <c r="O5" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G5:N5)</f>
         <v>0</v>
       </c>
       <c r="P5" s="81" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q5" s="81" t="s">
         <v>156</v>
       </c>
-      <c r="Q5" s="81" t="s">
+      <c r="R5" s="81" t="s">
         <v>157</v>
-      </c>
-      <c r="R5" s="81" t="s">
-        <v>158</v>
       </c>
       <c r="S5" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G5:R5)</f>
@@ -4929,10 +4910,10 @@
       <c r="U5" s="83"/>
       <c r="V5" s="83"/>
       <c r="W5" s="81" t="s">
+        <v>158</v>
+      </c>
+      <c r="X5" s="81" t="s">
         <v>159</v>
-      </c>
-      <c r="X5" s="81" t="s">
-        <v>160</v>
       </c>
       <c r="Y5" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G5:X5)</f>
@@ -4941,7 +4922,7 @@
     </row>
     <row r="6" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="101"/>
       <c r="C6" s="101"/>
@@ -4953,7 +4934,7 @@
         <v>62</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H6" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G6:G6)</f>
@@ -4961,47 +4942,47 @@
       </c>
       <c r="I6" s="82"/>
       <c r="J6" s="81" t="s">
+        <v>161</v>
+      </c>
+      <c r="K6" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="K6" s="81" t="s">
+      <c r="L6" s="81" t="s">
         <v>163</v>
-      </c>
-      <c r="L6" s="81" t="s">
-        <v>164</v>
       </c>
       <c r="M6" s="83"/>
       <c r="N6" s="81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O6" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G6:N6)</f>
         <v>0</v>
       </c>
       <c r="P6" s="81" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q6" s="81" t="s">
         <v>166</v>
       </c>
-      <c r="Q6" s="81" t="s">
+      <c r="R6" s="81" t="s">
         <v>167</v>
-      </c>
-      <c r="R6" s="81" t="s">
-        <v>168</v>
       </c>
       <c r="S6" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G6:R6)</f>
         <v>0</v>
       </c>
       <c r="T6" s="81" t="s">
+        <v>168</v>
+      </c>
+      <c r="U6" s="81" t="s">
         <v>169</v>
       </c>
-      <c r="U6" s="81" t="s">
+      <c r="V6" s="81" t="s">
         <v>170</v>
-      </c>
-      <c r="V6" s="81" t="s">
-        <v>171</v>
       </c>
       <c r="W6" s="83"/>
       <c r="X6" s="81" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Y6" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G6:X6)</f>
@@ -5010,7 +4991,7 @@
     </row>
     <row r="7" spans="1:25" ht="90" x14ac:dyDescent="0.2">
       <c r="A7" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" s="101"/>
       <c r="C7" s="101"/>
@@ -5048,7 +5029,7 @@
       <c r="V7" s="103"/>
       <c r="W7" s="103"/>
       <c r="X7" s="104" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y7" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G7:X7)</f>
@@ -5057,7 +5038,7 @@
     </row>
     <row r="8" spans="1:25" ht="140" x14ac:dyDescent="0.2">
       <c r="A8" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" s="101"/>
       <c r="C8" s="101"/>
@@ -5069,7 +5050,7 @@
         <v>58</v>
       </c>
       <c r="G8" s="81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H8" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G8:G8)</f>
@@ -5081,20 +5062,20 @@
       <c r="L8" s="85"/>
       <c r="M8" s="85"/>
       <c r="N8" s="81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O8" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G8:N8)</f>
         <v>0</v>
       </c>
       <c r="P8" s="81" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q8" s="81" t="s">
         <v>176</v>
       </c>
-      <c r="Q8" s="81" t="s">
+      <c r="R8" s="81" t="s">
         <v>177</v>
-      </c>
-      <c r="R8" s="81" t="s">
-        <v>178</v>
       </c>
       <c r="S8" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G8:R8)</f>
@@ -5105,7 +5086,7 @@
       <c r="V8" s="103"/>
       <c r="W8" s="103"/>
       <c r="X8" s="81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Y8" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G8:X8)</f>
@@ -5114,7 +5095,7 @@
     </row>
     <row r="9" spans="1:25" ht="154" x14ac:dyDescent="0.2">
       <c r="A9" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="101"/>
       <c r="C9" s="101"/>
@@ -5126,7 +5107,7 @@
         <v>56</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H9" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G9:G9)</f>
@@ -5138,20 +5119,20 @@
       <c r="L9" s="85"/>
       <c r="M9" s="85"/>
       <c r="N9" s="81" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O9" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G9:N9)</f>
         <v>0</v>
       </c>
       <c r="P9" s="81" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q9" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="Q9" s="81" t="s">
+      <c r="R9" s="81" t="s">
         <v>183</v>
-      </c>
-      <c r="R9" s="81" t="s">
-        <v>184</v>
       </c>
       <c r="S9" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G9:R9)</f>
@@ -5162,7 +5143,7 @@
       <c r="V9" s="103"/>
       <c r="W9" s="103"/>
       <c r="X9" s="81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Y9" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G9:X9)</f>
@@ -5171,7 +5152,7 @@
     </row>
     <row r="10" spans="1:25" ht="140" x14ac:dyDescent="0.2">
       <c r="A10" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="101"/>
       <c r="C10" s="101"/>
@@ -5183,7 +5164,7 @@
         <v>54</v>
       </c>
       <c r="G10" s="81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H10" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G10:G10)</f>
@@ -5195,20 +5176,20 @@
       <c r="L10" s="85"/>
       <c r="M10" s="85"/>
       <c r="N10" s="81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O10" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G10:N10)</f>
         <v>0</v>
       </c>
       <c r="P10" s="81" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q10" s="81" t="s">
         <v>188</v>
       </c>
-      <c r="Q10" s="81" t="s">
+      <c r="R10" s="81" t="s">
         <v>189</v>
-      </c>
-      <c r="R10" s="81" t="s">
-        <v>190</v>
       </c>
       <c r="S10" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G10:R10)</f>
@@ -5219,7 +5200,7 @@
       <c r="V10" s="103"/>
       <c r="W10" s="103"/>
       <c r="X10" s="81" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Y10" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G10:X10)</f>
@@ -5228,7 +5209,7 @@
     </row>
     <row r="11" spans="1:25" ht="140" x14ac:dyDescent="0.2">
       <c r="A11" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B11" s="101"/>
       <c r="C11" s="101"/>
@@ -5240,7 +5221,7 @@
         <v>52</v>
       </c>
       <c r="G11" s="81" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H11" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G11:G11)</f>
@@ -5252,20 +5233,20 @@
       <c r="L11" s="85"/>
       <c r="M11" s="85"/>
       <c r="N11" s="81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O11" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G11:N11)</f>
         <v>0</v>
       </c>
       <c r="P11" s="81" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q11" s="81" t="s">
         <v>194</v>
       </c>
-      <c r="Q11" s="81" t="s">
+      <c r="R11" s="81" t="s">
         <v>195</v>
-      </c>
-      <c r="R11" s="81" t="s">
-        <v>196</v>
       </c>
       <c r="S11" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G11:R11)</f>
@@ -5276,7 +5257,7 @@
       <c r="V11" s="103"/>
       <c r="W11" s="103"/>
       <c r="X11" s="81" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Y11" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G11:X11)</f>
@@ -5285,7 +5266,7 @@
     </row>
     <row r="12" spans="1:25" ht="168" x14ac:dyDescent="0.2">
       <c r="A12" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12" s="101"/>
       <c r="C12" s="101"/>
@@ -5297,7 +5278,7 @@
         <v>50</v>
       </c>
       <c r="G12" s="81" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H12" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G12:G12)</f>
@@ -5309,20 +5290,20 @@
       <c r="L12" s="85"/>
       <c r="M12" s="85"/>
       <c r="N12" s="81" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O12" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G12:N12)</f>
         <v>0</v>
       </c>
       <c r="P12" s="81" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q12" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="Q12" s="81" t="s">
+      <c r="R12" s="81" t="s">
         <v>201</v>
-      </c>
-      <c r="R12" s="81" t="s">
-        <v>202</v>
       </c>
       <c r="S12" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G12:R12)</f>
@@ -5333,7 +5314,7 @@
       <c r="V12" s="103"/>
       <c r="W12" s="103"/>
       <c r="X12" s="81" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Y12" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G12:X12)</f>
@@ -5342,7 +5323,7 @@
     </row>
     <row r="13" spans="1:25" ht="126" x14ac:dyDescent="0.2">
       <c r="A13" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B13" s="101"/>
       <c r="C13" s="101"/>
@@ -5354,7 +5335,7 @@
         <v>48</v>
       </c>
       <c r="G13" s="81" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H13" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G13:G13)</f>
@@ -5366,20 +5347,20 @@
       <c r="L13" s="85"/>
       <c r="M13" s="85"/>
       <c r="N13" s="81" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O13" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G13:N13)</f>
         <v>0</v>
       </c>
       <c r="P13" s="81" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q13" s="81" t="s">
         <v>206</v>
       </c>
-      <c r="Q13" s="81" t="s">
+      <c r="R13" s="81" t="s">
         <v>207</v>
-      </c>
-      <c r="R13" s="81" t="s">
-        <v>208</v>
       </c>
       <c r="S13" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G13:R13)</f>
@@ -5390,7 +5371,7 @@
       <c r="V13" s="103"/>
       <c r="W13" s="103"/>
       <c r="X13" s="81" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y13" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G13:X13)</f>
@@ -5399,7 +5380,7 @@
     </row>
     <row r="14" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B14" s="101"/>
       <c r="C14" s="101"/>
@@ -5411,61 +5392,61 @@
         <v>46</v>
       </c>
       <c r="G14" s="81" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H14" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G14:G14)</f>
         <v>0</v>
       </c>
       <c r="I14" s="81" t="s">
+        <v>210</v>
+      </c>
+      <c r="J14" s="81" t="s">
         <v>211</v>
       </c>
-      <c r="J14" s="81" t="s">
+      <c r="K14" s="81" t="s">
         <v>212</v>
       </c>
-      <c r="K14" s="81" t="s">
+      <c r="L14" s="81" t="s">
         <v>213</v>
       </c>
-      <c r="L14" s="81" t="s">
+      <c r="M14" s="81" t="s">
         <v>214</v>
       </c>
-      <c r="M14" s="81" t="s">
+      <c r="N14" s="81" t="s">
         <v>215</v>
-      </c>
-      <c r="N14" s="81" t="s">
-        <v>216</v>
       </c>
       <c r="O14" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G14:N14)</f>
         <v>0</v>
       </c>
       <c r="P14" s="81" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q14" s="81" t="s">
         <v>217</v>
       </c>
-      <c r="Q14" s="81" t="s">
+      <c r="R14" s="81" t="s">
         <v>218</v>
-      </c>
-      <c r="R14" s="81" t="s">
-        <v>219</v>
       </c>
       <c r="S14" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G14:R14)</f>
         <v>0</v>
       </c>
       <c r="T14" s="81" t="s">
+        <v>219</v>
+      </c>
+      <c r="U14" s="81" t="s">
         <v>220</v>
       </c>
-      <c r="U14" s="81" t="s">
+      <c r="V14" s="81" t="s">
         <v>221</v>
       </c>
-      <c r="V14" s="81" t="s">
+      <c r="W14" s="81" t="s">
         <v>222</v>
       </c>
-      <c r="W14" s="81" t="s">
+      <c r="X14" s="81" t="s">
         <v>223</v>
-      </c>
-      <c r="X14" s="81" t="s">
-        <v>224</v>
       </c>
       <c r="Y14" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G14:X14)</f>
@@ -5474,16 +5455,16 @@
     </row>
     <row r="15" spans="1:25" ht="224" x14ac:dyDescent="0.2">
       <c r="A15" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B15" s="101"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
       <c r="E15" s="101" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" s="105" t="s">
         <v>225</v>
-      </c>
-      <c r="F15" s="105" t="s">
-        <v>226</v>
       </c>
       <c r="G15" s="106"/>
       <c r="H15" s="79">
@@ -5501,13 +5482,13 @@
         <v>0</v>
       </c>
       <c r="P15" s="81" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q15" s="81" t="s">
         <v>227</v>
       </c>
-      <c r="Q15" s="81" t="s">
+      <c r="R15" s="81" t="s">
         <v>228</v>
-      </c>
-      <c r="R15" s="81" t="s">
-        <v>229</v>
       </c>
       <c r="S15" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G15:R15)</f>
@@ -5518,7 +5499,7 @@
       <c r="V15" s="108"/>
       <c r="W15" s="108"/>
       <c r="X15" s="81" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Y15" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G15:X15)</f>
@@ -5527,7 +5508,7 @@
     </row>
     <row r="16" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" s="101"/>
       <c r="C16" s="101"/>
@@ -5539,61 +5520,61 @@
         <v>44</v>
       </c>
       <c r="G16" s="81" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H16" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G16:G16)</f>
         <v>0</v>
       </c>
       <c r="I16" s="81" t="s">
+        <v>231</v>
+      </c>
+      <c r="J16" s="81" t="s">
         <v>232</v>
       </c>
-      <c r="J16" s="81" t="s">
+      <c r="K16" s="81" t="s">
         <v>233</v>
       </c>
-      <c r="K16" s="81" t="s">
+      <c r="L16" s="81" t="s">
         <v>234</v>
       </c>
-      <c r="L16" s="81" t="s">
+      <c r="M16" s="81" t="s">
         <v>235</v>
       </c>
-      <c r="M16" s="81" t="s">
+      <c r="N16" s="81" t="s">
         <v>236</v>
-      </c>
-      <c r="N16" s="81" t="s">
-        <v>237</v>
       </c>
       <c r="O16" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G16:N16)</f>
         <v>0</v>
       </c>
       <c r="P16" s="81" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q16" s="81" t="s">
         <v>238</v>
       </c>
-      <c r="Q16" s="81" t="s">
+      <c r="R16" s="81" t="s">
         <v>239</v>
-      </c>
-      <c r="R16" s="81" t="s">
-        <v>240</v>
       </c>
       <c r="S16" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G16:R16)</f>
         <v>0</v>
       </c>
       <c r="T16" s="81" t="s">
+        <v>240</v>
+      </c>
+      <c r="U16" s="81" t="s">
         <v>241</v>
       </c>
-      <c r="U16" s="81" t="s">
+      <c r="V16" s="81" t="s">
         <v>242</v>
       </c>
-      <c r="V16" s="81" t="s">
+      <c r="W16" s="81" t="s">
         <v>243</v>
       </c>
-      <c r="W16" s="81" t="s">
+      <c r="X16" s="81" t="s">
         <v>244</v>
-      </c>
-      <c r="X16" s="81" t="s">
-        <v>245</v>
       </c>
       <c r="Y16" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G16:X16)</f>
@@ -6027,7 +6008,7 @@
   <sheetPr codeName="Feuil13">
     <tabColor rgb="FF2C45E0"/>
   </sheetPr>
-  <dimension ref="A1:FG4"/>
+  <dimension ref="A1:FB4"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -6044,13 +6025,11 @@
     <col min="129" max="155" width="16.83203125" customWidth="1"/>
     <col min="156" max="156" width="20" customWidth="1"/>
     <col min="157" max="157" width="17" customWidth="1"/>
-    <col min="161" max="161" width="17.33203125" customWidth="1"/>
-    <col min="162" max="162" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:163" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:158" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>108</v>
       </c>
@@ -6062,19 +6041,14 @@
       <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="FA1" s="145" t="s">
-        <v>110</v>
-      </c>
-      <c r="FB1" s="145"/>
-      <c r="FC1" s="145"/>
-      <c r="FD1" s="145"/>
-      <c r="FE1" s="145"/>
-      <c r="FF1" s="145"/>
-      <c r="FG1" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:163" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="FA1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="FB1" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:158" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>8</v>
       </c>
@@ -6085,22 +6059,10 @@
         <v>34</v>
       </c>
       <c r="FB2" s="48" t="s">
-        <v>247</v>
-      </c>
-      <c r="FC2" s="48" t="s">
-        <v>248</v>
-      </c>
-      <c r="FD2" s="48" t="s">
-        <v>249</v>
-      </c>
-      <c r="FE2" s="48" t="s">
-        <v>250</v>
-      </c>
-      <c r="FF2" s="48" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="3" spans="1:163" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:158" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>11</v>
       </c>
@@ -6108,7 +6070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:163" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:158" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
@@ -6116,12 +6078,14 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
-  <mergeCells count="1">
-    <mergeCell ref="FA1:FF1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A1:FF1048576">
-    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A2:FA1048576 A1:EZ1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>AND(OR($N1&lt;&gt;"-",$O1&lt;&gt;0,$P1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FB2">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+      <formula>AND(OR($N2&lt;&gt;"-",$O2&lt;&gt;0,$P2&lt;&gt;0),ROW()&gt;2,$A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6138,7 +6102,7 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6162,7 +6126,7 @@
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D1" s="64"/>
       <c r="E1" s="7"/>
@@ -6217,28 +6181,28 @@
       <c r="D4" s="87"/>
       <c r="E4" s="87"/>
       <c r="F4" s="87"/>
-      <c r="G4" s="146" t="s">
+      <c r="G4" s="145" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="147"/>
-      <c r="I4" s="147"/>
-      <c r="J4" s="147"/>
-      <c r="K4" s="147"/>
-      <c r="L4" s="148"/>
-      <c r="M4" s="149"/>
-      <c r="N4" s="150" t="s">
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="146"/>
+      <c r="L4" s="147"/>
+      <c r="M4" s="148"/>
+      <c r="N4" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="148"/>
-      <c r="P4" s="148"/>
-      <c r="Q4" s="148"/>
-      <c r="R4" s="148"/>
-      <c r="S4" s="148"/>
-      <c r="T4" s="151"/>
-      <c r="U4" s="146" t="s">
+      <c r="O4" s="147"/>
+      <c r="P4" s="147"/>
+      <c r="Q4" s="147"/>
+      <c r="R4" s="147"/>
+      <c r="S4" s="147"/>
+      <c r="T4" s="150"/>
+      <c r="U4" s="145" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="149"/>
+      <c r="V4" s="148"/>
       <c r="W4" s="94"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -6253,7 +6217,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>14</v>
@@ -6268,13 +6232,13 @@
         <v>30</v>
       </c>
       <c r="M5" s="90" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="O5" s="93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P5" s="12" t="s">
         <v>17</v>
@@ -6289,13 +6253,13 @@
         <v>31</v>
       </c>
       <c r="T5" s="93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="U5" s="89" t="s">
         <v>29</v>
       </c>
       <c r="V5" s="90" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="W5" t="s">
         <v>20</v>
@@ -6307,16 +6271,16 @@
         <v>23</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="125" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G6" s="19" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FA,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="H6" s="91" t="str">
@@ -6324,26 +6288,26 @@
         <v/>
       </c>
       <c r="I6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FA,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"M-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="J6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FA,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"M-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="K6" s="18" t="e">
         <f>SUMIFS(
-INDEX('ETPT Format DDG'!$A:$FF,
+INDEX('ETPT Format DDG'!$A:$FA,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),'ETPT Format DDG'!$FG:$FG,"C",
+),'ETPT Format DDG'!$FB:$FB,"C",
 'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Magistrat")</f>
         <v>#N/A</v>
       </c>
       <c r="L6" s="19" t="e">
         <f>SUMIFS(
-INDEX('ETPT Format DDG'!$A:$FF,
+INDEX('ETPT Format DDG'!$A:$FA,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),
@@ -6356,7 +6320,7 @@
         <v/>
       </c>
       <c r="N6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FA,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"F-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="O6" s="91" t="str">
@@ -6364,20 +6328,20 @@
         <v/>
       </c>
       <c r="P6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FA,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"F-PLAC-ADD",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="Q6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FA,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"F-PLAC-SUB",'ETPT Format DDG'!$C:$C,$A$3)</f>
         <v>#N/A</v>
       </c>
       <c r="R6" s="18" t="e">
-        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FF,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FG:$FG,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
+        <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FA,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"C",'ETPT Format DDG'!$C:$C,$A$3,'ETPT Format DDG'!$G:$G,"Greffe")</f>
         <v>#N/A</v>
       </c>
       <c r="S6" s="19" t="e">
         <f>SUMIFS(
-INDEX('ETPT Format DDG'!$A:$FF,
+INDEX('ETPT Format DDG'!$A:$FA,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
 ),
@@ -6391,10 +6355,10 @@
       </c>
       <c r="U6" s="19" t="e">
         <f>SUMIFS(
-INDEX('ETPT Format DDG'!$A:$FF,
+INDEX('ETPT Format DDG'!$A:$FA,
 ,
 IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))
-),'ETPT Format DDG'!$FG:$FG,"C",
+),'ETPT Format DDG'!$FB:$FB,"C",
 'ETPT Format DDG'!$C:$C,$A$3,
 'ETPT Format DDG'!$G:$G,"Autour du magistrat")</f>
         <v>#N/A</v>
@@ -6435,64 +6399,64 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="14" priority="13">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L6)&lt;&gt;_xlfn.NUMBERVALUE($L7),_xlfn.NUMBERVALUE($S6)&lt;&gt;_xlfn.NUMBERVALUE($S7),_xlfn.NUMBERVALUE($U6)&lt;&gt;_xlfn.NUMBERVALUE($U7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="5" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6650,7 +6614,7 @@
       </c>
       <c r="H1"/>
       <c r="I1" s="49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M1" s="26" t="s">
         <v>0</v>
@@ -6815,33 +6779,33 @@
         <v>39</v>
       </c>
       <c r="F1" s="115" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G1" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="124" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" s="124" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" s="124" t="s">
+        <v>258</v>
+      </c>
+      <c r="G2" t="s">
         <v>259</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>260</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="D2" s="124" t="s">
-        <v>262</v>
-      </c>
-      <c r="E2" s="124" t="s">
-        <v>263</v>
-      </c>
-      <c r="F2" s="124" t="s">
-        <v>264</v>
-      </c>
-      <c r="G2" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -6889,9 +6853,9 @@
   <dimension ref="A1:BJ19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <pane xSplit="6" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="topRight" activeCell="R9" sqref="R9"/>
+      <selection pane="topRight" activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6910,7 +6874,7 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
@@ -7075,17 +7039,17 @@
         <v>94</v>
       </c>
       <c r="L3" s="120" t="s">
+        <v>140</v>
+      </c>
+      <c r="M3" s="120" t="s">
         <v>141</v>
-      </c>
-      <c r="M3" s="120" t="s">
-        <v>142</v>
       </c>
       <c r="N3" s="120" t="s">
         <v>93</v>
       </c>
       <c r="O3" s="123"/>
       <c r="P3" s="120" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q3" s="120" t="s">
         <v>91</v>
@@ -7101,10 +7065,10 @@
         <v>89</v>
       </c>
       <c r="V3" s="120" t="s">
+        <v>143</v>
+      </c>
+      <c r="W3" s="120" t="s">
         <v>144</v>
-      </c>
-      <c r="W3" s="120" t="s">
-        <v>145</v>
       </c>
       <c r="X3" s="120" t="s">
         <v>88</v>
@@ -7114,7 +7078,7 @@
         <v>87</v>
       </c>
       <c r="AA3" s="120" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="AB3" s="120" t="s">
         <v>86</v>
@@ -7158,17 +7122,17 @@
         <v>76</v>
       </c>
       <c r="L4" s="120" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="120" t="s">
         <v>146</v>
-      </c>
-      <c r="M4" s="120" t="s">
-        <v>147</v>
       </c>
       <c r="N4" s="120" t="s">
         <v>75</v>
       </c>
       <c r="O4" s="123"/>
       <c r="P4" s="120" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q4" s="120" t="s">
         <v>73</v>
@@ -7184,10 +7148,10 @@
         <v>71</v>
       </c>
       <c r="V4" s="120" t="s">
+        <v>148</v>
+      </c>
+      <c r="W4" s="120" t="s">
         <v>149</v>
-      </c>
-      <c r="W4" s="120" t="s">
-        <v>150</v>
       </c>
       <c r="X4" s="120" t="s">
         <v>70</v>
@@ -7197,7 +7161,7 @@
         <v>69</v>
       </c>
       <c r="AA4" s="120" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="AB4" s="120" t="s">
         <v>68</v>
@@ -7215,7 +7179,7 @@
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="47" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E5" s="117" t="s">
         <v>65</v>
@@ -7224,8 +7188,8 @@
         <v>64</v>
       </c>
       <c r="G5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
         <v>#N/A</v>
       </c>
       <c r="H5" s="79" t="e">
@@ -7233,19 +7197,19 @@
         <v>#N/A</v>
       </c>
       <c r="I5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="J5" s="103"/>
       <c r="K5" s="103"/>
       <c r="L5" s="103"/>
       <c r="M5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="N5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="O5" s="79" t="e">
@@ -7253,18 +7217,18 @@
         <v>#N/A</v>
       </c>
       <c r="P5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
         <v>#N/A</v>
       </c>
       <c r="Q5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
         <v>#N/A</v>
       </c>
       <c r="R5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
         <v>#N/A</v>
       </c>
       <c r="S5" s="79" t="e">
@@ -7275,12 +7239,12 @@
       <c r="U5" s="103"/>
       <c r="V5" s="103"/>
       <c r="W5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="X5" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="Y5" s="79" t="e">
@@ -7302,7 +7266,7 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="38" t="str">
-        <f t="shared" ref="D6:D15" si="0">IF(ISBLANK($D$5),"",$D$5)</f>
+        <f>IF(ISBLANK($D$5),"",$D$5)</f>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
       <c r="E6" s="117" t="s">
@@ -7312,8 +7276,8 @@
         <v>62</v>
       </c>
       <c r="G6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
         <v>#N/A</v>
       </c>
       <c r="H6" s="79" t="e">
@@ -7322,91 +7286,91 @@
       </c>
       <c r="I6" s="103"/>
       <c r="J6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="K6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="L6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="M6" s="103"/>
       <c r="N6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")  +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="O6" s="79" t="e">
-        <f t="shared" ref="O6:O15" si="1">SUM(I6:N6)</f>
+        <f t="shared" ref="O6:O15" si="0">SUM(I6:N6)</f>
         <v>#N/A</v>
       </c>
       <c r="P6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
         <v>#N/A</v>
       </c>
       <c r="Q6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
         <v>#N/A</v>
       </c>
       <c r="R6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.10. AUTRES FONCTIONNAIRES / JA AFFECTÉS AU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
         <v>#N/A</v>
       </c>
       <c r="S6" s="79" t="e">
-        <f t="shared" ref="S6:S16" si="2">SUM(P6:R6)</f>
+        <f t="shared" ref="S6:S16" si="1">SUM(P6:R6)</f>
         <v>#N/A</v>
       </c>
       <c r="T6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="U6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="V6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="W6" s="103"/>
       <c r="X6" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="Y6" s="79" t="e">
-        <f t="shared" ref="Y6:Y16" si="3">SUM(T6:X6)</f>
+        <f t="shared" ref="Y6:Y16" si="2">SUM(T6:X6)</f>
         <v>#N/A</v>
       </c>
       <c r="Z6" s="103"/>
@@ -7415,7 +7379,7 @@
       <c r="AC6" s="103"/>
       <c r="AD6" s="103"/>
       <c r="AE6" s="79">
-        <f t="shared" ref="AE6:AE15" si="4">SUM(Z6:AD6)</f>
+        <f t="shared" ref="AE6:AE15" si="3">SUM(Z6:AD6)</f>
         <v>0</v>
       </c>
     </row>
@@ -7424,7 +7388,7 @@
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D7:D15" si="4">IF(ISBLANK($D$5),"",$D$5)</f>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
       <c r="E7" s="117" t="s">
@@ -7445,14 +7409,14 @@
       <c r="M7" s="103"/>
       <c r="N7" s="103"/>
       <c r="O7" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P7" s="103"/>
       <c r="Q7" s="103"/>
       <c r="R7" s="103"/>
       <c r="S7" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T7" s="103"/>
@@ -7460,11 +7424,11 @@
       <c r="V7" s="103"/>
       <c r="W7" s="103"/>
       <c r="X7" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.4 CSM",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.4 CSM",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="Y7" s="79" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="Z7" s="103"/>
@@ -7473,7 +7437,7 @@
       <c r="AC7" s="103"/>
       <c r="AD7" s="103"/>
       <c r="AE7" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7482,7 +7446,7 @@
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
       <c r="E8" s="117" t="s">
@@ -7492,7 +7456,7 @@
         <v>58</v>
       </c>
       <c r="G8" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
         <v>#N/A</v>
       </c>
       <c r="H8" s="79" t="e">
@@ -7505,27 +7469,27 @@
       <c r="L8" s="103"/>
       <c r="M8" s="103"/>
       <c r="N8" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="O8" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P8" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q8" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R8" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S8" s="79" t="e">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P8" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q8" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R8" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S8" s="79" t="e">
-        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="T8" s="103"/>
@@ -7533,11 +7497,11 @@
       <c r="V8" s="103"/>
       <c r="W8" s="103"/>
       <c r="X8" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="Y8" s="79" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="Z8" s="103"/>
@@ -7546,7 +7510,7 @@
       <c r="AC8" s="103"/>
       <c r="AD8" s="103"/>
       <c r="AE8" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7555,7 +7519,7 @@
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
       <c r="D9" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
       <c r="E9" s="117" t="s">
@@ -7564,54 +7528,54 @@
       <c r="F9" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="79">
+      <c r="G9" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H9" s="79" t="e">
         <f>SUM(G9)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I9" s="103"/>
       <c r="J9" s="103"/>
       <c r="K9" s="103"/>
       <c r="L9" s="103"/>
       <c r="M9" s="103"/>
-      <c r="N9" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="79">
+      <c r="N9" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="O9" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P9" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q9" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R9" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S9" s="79" t="e">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
-        <v>0</v>
-      </c>
-      <c r="R9" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
-        <v>0</v>
-      </c>
-      <c r="S9" s="79">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="T9" s="103"/>
       <c r="U9" s="103"/>
       <c r="V9" s="103"/>
       <c r="W9" s="103"/>
-      <c r="X9" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
-        <v>0</v>
-      </c>
-      <c r="Y9" s="79">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="X9" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y9" s="79" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
       </c>
       <c r="Z9" s="103"/>
       <c r="AA9" s="103"/>
@@ -7619,7 +7583,7 @@
       <c r="AC9" s="103"/>
       <c r="AD9" s="103"/>
       <c r="AE9" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7628,7 +7592,7 @@
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
       <c r="E10" s="117" t="s">
@@ -7638,7 +7602,7 @@
         <v>54</v>
       </c>
       <c r="G10" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
         <v>#N/A</v>
       </c>
       <c r="H10" s="79" t="e">
@@ -7651,27 +7615,27 @@
       <c r="L10" s="103"/>
       <c r="M10" s="103"/>
       <c r="N10" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="O10" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P10" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q10" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R10" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S10" s="79" t="e">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P10" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q10" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R10" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S10" s="79" t="e">
-        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="T10" s="103"/>
@@ -7679,11 +7643,11 @@
       <c r="V10" s="103"/>
       <c r="W10" s="103"/>
       <c r="X10" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="Y10" s="79" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="Z10" s="103"/>
@@ -7692,7 +7656,7 @@
       <c r="AC10" s="103"/>
       <c r="AD10" s="103"/>
       <c r="AE10" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7701,7 +7665,7 @@
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
       <c r="D11" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
       <c r="E11" s="117" t="s">
@@ -7711,7 +7675,7 @@
         <v>52</v>
       </c>
       <c r="G11" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
         <v>#N/A</v>
       </c>
       <c r="H11" s="79" t="e">
@@ -7724,27 +7688,27 @@
       <c r="L11" s="103"/>
       <c r="M11" s="103"/>
       <c r="N11" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="O11" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P11" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q11" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R11" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S11" s="79" t="e">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P11" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q11" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R11" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S11" s="79" t="e">
-        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="T11" s="103"/>
@@ -7752,11 +7716,11 @@
       <c r="V11" s="103"/>
       <c r="W11" s="103"/>
       <c r="X11" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="Y11" s="79" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="Z11" s="103"/>
@@ -7765,7 +7729,7 @@
       <c r="AC11" s="103"/>
       <c r="AD11" s="103"/>
       <c r="AE11" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7774,7 +7738,7 @@
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
       <c r="D12" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
       <c r="E12" s="117" t="s">
@@ -7784,8 +7748,8 @@
         <v>50</v>
       </c>
       <c r="G12" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
         <v>#N/A</v>
       </c>
       <c r="H12" s="79" t="e">
@@ -7798,31 +7762,31 @@
       <c r="L12" s="103"/>
       <c r="M12" s="103"/>
       <c r="N12" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="O12" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P12" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q12" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R12" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S12" s="79" t="e">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P12" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q12" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R12" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S12" s="79" t="e">
-        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="T12" s="103"/>
@@ -7830,12 +7794,12 @@
       <c r="V12" s="103"/>
       <c r="W12" s="103"/>
       <c r="X12" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="Y12" s="79" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="Z12" s="103"/>
@@ -7844,7 +7808,7 @@
       <c r="AC12" s="103"/>
       <c r="AD12" s="103"/>
       <c r="AE12" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7863,7 +7827,7 @@
         <v>48</v>
       </c>
       <c r="G13" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
         <v>#N/A</v>
       </c>
       <c r="H13" s="79" t="e">
@@ -7876,27 +7840,27 @@
       <c r="L13" s="103"/>
       <c r="M13" s="103"/>
       <c r="N13" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR")</f>
         <v>#N/A</v>
       </c>
       <c r="O13" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P13" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q13" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R13" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S13" s="79" t="e">
         <f t="shared" si="1"/>
-        <v>#N/A</v>
-      </c>
-      <c r="P13" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q13" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R13" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S13" s="79" t="e">
-        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="T13" s="103"/>
@@ -7904,11 +7868,11 @@
       <c r="V13" s="103"/>
       <c r="W13" s="103"/>
       <c r="X13" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE")</f>
         <v>#N/A</v>
       </c>
       <c r="Y13" s="79" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="Z13" s="103"/>
@@ -7917,7 +7881,7 @@
       <c r="AC13" s="103"/>
       <c r="AD13" s="103"/>
       <c r="AE13" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7935,109 +7899,109 @@
       <c r="F14" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="79">
+      <c r="G14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H14" s="79" t="e">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
         <v>#N/A</v>
       </c>
       <c r="J14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
         <v>#N/A</v>
       </c>
       <c r="K14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
         <v>#N/A</v>
       </c>
       <c r="L14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
         <v>#N/A</v>
       </c>
       <c r="M14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
         <v>#N/A</v>
       </c>
       <c r="N14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD")</f>
         <v>#N/A</v>
       </c>
       <c r="O14" s="79" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="P14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S14" s="79" t="e">
         <f t="shared" si="1"/>
         <v>#N/A</v>
       </c>
-      <c r="P14" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales placé ADD")</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres placé ADD")</f>
-        <v>0</v>
-      </c>
-      <c r="R14" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général placé ADD")</f>
-        <v>0</v>
-      </c>
-      <c r="S14" s="79">
+      <c r="T14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="W14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X14" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y14" s="79" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé ADD")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X14" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y14" s="79" t="e">
-        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="Z14" s="103"/>
@@ -8046,20 +8010,20 @@
       <c r="AC14" s="103"/>
       <c r="AD14" s="103"/>
       <c r="AE14" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:62" x14ac:dyDescent="0.2">
       <c r="D15" s="38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
       <c r="E15" s="117" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" s="117" t="s">
         <v>225</v>
-      </c>
-      <c r="F15" s="117" t="s">
-        <v>226</v>
       </c>
       <c r="G15" s="103"/>
       <c r="H15" s="79">
@@ -8073,26 +8037,26 @@
       <c r="M15" s="103"/>
       <c r="N15" s="103"/>
       <c r="O15" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q15" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R15" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S15" s="79" t="e">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q15" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres placé SUB")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R15" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général placé SUB")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S15" s="79" t="e">
-        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="T15" s="103"/>
@@ -8100,12 +8064,12 @@
       <c r="V15" s="103"/>
       <c r="W15" s="103"/>
       <c r="X15" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="Y15" s="79" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
       <c r="Z15" s="103"/>
@@ -8114,7 +8078,7 @@
       <c r="AC15" s="103"/>
       <c r="AD15" s="103"/>
       <c r="AE15" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -8126,109 +8090,109 @@
       <c r="F16" s="117" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="79">
+      <c r="G16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="H16" s="79" t="e">
         <f>SUM(G16)</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="I16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="J16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="K16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="L16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="M16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="N16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB") -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB") -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.9. FONCTIONNAIRES / JA AFFECTÉS AUX ACTIVITÉS CIVILES ET COMMERCIALES DU PARQUET GÉNÉRAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="O16" s="79" t="e">
         <f>SUM(I16:N16)</f>
         <v>#N/A</v>
       </c>
-      <c r="P16" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales placé SUB")</f>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres placé SUB")</f>
-        <v>0</v>
-      </c>
-      <c r="R16" s="103">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général placé SUB")</f>
-        <v>0</v>
-      </c>
-      <c r="S16" s="79">
+      <c r="P16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS chambres sociales placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS siège Autres placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"JURISTE AS parquet général placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="S16" s="79" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="T16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="V16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")+
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="W16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="X16" s="103" t="e">
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Y16" s="79" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="V16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")+
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat SIEGE placé SUB")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="X16" s="103" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.1. ASSISES HORS JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.2 ASSISES JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("11.3. COUR CRIMINELLE DÉPARTEMENTALE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.4. CONTENTIEUX JIRS CRIM-ORG",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("8.7. CONTENTIEUX JIRS ÉCO-FI",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.3. CONTENTIEUX DE LA DÉTENTION JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.5. CONTENTIEUX DU CONTRÔLE JUDICIAIRE JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("9.7. CONTENTIEUX DE FOND JIRS",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")  -
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("1. TOTAL CONTENTIEUX SOCIAL",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Magistrat placé SUB")</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Y16" s="79" t="e">
-        <f t="shared" si="3"/>
         <v>#N/A</v>
       </c>
       <c r="Z16" s="103"/>
@@ -8351,19 +8315,19 @@
     <row r="19" spans="1:31" customFormat="1" ht="102.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="F19" s="121" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="G19" s="81" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="M19" s="122" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="N19" s="81" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8381,7 +8345,7 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8407,12 +8371,12 @@
   <sheetData>
     <row r="1" spans="1:31" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
@@ -8546,17 +8510,17 @@
         <v>94</v>
       </c>
       <c r="L3" s="120" t="s">
+        <v>140</v>
+      </c>
+      <c r="M3" s="120" t="s">
         <v>141</v>
-      </c>
-      <c r="M3" s="120" t="s">
-        <v>142</v>
       </c>
       <c r="N3" s="120" t="s">
         <v>93</v>
       </c>
       <c r="O3" s="123"/>
       <c r="P3" s="120" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q3" s="120" t="s">
         <v>91</v>
@@ -8572,10 +8536,10 @@
         <v>89</v>
       </c>
       <c r="V3" s="120" t="s">
+        <v>143</v>
+      </c>
+      <c r="W3" s="120" t="s">
         <v>144</v>
-      </c>
-      <c r="W3" s="120" t="s">
-        <v>145</v>
       </c>
       <c r="X3" s="120" t="s">
         <v>88</v>
@@ -8585,7 +8549,7 @@
         <v>87</v>
       </c>
       <c r="AA3" s="120" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="AB3" s="120" t="s">
         <v>86</v>
@@ -8629,17 +8593,17 @@
         <v>76</v>
       </c>
       <c r="L4" s="120" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="120" t="s">
         <v>146</v>
-      </c>
-      <c r="M4" s="120" t="s">
-        <v>147</v>
       </c>
       <c r="N4" s="120" t="s">
         <v>75</v>
       </c>
       <c r="O4" s="123"/>
       <c r="P4" s="120" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="Q4" s="120" t="s">
         <v>73</v>
@@ -8655,10 +8619,10 @@
         <v>71</v>
       </c>
       <c r="V4" s="120" t="s">
+        <v>148</v>
+      </c>
+      <c r="W4" s="120" t="s">
         <v>149</v>
-      </c>
-      <c r="W4" s="120" t="s">
-        <v>150</v>
       </c>
       <c r="X4" s="120" t="s">
         <v>70</v>
@@ -8668,7 +8632,7 @@
         <v>69</v>
       </c>
       <c r="AA4" s="120" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="AB4" s="120" t="s">
         <v>68</v>
@@ -8685,7 +8649,9 @@
       <c r="A5" s="42"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
-      <c r="D5" s="47"/>
+      <c r="D5" s="47" t="s">
+        <v>261</v>
+      </c>
       <c r="E5" s="117" t="s">
         <v>65</v>
       </c>
@@ -8798,8 +8764,8 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="38" t="str">
-        <f t="shared" ref="D6:D15" si="0">IF(ISBLANK($D$5),"",$D$5)</f>
-        <v/>
+        <f>IF(ISBLANK($D$5),"",$D$5)</f>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E6" s="117" t="s">
         <v>63</v>
@@ -8840,7 +8806,7 @@
         <v/>
       </c>
       <c r="O6" s="79">
-        <f t="shared" ref="O6:O15" si="1">SUM(I6:N6)</f>
+        <f t="shared" ref="O6:O15" si="0">SUM(I6:N6)</f>
         <v>0</v>
       </c>
       <c r="P6" s="103" t="str">
@@ -8856,7 +8822,7 @@
         <v/>
       </c>
       <c r="S6" s="79">
-        <f t="shared" ref="S6:S16" si="2">SUM(P6:R6)</f>
+        <f t="shared" ref="S6:S16" si="1">SUM(P6:R6)</f>
         <v>0</v>
       </c>
       <c r="T6" s="103" t="str">
@@ -8880,7 +8846,7 @@
         <v/>
       </c>
       <c r="Y6" s="79">
-        <f t="shared" ref="Y6:Y16" si="3">SUM(T6:X6)</f>
+        <f t="shared" ref="Y6:Y16" si="2">SUM(T6:X6)</f>
         <v>0</v>
       </c>
       <c r="Z6" s="103" t="str">
@@ -8904,7 +8870,7 @@
         <v/>
       </c>
       <c r="AE6" s="79">
-        <f t="shared" ref="AE6:AE15" si="4">SUM(Z6:AD6)</f>
+        <f t="shared" ref="AE6:AE15" si="3">SUM(Z6:AD6)</f>
         <v>0</v>
       </c>
     </row>
@@ -8913,8 +8879,8 @@
       <c r="B7" s="41"/>
       <c r="C7" s="41"/>
       <c r="D7" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" ref="D7:D15" si="4">IF(ISBLANK($D$5),"",$D$5)</f>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E7" s="117" t="s">
         <v>61</v>
@@ -8955,7 +8921,7 @@
         <v/>
       </c>
       <c r="O7" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P7" s="103" t="str">
@@ -8971,7 +8937,7 @@
         <v/>
       </c>
       <c r="S7" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T7" s="103" t="str">
@@ -8995,7 +8961,7 @@
         <v/>
       </c>
       <c r="Y7" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z7" s="103" t="str">
@@ -9019,7 +8985,7 @@
         <v/>
       </c>
       <c r="AE7" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9028,8 +8994,8 @@
       <c r="B8" s="41"/>
       <c r="C8" s="41"/>
       <c r="D8" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E8" s="117" t="s">
         <v>59</v>
@@ -9070,7 +9036,7 @@
         <v/>
       </c>
       <c r="O8" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P8" s="103" t="str">
@@ -9086,7 +9052,7 @@
         <v/>
       </c>
       <c r="S8" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T8" s="103" t="str">
@@ -9110,7 +9076,7 @@
         <v/>
       </c>
       <c r="Y8" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z8" s="103" t="str">
@@ -9134,7 +9100,7 @@
         <v/>
       </c>
       <c r="AE8" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9143,8 +9109,8 @@
       <c r="B9" s="41"/>
       <c r="C9" s="41"/>
       <c r="D9" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E9" s="117" t="s">
         <v>57</v>
@@ -9185,7 +9151,7 @@
         <v/>
       </c>
       <c r="O9" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P9" s="103" t="str">
@@ -9201,7 +9167,7 @@
         <v/>
       </c>
       <c r="S9" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T9" s="103" t="str">
@@ -9225,7 +9191,7 @@
         <v/>
       </c>
       <c r="Y9" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z9" s="103" t="str">
@@ -9249,7 +9215,7 @@
         <v/>
       </c>
       <c r="AE9" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9258,8 +9224,8 @@
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
       <c r="D10" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E10" s="117" t="s">
         <v>55</v>
@@ -9300,7 +9266,7 @@
         <v/>
       </c>
       <c r="O10" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P10" s="103" t="str">
@@ -9316,7 +9282,7 @@
         <v/>
       </c>
       <c r="S10" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T10" s="103" t="str">
@@ -9340,7 +9306,7 @@
         <v/>
       </c>
       <c r="Y10" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z10" s="103" t="str">
@@ -9364,7 +9330,7 @@
         <v/>
       </c>
       <c r="AE10" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9373,8 +9339,8 @@
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
       <c r="D11" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E11" s="117" t="s">
         <v>53</v>
@@ -9415,7 +9381,7 @@
         <v/>
       </c>
       <c r="O11" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P11" s="103" t="str">
@@ -9431,7 +9397,7 @@
         <v/>
       </c>
       <c r="S11" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T11" s="103" t="str">
@@ -9455,7 +9421,7 @@
         <v/>
       </c>
       <c r="Y11" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z11" s="103" t="str">
@@ -9479,7 +9445,7 @@
         <v/>
       </c>
       <c r="AE11" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9488,8 +9454,8 @@
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
       <c r="D12" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E12" s="117" t="s">
         <v>51</v>
@@ -9530,7 +9496,7 @@
         <v/>
       </c>
       <c r="O12" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P12" s="103" t="str">
@@ -9546,7 +9512,7 @@
         <v/>
       </c>
       <c r="S12" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T12" s="103" t="str">
@@ -9570,7 +9536,7 @@
         <v/>
       </c>
       <c r="Y12" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z12" s="103" t="str">
@@ -9594,7 +9560,7 @@
         <v/>
       </c>
       <c r="AE12" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9603,8 +9569,8 @@
       <c r="B13" s="41"/>
       <c r="C13" s="41"/>
       <c r="D13" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E13" s="117" t="s">
         <v>49</v>
@@ -9645,7 +9611,7 @@
         <v/>
       </c>
       <c r="O13" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P13" s="103" t="str">
@@ -9661,7 +9627,7 @@
         <v/>
       </c>
       <c r="S13" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T13" s="103" t="str">
@@ -9685,7 +9651,7 @@
         <v/>
       </c>
       <c r="Y13" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z13" s="103" t="str">
@@ -9709,7 +9675,7 @@
         <v/>
       </c>
       <c r="AE13" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9718,8 +9684,8 @@
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E14" s="117" t="s">
         <v>47</v>
@@ -9760,7 +9726,7 @@
         <v/>
       </c>
       <c r="O14" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P14" s="103" t="str">
@@ -9776,7 +9742,7 @@
         <v/>
       </c>
       <c r="S14" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T14" s="103" t="str">
@@ -9800,7 +9766,7 @@
         <v/>
       </c>
       <c r="Y14" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z14" s="103" t="str">
@@ -9824,20 +9790,20 @@
         <v/>
       </c>
       <c r="AE14" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="D15" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f t="shared" si="4"/>
+        <v>=ETPT_CA_JUR!D5</v>
       </c>
       <c r="E15" s="117" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" s="117" t="s">
         <v>225</v>
-      </c>
-      <c r="F15" s="117" t="s">
-        <v>226</v>
       </c>
       <c r="G15" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G15),"",IF(ETPT_CA_JUR!G15=0,"",ETPT_CA_JUR!G15)))</f>
@@ -9872,7 +9838,7 @@
         <v/>
       </c>
       <c r="O15" s="79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P15" s="103" t="str">
@@ -9888,7 +9854,7 @@
         <v/>
       </c>
       <c r="S15" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T15" s="103" t="str">
@@ -9912,7 +9878,7 @@
         <v/>
       </c>
       <c r="Y15" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z15" s="103" t="str">
@@ -9936,7 +9902,7 @@
         <v/>
       </c>
       <c r="AE15" s="79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -9997,7 +9963,7 @@
         <v/>
       </c>
       <c r="S16" s="79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T16" s="103" t="str">
@@ -10021,7 +9987,7 @@
         <v/>
       </c>
       <c r="Y16" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Z16" s="103" t="str">
@@ -10163,11 +10129,11 @@
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19" s="121" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="G19" s="81" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="H19"/>
@@ -10176,11 +10142,11 @@
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19" s="122" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="N19" s="81" t="e">
-        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
-SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FF,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
+        <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
+SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé SUB")</f>
         <v>#N/A</v>
       </c>
       <c r="O19"/>

</xml_diff>

<commit_message>
update tj formulas and ca formulas for red flags
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59FE00-0DE0-B74A-85D2-839147B6F581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2295E3-2210-BD4B-8397-364EAA6F4CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="3" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -3468,7 +3468,47 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3608,26 +3648,6 @@
       <font>
         <color theme="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6013,11 +6033,11 @@
   </sheetPr>
   <dimension ref="A1:FB4"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6085,13 +6105,13 @@
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <conditionalFormatting sqref="A1:EZ1 A2:FB1048576">
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
-      <formula>AND(OR($N1&lt;&gt;"-",$O1&lt;&gt;0,$P1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+      <formula>AND(OR($Q1&lt;&gt;"-",$R1&lt;&gt;0,$S1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FB2">
-    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
-      <formula>AND(OR($N2&lt;&gt;"-",$O2&lt;&gt;0,$P2&lt;&gt;0),ROW()&gt;2,$A2&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+      <formula>AND(OR($Q2&lt;&gt;"-",$R2&lt;&gt;0,$S2&lt;&gt;0),ROW()&gt;2,$A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6107,7 +6127,7 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -6405,64 +6425,64 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="12" priority="15">
+    <cfRule type="expression" dxfId="16" priority="15">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="10" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L6)&lt;&gt;_xlfn.NUMBERVALUE($L7),_xlfn.NUMBERVALUE($S6)&lt;&gt;_xlfn.NUMBERVALUE($S7),_xlfn.NUMBERVALUE($U6)&lt;&gt;_xlfn.NUMBERVALUE($U7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="8" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="4" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update ca fct extractor
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2295E3-2210-BD4B-8397-364EAA6F4CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B912543D-DB11-D549-B65C-628E6050E5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="2" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="6" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId2"/>
     <sheet name="ETPT Format DDG" sheetId="9" r:id="rId3"/>
     <sheet name="Agrégats DDG" sheetId="10" r:id="rId4"/>
-    <sheet name="codage tribunal" sheetId="12" state="hidden" r:id="rId5"/>
-    <sheet name="Juridictions" sheetId="17" state="hidden" r:id="rId6"/>
-    <sheet name="Table_Fonctions" sheetId="19" state="hidden" r:id="rId7"/>
-    <sheet name="ETPT_CA_JUR" sheetId="30" state="hidden" r:id="rId8"/>
+    <sheet name="codage tribunal" sheetId="12" r:id="rId5"/>
+    <sheet name="Juridictions" sheetId="17" r:id="rId6"/>
+    <sheet name="Table_Fonctions" sheetId="19" r:id="rId7"/>
+    <sheet name="ETPT_CA_JUR" sheetId="30" r:id="rId8"/>
     <sheet name="ETPT_CA_JUR_DDG" sheetId="25" r:id="rId9"/>
-    <sheet name="ETPT_CA_JUR Corresp" sheetId="38" state="hidden" r:id="rId10"/>
+    <sheet name="ETPT_CA_JUR Corresp" sheetId="38" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="265">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Juridiction</t>
   </si>
   <si>
-    <t>Fonction</t>
-  </si>
-  <si>
     <t>Fonction recodée</t>
   </si>
   <si>
@@ -167,18 +164,6 @@
   </si>
   <si>
     <t>JURISTE AS</t>
-  </si>
-  <si>
-    <t>CODE EXTRACTEUR</t>
-  </si>
-  <si>
-    <t>Titulaire / Placé / Contractuel</t>
-  </si>
-  <si>
-    <t>Raccourci</t>
-  </si>
-  <si>
-    <t>Catégorie(s)</t>
   </si>
   <si>
     <t>TOTAL ETPT</t>
@@ -2109,9 +2094,6 @@
     </r>
   </si>
   <si>
-    <t>Correspondance</t>
-  </si>
-  <si>
     <t>PARQUET_JIRS</t>
   </si>
   <si>
@@ -2164,6 +2146,27 @@
   </si>
   <si>
     <t>#! DUMP_COLS subtitles1</t>
+  </si>
+  <si>
+    <t>CONCAT</t>
+  </si>
+  <si>
+    <t>Catégorie</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Fonction recodée DDG</t>
+  </si>
+  <si>
+    <t>Fonction onglet agrégat</t>
+  </si>
+  <si>
+    <t>## f.CONCAT</t>
   </si>
 </sst>
 </file>
@@ -2503,7 +2506,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2621,12 +2624,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B252"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3005,7 +3002,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3339,15 +3336,6 @@
     <xf numFmtId="49" fontId="45" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="20" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3457,6 +3445,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3468,47 +3462,7 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3648,6 +3602,26 @@
       <font>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4420,13 +4394,13 @@
     <row r="1" spans="1:8" s="26" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="50"/>
       <c r="B1" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="126" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
+        <v>106</v>
+      </c>
+      <c r="C1" s="123" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
       <c r="F1" s="52"/>
       <c r="H1" s="26" t="s">
         <v>0</v>
@@ -4435,11 +4409,11 @@
     <row r="2" spans="1:8" s="56" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="53"/>
       <c r="B2" s="54"/>
-      <c r="C2" s="127" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
+      <c r="C2" s="124" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
       <c r="F2" s="55"/>
       <c r="H2" s="26" t="s">
         <v>0</v>
@@ -4455,18 +4429,18 @@
     <row r="4" spans="1:8" s="62" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="60" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D4" s="61" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" s="133" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" s="134"/>
+        <v>110</v>
+      </c>
+      <c r="E4" s="130" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="131"/>
       <c r="G4" s="68"/>
       <c r="H4" s="26" t="s">
         <v>0</v>
@@ -4475,18 +4449,18 @@
     <row r="5" spans="1:8" s="26" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="57"/>
       <c r="B5" s="72" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="135" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="136"/>
+        <v>114</v>
+      </c>
+      <c r="E5" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="133"/>
       <c r="G5" s="67"/>
       <c r="H5" s="26" t="s">
         <v>0</v>
@@ -4495,18 +4469,18 @@
     <row r="6" spans="1:8" s="26" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="57"/>
       <c r="B6" s="73" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D6" s="66" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" s="137" t="s">
-        <v>133</v>
-      </c>
-      <c r="F6" s="138"/>
+        <v>117</v>
+      </c>
+      <c r="E6" s="134" t="s">
+        <v>128</v>
+      </c>
+      <c r="F6" s="135"/>
       <c r="G6" s="67"/>
       <c r="H6" s="26" t="s">
         <v>0</v>
@@ -4515,18 +4489,18 @@
     <row r="7" spans="1:8" s="26" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="57"/>
       <c r="B7" s="74" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D7" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" s="137" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="138"/>
+        <v>120</v>
+      </c>
+      <c r="E7" s="134" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="135"/>
       <c r="G7" s="67"/>
       <c r="H7" s="26" t="s">
         <v>0</v>
@@ -4535,18 +4509,18 @@
     <row r="8" spans="1:8" s="26" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="57"/>
       <c r="B8" s="75" t="s">
-        <v>126</v>
-      </c>
-      <c r="C8" s="128" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="128" t="s">
-        <v>128</v>
-      </c>
-      <c r="E8" s="139" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="140"/>
+        <v>121</v>
+      </c>
+      <c r="C8" s="125" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="125" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="136" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="137"/>
       <c r="G8" s="67"/>
       <c r="H8" s="26" t="s">
         <v>0</v>
@@ -4555,12 +4529,12 @@
     <row r="9" spans="1:8" s="26" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="57"/>
       <c r="B9" s="76" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="128"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="142"/>
+        <v>124</v>
+      </c>
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="139"/>
       <c r="G9" s="67"/>
       <c r="H9" s="26" t="s">
         <v>0</v>
@@ -4569,12 +4543,12 @@
     <row r="10" spans="1:8" s="26" customFormat="1" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="57"/>
       <c r="B10" s="77" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="129"/>
-      <c r="D10" s="129"/>
-      <c r="E10" s="143"/>
-      <c r="F10" s="144"/>
+        <v>125</v>
+      </c>
+      <c r="C10" s="126"/>
+      <c r="D10" s="126"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="141"/>
       <c r="G10" s="67"/>
       <c r="H10" s="26" t="s">
         <v>0</v>
@@ -4594,11 +4568,11 @@
     <row r="12" spans="1:8" s="26" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="57"/>
       <c r="B12" s="69"/>
-      <c r="C12" s="132" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="132"/>
-      <c r="E12" s="132"/>
+      <c r="C12" s="129" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="129"/>
+      <c r="E12" s="129"/>
       <c r="F12" s="70"/>
       <c r="H12" s="26" t="s">
         <v>0</v>
@@ -4612,14 +4586,14 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="130" t="s">
+      <c r="A14" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="130"/>
-      <c r="C14" s="130"/>
-      <c r="D14" s="130"/>
-      <c r="E14" s="130"/>
-      <c r="F14" s="131"/>
+      <c r="B14" s="127"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="127"/>
+      <c r="E14" s="127"/>
+      <c r="F14" s="128"/>
       <c r="H14" s="26" t="s">
         <v>0</v>
       </c>
@@ -4663,13 +4637,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A1" s="151" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="151"/>
-      <c r="E1" s="151"/>
+      <c r="A1" s="148" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
       <c r="F1" s="96"/>
       <c r="G1" s="78"/>
       <c r="H1" s="78"/>
@@ -4699,61 +4673,61 @@
       <c r="E2" s="97"/>
       <c r="F2" s="97"/>
       <c r="G2" s="80" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="152" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+      <c r="H2" s="149" t="s">
+        <v>100</v>
       </c>
       <c r="I2" s="80" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J2" s="80" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K2" s="80" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="L2" s="80" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M2" s="80" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="O2" s="152" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="O2" s="149" t="s">
+        <v>98</v>
       </c>
       <c r="P2" s="80" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q2" s="80" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R2" s="80" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="152" t="s">
-        <v>102</v>
+        <v>37</v>
+      </c>
+      <c r="S2" s="149" t="s">
+        <v>97</v>
       </c>
       <c r="T2" s="80" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="U2" s="80" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="V2" s="80" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="W2" s="80" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="X2" s="80" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y2" s="152" t="s">
-        <v>100</v>
+        <v>96</v>
+      </c>
+      <c r="Y2" s="149" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="56" x14ac:dyDescent="0.2">
@@ -4764,166 +4738,166 @@
       <c r="E3" s="97"/>
       <c r="F3" s="97"/>
       <c r="G3" s="80" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="152"/>
+        <v>92</v>
+      </c>
+      <c r="H3" s="149"/>
       <c r="I3" s="80" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J3" s="80" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="K3" s="80" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="L3" s="80" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="M3" s="80" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="N3" s="80" t="s">
-        <v>93</v>
-      </c>
-      <c r="O3" s="152"/>
+        <v>88</v>
+      </c>
+      <c r="O3" s="149"/>
       <c r="P3" s="80" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="Q3" s="80" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="R3" s="80" t="s">
-        <v>92</v>
-      </c>
-      <c r="S3" s="152"/>
+        <v>87</v>
+      </c>
+      <c r="S3" s="149"/>
       <c r="T3" s="80" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="U3" s="80" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="V3" s="80" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="W3" s="80" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="X3" s="80" t="s">
-        <v>88</v>
-      </c>
-      <c r="Y3" s="152"/>
+        <v>83</v>
+      </c>
+      <c r="Y3" s="149"/>
     </row>
     <row r="4" spans="1:25" ht="84" x14ac:dyDescent="0.2">
       <c r="A4" s="98"/>
       <c r="B4" s="99" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C4" s="99" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4" s="99" t="s">
         <v>32</v>
       </c>
       <c r="E4" s="99" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F4" s="99" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G4" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="152"/>
+        <v>74</v>
+      </c>
+      <c r="H4" s="149"/>
       <c r="I4" s="80" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J4" s="80" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K4" s="80" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L4" s="80" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="M4" s="80" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="N4" s="80" t="s">
-        <v>75</v>
-      </c>
-      <c r="O4" s="152"/>
+        <v>70</v>
+      </c>
+      <c r="O4" s="149"/>
       <c r="P4" s="80" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="Q4" s="80" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="R4" s="80" t="s">
-        <v>74</v>
-      </c>
-      <c r="S4" s="152"/>
+        <v>69</v>
+      </c>
+      <c r="S4" s="149"/>
       <c r="T4" s="80" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="U4" s="80" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="V4" s="80" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="W4" s="80" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="X4" s="80" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y4" s="152"/>
+        <v>65</v>
+      </c>
+      <c r="Y4" s="149"/>
     </row>
     <row r="5" spans="1:25" ht="332" x14ac:dyDescent="0.2">
       <c r="A5" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B5" s="101"/>
       <c r="C5" s="101"/>
       <c r="D5" s="101"/>
       <c r="E5" s="101" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F5" s="102" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G5" s="81" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H5" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G5:G5)</f>
         <v>0</v>
       </c>
       <c r="I5" s="81" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="J5" s="83"/>
       <c r="K5" s="83"/>
       <c r="L5" s="83"/>
       <c r="M5" s="81" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="N5" s="81" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="O5" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G5:N5)</f>
         <v>0</v>
       </c>
       <c r="P5" s="81" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="Q5" s="81" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="R5" s="81" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="S5" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G5:R5)</f>
@@ -4933,10 +4907,10 @@
       <c r="U5" s="83"/>
       <c r="V5" s="83"/>
       <c r="W5" s="81" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="X5" s="81" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="Y5" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G5:X5)</f>
@@ -4945,19 +4919,19 @@
     </row>
     <row r="6" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B6" s="101"/>
       <c r="C6" s="101"/>
       <c r="D6" s="101"/>
       <c r="E6" s="101" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F6" s="102" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H6" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G6:G6)</f>
@@ -4965,47 +4939,47 @@
       </c>
       <c r="I6" s="82"/>
       <c r="J6" s="81" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K6" s="81" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="L6" s="81" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M6" s="83"/>
       <c r="N6" s="81" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="O6" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G6:N6)</f>
         <v>0</v>
       </c>
       <c r="P6" s="81" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="Q6" s="81" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="R6" s="81" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="S6" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G6:R6)</f>
         <v>0</v>
       </c>
       <c r="T6" s="81" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="U6" s="81" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="V6" s="81" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="W6" s="83"/>
       <c r="X6" s="81" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="Y6" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G6:X6)</f>
@@ -5014,16 +4988,16 @@
     </row>
     <row r="7" spans="1:25" ht="90" x14ac:dyDescent="0.2">
       <c r="A7" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B7" s="101"/>
       <c r="C7" s="101"/>
       <c r="D7" s="101"/>
       <c r="E7" s="101" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F7" s="102" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G7" s="86"/>
       <c r="H7" s="79">
@@ -5052,7 +5026,7 @@
       <c r="V7" s="103"/>
       <c r="W7" s="103"/>
       <c r="X7" s="104" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="Y7" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G7:X7)</f>
@@ -5061,19 +5035,19 @@
     </row>
     <row r="8" spans="1:25" ht="140" x14ac:dyDescent="0.2">
       <c r="A8" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B8" s="101"/>
       <c r="C8" s="101"/>
       <c r="D8" s="101"/>
       <c r="E8" s="101" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F8" s="102" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G8" s="81" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H8" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G8:G8)</f>
@@ -5085,20 +5059,20 @@
       <c r="L8" s="85"/>
       <c r="M8" s="85"/>
       <c r="N8" s="81" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="O8" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G8:N8)</f>
         <v>0</v>
       </c>
       <c r="P8" s="81" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q8" s="81" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="R8" s="81" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="S8" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G8:R8)</f>
@@ -5109,7 +5083,7 @@
       <c r="V8" s="103"/>
       <c r="W8" s="103"/>
       <c r="X8" s="81" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="Y8" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G8:X8)</f>
@@ -5118,19 +5092,19 @@
     </row>
     <row r="9" spans="1:25" ht="154" x14ac:dyDescent="0.2">
       <c r="A9" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B9" s="101"/>
       <c r="C9" s="101"/>
       <c r="D9" s="101"/>
       <c r="E9" s="101" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F9" s="102" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H9" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G9:G9)</f>
@@ -5142,20 +5116,20 @@
       <c r="L9" s="85"/>
       <c r="M9" s="85"/>
       <c r="N9" s="81" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="O9" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G9:N9)</f>
         <v>0</v>
       </c>
       <c r="P9" s="81" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="Q9" s="81" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="R9" s="81" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="S9" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G9:R9)</f>
@@ -5166,7 +5140,7 @@
       <c r="V9" s="103"/>
       <c r="W9" s="103"/>
       <c r="X9" s="81" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="Y9" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G9:X9)</f>
@@ -5175,19 +5149,19 @@
     </row>
     <row r="10" spans="1:25" ht="140" x14ac:dyDescent="0.2">
       <c r="A10" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B10" s="101"/>
       <c r="C10" s="101"/>
       <c r="D10" s="101"/>
       <c r="E10" s="101" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F10" s="102" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G10" s="81" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H10" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G10:G10)</f>
@@ -5199,20 +5173,20 @@
       <c r="L10" s="85"/>
       <c r="M10" s="85"/>
       <c r="N10" s="81" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="O10" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G10:N10)</f>
         <v>0</v>
       </c>
       <c r="P10" s="81" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="Q10" s="81" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="R10" s="81" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="S10" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G10:R10)</f>
@@ -5223,7 +5197,7 @@
       <c r="V10" s="103"/>
       <c r="W10" s="103"/>
       <c r="X10" s="81" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="Y10" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G10:X10)</f>
@@ -5232,19 +5206,19 @@
     </row>
     <row r="11" spans="1:25" ht="140" x14ac:dyDescent="0.2">
       <c r="A11" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B11" s="101"/>
       <c r="C11" s="101"/>
       <c r="D11" s="101"/>
       <c r="E11" s="101" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F11" s="102" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G11" s="81" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H11" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G11:G11)</f>
@@ -5256,20 +5230,20 @@
       <c r="L11" s="85"/>
       <c r="M11" s="85"/>
       <c r="N11" s="81" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="O11" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G11:N11)</f>
         <v>0</v>
       </c>
       <c r="P11" s="81" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="Q11" s="81" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="R11" s="81" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="S11" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G11:R11)</f>
@@ -5280,7 +5254,7 @@
       <c r="V11" s="103"/>
       <c r="W11" s="103"/>
       <c r="X11" s="81" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="Y11" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G11:X11)</f>
@@ -5289,19 +5263,19 @@
     </row>
     <row r="12" spans="1:25" ht="168" x14ac:dyDescent="0.2">
       <c r="A12" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B12" s="101"/>
       <c r="C12" s="101"/>
       <c r="D12" s="101"/>
       <c r="E12" s="101" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F12" s="102" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G12" s="81" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H12" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G12:G12)</f>
@@ -5313,20 +5287,20 @@
       <c r="L12" s="85"/>
       <c r="M12" s="85"/>
       <c r="N12" s="81" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="O12" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G12:N12)</f>
         <v>0</v>
       </c>
       <c r="P12" s="81" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="Q12" s="81" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="R12" s="81" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="S12" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G12:R12)</f>
@@ -5337,7 +5311,7 @@
       <c r="V12" s="103"/>
       <c r="W12" s="103"/>
       <c r="X12" s="81" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="Y12" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G12:X12)</f>
@@ -5346,19 +5320,19 @@
     </row>
     <row r="13" spans="1:25" ht="126" x14ac:dyDescent="0.2">
       <c r="A13" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B13" s="101"/>
       <c r="C13" s="101"/>
       <c r="D13" s="101"/>
       <c r="E13" s="101" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F13" s="102" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G13" s="81" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H13" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G13:G13)</f>
@@ -5370,20 +5344,20 @@
       <c r="L13" s="85"/>
       <c r="M13" s="85"/>
       <c r="N13" s="81" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="O13" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G13:N13)</f>
         <v>0</v>
       </c>
       <c r="P13" s="81" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="Q13" s="81" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="R13" s="81" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="S13" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G13:R13)</f>
@@ -5394,7 +5368,7 @@
       <c r="V13" s="103"/>
       <c r="W13" s="103"/>
       <c r="X13" s="81" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="Y13" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G13:X13)</f>
@@ -5403,73 +5377,73 @@
     </row>
     <row r="14" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B14" s="101"/>
       <c r="C14" s="101"/>
       <c r="D14" s="101"/>
       <c r="E14" s="101" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F14" s="102" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G14" s="81" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H14" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G14:G14)</f>
         <v>0</v>
       </c>
       <c r="I14" s="81" t="s">
+        <v>205</v>
+      </c>
+      <c r="J14" s="81" t="s">
+        <v>206</v>
+      </c>
+      <c r="K14" s="81" t="s">
+        <v>207</v>
+      </c>
+      <c r="L14" s="81" t="s">
+        <v>208</v>
+      </c>
+      <c r="M14" s="81" t="s">
+        <v>209</v>
+      </c>
+      <c r="N14" s="81" t="s">
         <v>210</v>
-      </c>
-      <c r="J14" s="81" t="s">
-        <v>211</v>
-      </c>
-      <c r="K14" s="81" t="s">
-        <v>212</v>
-      </c>
-      <c r="L14" s="81" t="s">
-        <v>213</v>
-      </c>
-      <c r="M14" s="81" t="s">
-        <v>214</v>
-      </c>
-      <c r="N14" s="81" t="s">
-        <v>215</v>
       </c>
       <c r="O14" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G14:N14)</f>
         <v>0</v>
       </c>
       <c r="P14" s="81" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="Q14" s="81" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="R14" s="81" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="S14" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G14:R14)</f>
         <v>0</v>
       </c>
       <c r="T14" s="81" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="U14" s="81" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="V14" s="81" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="W14" s="81" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="X14" s="81" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="Y14" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G14:X14)</f>
@@ -5478,16 +5452,16 @@
     </row>
     <row r="15" spans="1:25" ht="224" x14ac:dyDescent="0.2">
       <c r="A15" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B15" s="101"/>
       <c r="C15" s="101"/>
       <c r="D15" s="101"/>
       <c r="E15" s="101" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F15" s="105" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G15" s="106"/>
       <c r="H15" s="79">
@@ -5505,13 +5479,13 @@
         <v>0</v>
       </c>
       <c r="P15" s="81" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="Q15" s="81" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="R15" s="81" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="S15" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G15:R15)</f>
@@ -5522,7 +5496,7 @@
       <c r="V15" s="108"/>
       <c r="W15" s="108"/>
       <c r="X15" s="81" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="Y15" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G15:X15)</f>
@@ -5531,73 +5505,73 @@
     </row>
     <row r="16" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16" s="100" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B16" s="101"/>
       <c r="C16" s="101"/>
       <c r="D16" s="101"/>
       <c r="E16" s="101" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F16" s="102" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G16" s="81" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H16" s="79">
         <f>SUMIF($G$2:G$2,G$2,$G16:G16)</f>
         <v>0</v>
       </c>
       <c r="I16" s="81" t="s">
+        <v>226</v>
+      </c>
+      <c r="J16" s="81" t="s">
+        <v>227</v>
+      </c>
+      <c r="K16" s="81" t="s">
+        <v>228</v>
+      </c>
+      <c r="L16" s="81" t="s">
+        <v>229</v>
+      </c>
+      <c r="M16" s="81" t="s">
+        <v>230</v>
+      </c>
+      <c r="N16" s="81" t="s">
         <v>231</v>
-      </c>
-      <c r="J16" s="81" t="s">
-        <v>232</v>
-      </c>
-      <c r="K16" s="81" t="s">
-        <v>233</v>
-      </c>
-      <c r="L16" s="81" t="s">
-        <v>234</v>
-      </c>
-      <c r="M16" s="81" t="s">
-        <v>235</v>
-      </c>
-      <c r="N16" s="81" t="s">
-        <v>236</v>
       </c>
       <c r="O16" s="79">
         <f>SUMIF($G$2:N$2,N$2,$G16:N16)</f>
         <v>0</v>
       </c>
       <c r="P16" s="81" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="Q16" s="81" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="R16" s="81" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="S16" s="79">
         <f>SUMIF($G$2:R$2,R$2,$G16:R16)</f>
         <v>0</v>
       </c>
       <c r="T16" s="81" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="U16" s="81" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="V16" s="81" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="W16" s="81" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="X16" s="81" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="Y16" s="79">
         <f>SUMIF($G$2:X$2,X$2,$G16:X16)</f>
@@ -5611,7 +5585,7 @@
       <c r="D17" s="110"/>
       <c r="E17" s="110"/>
       <c r="F17" s="112" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G17" s="79">
         <f>SUMIF($C$5:$C16,$C16,G$5:G16)</f>
@@ -5727,7 +5701,7 @@
   <sheetData>
     <row r="1" spans="1:118" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -6033,11 +6007,11 @@
   </sheetPr>
   <dimension ref="A1:FB4"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showFormulas="1" zoomScale="75" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6057,7 +6031,7 @@
   <sheetData>
     <row r="1" spans="1:158" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -6065,7 +6039,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="FA1" s="8" t="s">
         <v>0</v>
@@ -6082,10 +6056,10 @@
         <v>9</v>
       </c>
       <c r="FA2" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="FB2" s="48" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:158" x14ac:dyDescent="0.2">
@@ -6105,12 +6079,12 @@
   </sheetData>
   <autoFilter ref="A2:DT2" xr:uid="{3B89445B-6ECC-4440-B85C-E593AE209933}"/>
   <conditionalFormatting sqref="A1:EZ1 A2:FB1048576">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
       <formula>AND(OR($Q1&lt;&gt;"-",$R1&lt;&gt;0,$S1&lt;&gt;0),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FB2">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="1" stopIfTrue="1">
       <formula>AND(OR($Q2&lt;&gt;"-",$R2&lt;&gt;0,$S2&lt;&gt;0),ROW()&gt;2,$A2&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6152,7 +6126,7 @@
       <c r="A1" s="3"/>
       <c r="B1" s="5"/>
       <c r="C1" s="64" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D1" s="64"/>
       <c r="E1" s="7"/>
@@ -6207,28 +6181,28 @@
       <c r="D4" s="87"/>
       <c r="E4" s="87"/>
       <c r="F4" s="87"/>
-      <c r="G4" s="145" t="s">
+      <c r="G4" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-      <c r="J4" s="146"/>
-      <c r="K4" s="146"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="148"/>
-      <c r="N4" s="149" t="s">
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="144"/>
+      <c r="M4" s="145"/>
+      <c r="N4" s="146" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="147"/>
-      <c r="P4" s="147"/>
-      <c r="Q4" s="147"/>
-      <c r="R4" s="147"/>
-      <c r="S4" s="147"/>
-      <c r="T4" s="150"/>
-      <c r="U4" s="145" t="s">
+      <c r="O4" s="144"/>
+      <c r="P4" s="144"/>
+      <c r="Q4" s="144"/>
+      <c r="R4" s="144"/>
+      <c r="S4" s="144"/>
+      <c r="T4" s="147"/>
+      <c r="U4" s="142" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="148"/>
+      <c r="V4" s="145"/>
       <c r="W4" s="94"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -6243,7 +6217,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="93" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>14</v>
@@ -6258,13 +6232,13 @@
         <v>30</v>
       </c>
       <c r="M5" s="90" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="N5" s="12" t="s">
         <v>16</v>
       </c>
       <c r="O5" s="93" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="P5" s="12" t="s">
         <v>17</v>
@@ -6279,13 +6253,13 @@
         <v>31</v>
       </c>
       <c r="T5" s="93" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="U5" s="89" t="s">
         <v>29</v>
       </c>
       <c r="V5" s="90" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="W5" t="s">
         <v>20</v>
@@ -6297,13 +6271,13 @@
         <v>23</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="125" t="s">
-        <v>137</v>
+      <c r="F6" s="122" t="s">
+        <v>132</v>
       </c>
       <c r="G6" s="19" t="e">
         <f>SUMIFS(INDEX('ETPT Format DDG'!$A:$FA,,IFERROR(MATCH(E6,'ETPT Format DDG'!$2:$2,0),MATCH(C6,'ETPT Format DDG'!$2:$2,0))),'ETPT Format DDG'!$FB:$FB,"M-TIT",'ETPT Format DDG'!$C:$C,$A$3)</f>
@@ -6425,64 +6399,64 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="17" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:V151">
-    <cfRule type="expression" dxfId="16" priority="15">
+    <cfRule type="expression" dxfId="12" priority="15">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="15" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)-_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",OR(_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0,_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0,_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="13" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L6)&lt;&gt;_xlfn.NUMBERVALUE($L7),_xlfn.NUMBERVALUE($S6)&lt;&gt;_xlfn.NUMBERVALUE($S7),_xlfn.NUMBERVALUE($U6)&lt;&gt;_xlfn.NUMBERVALUE($U7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="12" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3)+_xlfn.NUMBERVALUE($L4)+_xlfn.NUMBERVALUE($L5)+_xlfn.NUMBERVALUE($L6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($L1)-(_xlfn.NUMBERVALUE($L2)+_xlfn.NUMBERVALUE($L3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="9" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3)+_xlfn.NUMBERVALUE($S4)+_xlfn.NUMBERVALUE($S5)+_xlfn.NUMBERVALUE($S6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($S1)-(_xlfn.NUMBERVALUE($S2)+_xlfn.NUMBERVALUE($S3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="7" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>AND($D1="8. TOTAL JUGES D'INSTRUCTION",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3)+_xlfn.NUMBERVALUE($U4)+_xlfn.NUMBERVALUE($U5)+_xlfn.NUMBERVALUE($U6))&lt;&gt;0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",_xlfn.NUMBERVALUE($U1)-(_xlfn.NUMBERVALUE($U2)+_xlfn.NUMBERVALUE($U3))&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6628,19 +6602,19 @@
   <sheetData>
     <row r="1" spans="1:13" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1"/>
       <c r="D1" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E1"/>
       <c r="G1" s="34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1"/>
       <c r="I1" s="49" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M1" s="26" t="s">
         <v>0</v>
@@ -6770,10 +6744,10 @@
   <sheetPr codeName="Feuil14">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G3"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6788,54 +6762,60 @@
     <col min="8" max="16384" width="11" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="113" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="114" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="114" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="114" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="114" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="115" t="s">
-        <v>245</v>
-      </c>
-      <c r="G1" t="s">
+    <row r="1" spans="1:8" ht="76" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="150" t="s">
+        <v>258</v>
+      </c>
+      <c r="B1" s="151" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="151" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="D1" s="151" t="s">
+        <v>261</v>
+      </c>
+      <c r="E1" s="151" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="151" t="s">
+        <v>262</v>
+      </c>
+      <c r="G1" s="151" t="s">
+        <v>263</v>
+      </c>
+      <c r="H1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="35" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="D2" s="121" t="s">
+        <v>250</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="F2" s="121" t="s">
+        <v>252</v>
+      </c>
+      <c r="G2" s="121" t="s">
+        <v>251</v>
+      </c>
+      <c r="H2" t="s">
         <v>253</v>
       </c>
-      <c r="B2" s="35" t="s">
-        <v>254</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>255</v>
-      </c>
-      <c r="D2" s="124" t="s">
-        <v>256</v>
-      </c>
-      <c r="E2" s="124" t="s">
-        <v>257</v>
-      </c>
-      <c r="F2" s="124" t="s">
-        <v>258</v>
-      </c>
-      <c r="G2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G3" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -6895,12 +6875,12 @@
   <sheetData>
     <row r="1" spans="1:62" s="4" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
@@ -6968,80 +6948,80 @@
       <c r="D2" s="45"/>
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
-      <c r="G2" s="120" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="123" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="L2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="M2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="N2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="O2" s="123" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" s="120" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="120" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="120" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="123" t="s">
-        <v>102</v>
-      </c>
-      <c r="T2" s="120" t="s">
+      <c r="G2" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="U2" s="120" t="s">
-        <v>101</v>
-      </c>
-      <c r="V2" s="120" t="s">
-        <v>101</v>
-      </c>
-      <c r="W2" s="120" t="s">
-        <v>101</v>
-      </c>
-      <c r="X2" s="120" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y2" s="123" t="s">
+      <c r="H2" s="120" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" s="120" t="s">
+      <c r="I2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AA2" s="120" t="s">
+      <c r="J2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AB2" s="120" t="s">
+      <c r="K2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AC2" s="120" t="s">
+      <c r="L2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="120" t="s">
+      <c r="M2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AE2" s="123" t="s">
+      <c r="N2" s="117" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="120" t="s">
         <v>98</v>
+      </c>
+      <c r="P2" s="117" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="117" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="117" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="120" t="s">
+        <v>97</v>
+      </c>
+      <c r="T2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="U2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="W2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="X2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="120" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE2" s="120" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:62" ht="36" x14ac:dyDescent="0.2">
@@ -7051,167 +7031,167 @@
       <c r="D3" s="45"/>
       <c r="E3" s="45"/>
       <c r="F3" s="45"/>
-      <c r="G3" s="120" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="120" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="120" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="120" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="120" t="s">
-        <v>140</v>
-      </c>
-      <c r="M3" s="120" t="s">
-        <v>141</v>
-      </c>
-      <c r="N3" s="120" t="s">
-        <v>93</v>
-      </c>
-      <c r="O3" s="123"/>
-      <c r="P3" s="120" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q3" s="120" t="s">
+      <c r="G3" s="117" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="120"/>
+      <c r="I3" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="120" t="s">
-        <v>92</v>
-      </c>
-      <c r="S3" s="123"/>
-      <c r="T3" s="120" t="s">
+      <c r="J3" s="117" t="s">
         <v>90</v>
       </c>
-      <c r="U3" s="120" t="s">
+      <c r="K3" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="V3" s="120" t="s">
-        <v>143</v>
-      </c>
-      <c r="W3" s="120" t="s">
-        <v>144</v>
-      </c>
-      <c r="X3" s="120" t="s">
+      <c r="L3" s="117" t="s">
+        <v>135</v>
+      </c>
+      <c r="M3" s="117" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="Y3" s="123"/>
-      <c r="Z3" s="120" t="s">
+      <c r="O3" s="120"/>
+      <c r="P3" s="117" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q3" s="117" t="s">
+        <v>86</v>
+      </c>
+      <c r="R3" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="AA3" s="120" t="s">
-        <v>246</v>
-      </c>
-      <c r="AB3" s="120" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC3" s="120" t="s">
+      <c r="S3" s="120"/>
+      <c r="T3" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="AD3" s="120" t="s">
+      <c r="U3" s="117" t="s">
         <v>84</v>
       </c>
-      <c r="AE3" s="123"/>
+      <c r="V3" s="117" t="s">
+        <v>138</v>
+      </c>
+      <c r="W3" s="117" t="s">
+        <v>139</v>
+      </c>
+      <c r="X3" s="117" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y3" s="120"/>
+      <c r="Z3" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA3" s="117" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB3" s="117" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC3" s="117" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD3" s="117" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE3" s="120"/>
     </row>
     <row r="4" spans="1:62" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="44"/>
       <c r="B4" s="43" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="116" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="116" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="120" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="120" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" s="120" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="120" t="s">
+      <c r="E4" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="L4" s="120" t="s">
-        <v>145</v>
-      </c>
-      <c r="M4" s="120" t="s">
-        <v>146</v>
-      </c>
-      <c r="N4" s="120" t="s">
+      <c r="F4" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="123"/>
-      <c r="P4" s="120" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q4" s="120" t="s">
+      <c r="G4" s="117" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="120"/>
+      <c r="I4" s="117" t="s">
         <v>73</v>
       </c>
-      <c r="R4" s="120" t="s">
-        <v>74</v>
-      </c>
-      <c r="S4" s="123"/>
-      <c r="T4" s="120" t="s">
+      <c r="J4" s="117" t="s">
         <v>72</v>
       </c>
-      <c r="U4" s="120" t="s">
+      <c r="K4" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="V4" s="120" t="s">
-        <v>148</v>
-      </c>
-      <c r="W4" s="120" t="s">
-        <v>149</v>
-      </c>
-      <c r="X4" s="120" t="s">
+      <c r="L4" s="117" t="s">
+        <v>140</v>
+      </c>
+      <c r="M4" s="117" t="s">
+        <v>141</v>
+      </c>
+      <c r="N4" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="Y4" s="123"/>
-      <c r="Z4" s="120" t="s">
+      <c r="O4" s="120"/>
+      <c r="P4" s="117" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q4" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="117" t="s">
         <v>69</v>
       </c>
-      <c r="AA4" s="120" t="s">
-        <v>247</v>
-      </c>
-      <c r="AB4" s="120" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC4" s="120" t="s">
+      <c r="S4" s="120"/>
+      <c r="T4" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="AD4" s="120" t="s">
+      <c r="U4" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="AE4" s="123"/>
+      <c r="V4" s="117" t="s">
+        <v>143</v>
+      </c>
+      <c r="W4" s="117" t="s">
+        <v>144</v>
+      </c>
+      <c r="X4" s="117" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y4" s="120"/>
+      <c r="Z4" s="117" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA4" s="117" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB4" s="117" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC4" s="117" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD4" s="117" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE4" s="120"/>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A5" s="42"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="47" t="s">
-        <v>252</v>
-      </c>
-      <c r="E5" s="117" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="117" t="s">
-        <v>64</v>
+        <v>246</v>
+      </c>
+      <c r="E5" s="114" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="114" t="s">
+        <v>59</v>
       </c>
       <c r="G5" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (contentieux sociaux civils et commerciaux)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") +
@@ -7295,11 +7275,11 @@
         <f>IF(ISBLANK($D$5),"",$D$5)</f>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E6" s="117" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="117" t="s">
-        <v>62</v>
+      <c r="E6" s="114" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="114" t="s">
+        <v>57</v>
       </c>
       <c r="G6" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (service pénal)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") +
@@ -7417,11 +7397,11 @@
         <f t="shared" ref="D7:D15" si="4">IF(ISBLANK($D$5),"",$D$5)</f>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E7" s="117" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="117" t="s">
-        <v>60</v>
+      <c r="E7" s="114" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="114" t="s">
+        <v>55</v>
       </c>
       <c r="G7" s="103"/>
       <c r="H7" s="79">
@@ -7475,11 +7455,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E8" s="117" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="117" t="s">
-        <v>58</v>
+      <c r="E8" s="114" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="114" t="s">
+        <v>53</v>
       </c>
       <c r="G8" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.8. ACCUEIL DU JUSTICIABLE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
@@ -7548,11 +7528,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E9" s="117" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="117" t="s">
-        <v>56</v>
+      <c r="E9" s="114" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>51</v>
       </c>
       <c r="G9" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Soutien (Hors accueil du justiciable)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
@@ -7621,11 +7601,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E10" s="117" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="117" t="s">
-        <v>54</v>
+      <c r="E10" s="114" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="114" t="s">
+        <v>49</v>
       </c>
       <c r="G10" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.3. FORMATIONS DISPENSÉES",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
@@ -7694,11 +7674,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E11" s="117" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="117" t="s">
-        <v>52</v>
+      <c r="E11" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="114" t="s">
+        <v>47</v>
       </c>
       <c r="G11" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("13.7. ACCÈS AU DROIT ET À LA JUSTICE",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
@@ -7767,11 +7747,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E12" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="117" t="s">
-        <v>50</v>
+      <c r="E12" s="114" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="114" t="s">
+        <v>45</v>
       </c>
       <c r="G12" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH") -
@@ -7846,11 +7826,11 @@
         <f>IF(ISBLANK($D$5),"",$D$5)</f>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E13" s="117" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="117" t="s">
-        <v>48</v>
+      <c r="E13" s="114" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="114" t="s">
+        <v>43</v>
       </c>
       <c r="G13" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14.9. MISE À DISPOSITION",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH")</f>
@@ -7919,11 +7899,11 @@
         <f>IF(ISBLANK($D$5),"",$D$5)</f>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E14" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="117" t="s">
-        <v>46</v>
+      <c r="E14" s="114" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="114" t="s">
+        <v>41</v>
       </c>
       <c r="G14" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD")</f>
@@ -8045,11 +8025,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR_DDG!D5</v>
       </c>
-      <c r="E15" s="117" t="s">
-        <v>224</v>
-      </c>
-      <c r="F15" s="117" t="s">
-        <v>225</v>
+      <c r="E15" s="114" t="s">
+        <v>219</v>
+      </c>
+      <c r="F15" s="114" t="s">
+        <v>220</v>
       </c>
       <c r="G15" s="103"/>
       <c r="H15" s="79">
@@ -8110,11 +8090,11 @@
     </row>
     <row r="16" spans="1:62" x14ac:dyDescent="0.2">
       <c r="D16" s="39"/>
-      <c r="E16" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="117" t="s">
-        <v>44</v>
+      <c r="E16" s="114" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="114" t="s">
+        <v>39</v>
       </c>
       <c r="G16" s="103" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("Temps ventilés sur la période (hors indisponibilité)",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
@@ -8233,9 +8213,9 @@
     </row>
     <row r="17" spans="1:31" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" s="39"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="119" t="s">
-        <v>43</v>
+      <c r="E17" s="115"/>
+      <c r="F17" s="116" t="s">
+        <v>38</v>
       </c>
       <c r="G17" s="79" t="e">
         <f>SUM(G5:G16)</f>
@@ -8340,16 +8320,16 @@
     </row>
     <row r="19" spans="1:31" customFormat="1" ht="102.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="F19" s="121" t="s">
-        <v>249</v>
+      <c r="F19" s="118" t="s">
+        <v>243</v>
       </c>
       <c r="G19" s="81" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD") +
 SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé SUB")</f>
         <v>#N/A</v>
       </c>
-      <c r="M19" s="122" t="s">
-        <v>250</v>
+      <c r="M19" s="119" t="s">
+        <v>244</v>
       </c>
       <c r="N19" s="81" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL des INDISPONIBILITÉS relevant de l'action 99",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +
@@ -8397,12 +8377,12 @@
   <sheetData>
     <row r="1" spans="1:31" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="6"/>
@@ -8439,80 +8419,80 @@
       <c r="D2" s="45"/>
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
-      <c r="G2" s="120" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="123" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="K2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="L2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="M2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="N2" s="120" t="s">
-        <v>104</v>
-      </c>
-      <c r="O2" s="123" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" s="120" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="120" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="120" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="123" t="s">
-        <v>102</v>
-      </c>
-      <c r="T2" s="120" t="s">
+      <c r="G2" s="117" t="s">
         <v>101</v>
       </c>
-      <c r="U2" s="120" t="s">
-        <v>101</v>
-      </c>
-      <c r="V2" s="120" t="s">
-        <v>101</v>
-      </c>
-      <c r="W2" s="120" t="s">
-        <v>101</v>
-      </c>
-      <c r="X2" s="120" t="s">
-        <v>101</v>
-      </c>
-      <c r="Y2" s="123" t="s">
+      <c r="H2" s="120" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" s="120" t="s">
+      <c r="I2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AA2" s="120" t="s">
+      <c r="J2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AB2" s="120" t="s">
+      <c r="K2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AC2" s="120" t="s">
+      <c r="L2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="120" t="s">
+      <c r="M2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AE2" s="123" t="s">
+      <c r="N2" s="117" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="120" t="s">
         <v>98</v>
+      </c>
+      <c r="P2" s="117" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="117" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="117" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="120" t="s">
+        <v>97</v>
+      </c>
+      <c r="T2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="U2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="V2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="W2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="X2" s="117" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="120" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AA2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD2" s="117" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE2" s="120" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:31" ht="36" x14ac:dyDescent="0.2">
@@ -8522,167 +8502,167 @@
       <c r="D3" s="45"/>
       <c r="E3" s="45"/>
       <c r="F3" s="45"/>
-      <c r="G3" s="120" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" s="123"/>
-      <c r="I3" s="120" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="120" t="s">
-        <v>95</v>
-      </c>
-      <c r="K3" s="120" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="120" t="s">
-        <v>140</v>
-      </c>
-      <c r="M3" s="120" t="s">
-        <v>141</v>
-      </c>
-      <c r="N3" s="120" t="s">
-        <v>93</v>
-      </c>
-      <c r="O3" s="123"/>
-      <c r="P3" s="120" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q3" s="120" t="s">
+      <c r="G3" s="117" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="120"/>
+      <c r="I3" s="117" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="120" t="s">
-        <v>92</v>
-      </c>
-      <c r="S3" s="123"/>
-      <c r="T3" s="120" t="s">
+      <c r="J3" s="117" t="s">
         <v>90</v>
       </c>
-      <c r="U3" s="120" t="s">
+      <c r="K3" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="V3" s="120" t="s">
-        <v>143</v>
-      </c>
-      <c r="W3" s="120" t="s">
-        <v>144</v>
-      </c>
-      <c r="X3" s="120" t="s">
+      <c r="L3" s="117" t="s">
+        <v>135</v>
+      </c>
+      <c r="M3" s="117" t="s">
+        <v>136</v>
+      </c>
+      <c r="N3" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="Y3" s="123"/>
-      <c r="Z3" s="120" t="s">
+      <c r="O3" s="120"/>
+      <c r="P3" s="117" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q3" s="117" t="s">
+        <v>86</v>
+      </c>
+      <c r="R3" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="AA3" s="120" t="s">
-        <v>246</v>
-      </c>
-      <c r="AB3" s="120" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC3" s="120" t="s">
+      <c r="S3" s="120"/>
+      <c r="T3" s="117" t="s">
         <v>85</v>
       </c>
-      <c r="AD3" s="120" t="s">
+      <c r="U3" s="117" t="s">
         <v>84</v>
       </c>
-      <c r="AE3" s="123"/>
+      <c r="V3" s="117" t="s">
+        <v>138</v>
+      </c>
+      <c r="W3" s="117" t="s">
+        <v>139</v>
+      </c>
+      <c r="X3" s="117" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y3" s="120"/>
+      <c r="Z3" s="117" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA3" s="117" t="s">
+        <v>240</v>
+      </c>
+      <c r="AB3" s="117" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC3" s="117" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD3" s="117" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE3" s="120"/>
     </row>
     <row r="4" spans="1:31" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="44"/>
       <c r="B4" s="43" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="116" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" s="116" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="120" t="s">
-        <v>79</v>
-      </c>
-      <c r="H4" s="123"/>
-      <c r="I4" s="120" t="s">
-        <v>78</v>
-      </c>
-      <c r="J4" s="120" t="s">
-        <v>77</v>
-      </c>
-      <c r="K4" s="120" t="s">
+      <c r="E4" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="L4" s="120" t="s">
-        <v>145</v>
-      </c>
-      <c r="M4" s="120" t="s">
-        <v>146</v>
-      </c>
-      <c r="N4" s="120" t="s">
+      <c r="F4" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="O4" s="123"/>
-      <c r="P4" s="120" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q4" s="120" t="s">
+      <c r="G4" s="117" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="120"/>
+      <c r="I4" s="117" t="s">
         <v>73</v>
       </c>
-      <c r="R4" s="120" t="s">
-        <v>74</v>
-      </c>
-      <c r="S4" s="123"/>
-      <c r="T4" s="120" t="s">
+      <c r="J4" s="117" t="s">
         <v>72</v>
       </c>
-      <c r="U4" s="120" t="s">
+      <c r="K4" s="117" t="s">
         <v>71</v>
       </c>
-      <c r="V4" s="120" t="s">
-        <v>148</v>
-      </c>
-      <c r="W4" s="120" t="s">
-        <v>149</v>
-      </c>
-      <c r="X4" s="120" t="s">
+      <c r="L4" s="117" t="s">
+        <v>140</v>
+      </c>
+      <c r="M4" s="117" t="s">
+        <v>141</v>
+      </c>
+      <c r="N4" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="Y4" s="123"/>
-      <c r="Z4" s="120" t="s">
+      <c r="O4" s="120"/>
+      <c r="P4" s="117" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q4" s="117" t="s">
+        <v>68</v>
+      </c>
+      <c r="R4" s="117" t="s">
         <v>69</v>
       </c>
-      <c r="AA4" s="120" t="s">
-        <v>247</v>
-      </c>
-      <c r="AB4" s="120" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC4" s="120" t="s">
+      <c r="S4" s="120"/>
+      <c r="T4" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="AD4" s="120" t="s">
+      <c r="U4" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="AE4" s="123"/>
+      <c r="V4" s="117" t="s">
+        <v>143</v>
+      </c>
+      <c r="W4" s="117" t="s">
+        <v>144</v>
+      </c>
+      <c r="X4" s="117" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y4" s="120"/>
+      <c r="Z4" s="117" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA4" s="117" t="s">
+        <v>241</v>
+      </c>
+      <c r="AB4" s="117" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC4" s="117" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD4" s="117" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE4" s="120"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="42"/>
       <c r="B5" s="41"/>
       <c r="C5" s="41"/>
       <c r="D5" s="47" t="s">
-        <v>261</v>
-      </c>
-      <c r="E5" s="117" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="117" t="s">
-        <v>64</v>
+        <v>255</v>
+      </c>
+      <c r="E5" s="114" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="114" t="s">
+        <v>59</v>
       </c>
       <c r="G5" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G5),"",IF(ETPT_CA_JUR!G5=0,"",ETPT_CA_JUR!G5)))</f>
@@ -8793,11 +8773,11 @@
         <f>IF(ISBLANK($D$5),"",$D$5)</f>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E6" s="117" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="117" t="s">
-        <v>62</v>
+      <c r="E6" s="114" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="114" t="s">
+        <v>57</v>
       </c>
       <c r="G6" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G6),"",IF(ETPT_CA_JUR!G6=0,"",ETPT_CA_JUR!G6)))</f>
@@ -8908,11 +8888,11 @@
         <f t="shared" ref="D7:D15" si="4">IF(ISBLANK($D$5),"",$D$5)</f>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E7" s="117" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="117" t="s">
-        <v>60</v>
+      <c r="E7" s="114" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="114" t="s">
+        <v>55</v>
       </c>
       <c r="G7" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G7),"",IF(ETPT_CA_JUR!G7=0,"",ETPT_CA_JUR!G7)))</f>
@@ -9023,11 +9003,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E8" s="117" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="117" t="s">
-        <v>58</v>
+      <c r="E8" s="114" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="114" t="s">
+        <v>53</v>
       </c>
       <c r="G8" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G8),"",IF(ETPT_CA_JUR!G8=0,"",ETPT_CA_JUR!G8)))</f>
@@ -9138,11 +9118,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E9" s="117" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="117" t="s">
-        <v>56</v>
+      <c r="E9" s="114" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>51</v>
       </c>
       <c r="G9" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G9),"",IF(ETPT_CA_JUR!G9=0,"",ETPT_CA_JUR!G9)))</f>
@@ -9253,11 +9233,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E10" s="117" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="117" t="s">
-        <v>54</v>
+      <c r="E10" s="114" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="114" t="s">
+        <v>49</v>
       </c>
       <c r="G10" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G10),"",IF(ETPT_CA_JUR!G10=0,"",ETPT_CA_JUR!G10)))</f>
@@ -9368,11 +9348,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E11" s="117" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="117" t="s">
-        <v>52</v>
+      <c r="E11" s="114" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="114" t="s">
+        <v>47</v>
       </c>
       <c r="G11" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G11),"",IF(ETPT_CA_JUR!G11=0,"",ETPT_CA_JUR!G11)))</f>
@@ -9483,11 +9463,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E12" s="117" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="117" t="s">
-        <v>50</v>
+      <c r="E12" s="114" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="114" t="s">
+        <v>45</v>
       </c>
       <c r="G12" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G12),"",IF(ETPT_CA_JUR!G12=0,"",ETPT_CA_JUR!G12)))</f>
@@ -9598,11 +9578,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E13" s="117" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="117" t="s">
-        <v>48</v>
+      <c r="E13" s="114" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="114" t="s">
+        <v>43</v>
       </c>
       <c r="G13" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G13),"",IF(ETPT_CA_JUR!G13=0,"",ETPT_CA_JUR!G13)))</f>
@@ -9713,11 +9693,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E14" s="117" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="117" t="s">
-        <v>46</v>
+      <c r="E14" s="114" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="114" t="s">
+        <v>41</v>
       </c>
       <c r="G14" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G14),"",IF(ETPT_CA_JUR!G14=0,"",ETPT_CA_JUR!G14)))</f>
@@ -9825,11 +9805,11 @@
         <f t="shared" si="4"/>
         <v>=ETPT_CA_JUR!D5</v>
       </c>
-      <c r="E15" s="117" t="s">
-        <v>224</v>
-      </c>
-      <c r="F15" s="117" t="s">
-        <v>225</v>
+      <c r="E15" s="114" t="s">
+        <v>219</v>
+      </c>
+      <c r="F15" s="114" t="s">
+        <v>220</v>
       </c>
       <c r="G15" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G15),"",IF(ETPT_CA_JUR!G15=0,"",ETPT_CA_JUR!G15)))</f>
@@ -9934,11 +9914,11 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="D16" s="39"/>
-      <c r="E16" s="117" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="117" t="s">
-        <v>44</v>
+      <c r="E16" s="114" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="114" t="s">
+        <v>39</v>
       </c>
       <c r="G16" s="103" t="str">
         <f>IF(ISBLANK($D$5),"",IF(ISERROR(ETPT_CA_JUR!G16),"",IF(ETPT_CA_JUR!G16=0,"",ETPT_CA_JUR!G16)))</f>
@@ -10043,9 +10023,9 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="D17" s="39"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="119" t="s">
-        <v>43</v>
+      <c r="E17" s="115"/>
+      <c r="F17" s="116" t="s">
+        <v>38</v>
       </c>
       <c r="G17" s="79">
         <f>SUM(G5:G16)</f>
@@ -10154,8 +10134,8 @@
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
-      <c r="F19" s="121" t="s">
-        <v>249</v>
+      <c r="F19" s="118" t="s">
+        <v>243</v>
       </c>
       <c r="G19" s="81" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire CTECH placé ADD") +
@@ -10167,8 +10147,8 @@
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
-      <c r="M19" s="122" t="s">
-        <v>250</v>
+      <c r="M19" s="119" t="s">
+        <v>244</v>
       </c>
       <c r="N19" s="81" t="e">
         <f>SUMIFS( INDEX( 'ETPT Format DDG'!$A:$FA,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT Format DDG'!2:2,0)),'ETPT Format DDG'!$C:$C,$D$5,'ETPT Format DDG'!$FA:$FA,"Fonctionnaire A-B-CBUR placé ADD") +

</xml_diff>

<commit_message>
Features/extractor without cache memory new (#339)
* New extractor

* update detail tab

* update rules

* add column

---------

Co-authored-by: MrJimmyChevallier <103670713+MrJimmyChevallier@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -1,36 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmychevallier/Documents/GitHub/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CF8384-ABF0-2340-89BC-06326EA5BD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C306BD-11FC-ED4D-AA95-190E88A83AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15720" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
     <sheet name="ETPT A-JUST" sheetId="1" r:id="rId2"/>
     <sheet name="ETPT Format DDG" sheetId="9" r:id="rId3"/>
-    <sheet name="Agrégats DDG" sheetId="10" r:id="rId4"/>
-    <sheet name="codage tribunal" sheetId="12" state="hidden" r:id="rId5"/>
-    <sheet name="Juridictions" sheetId="17" state="hidden" r:id="rId6"/>
-    <sheet name="Table_Fonctions" sheetId="19" state="hidden" r:id="rId7"/>
-    <sheet name="ETPT_CA_JUR" sheetId="30" state="hidden" r:id="rId8"/>
-    <sheet name="ETPT_CA_JUR_DDG" sheetId="25" r:id="rId9"/>
-    <sheet name="ETPT_ATTACHES_JUSTICE" sheetId="41" state="hidden" r:id="rId10"/>
-    <sheet name="ETPT_ATTACHES_JUSTICE_DDG" sheetId="42" r:id="rId11"/>
-    <sheet name="ETPT_CA_JUR Corresp" sheetId="38" state="hidden" r:id="rId12"/>
-    <sheet name="ETPT_ATTACHES_JUSTICE Corresp" sheetId="43" state="hidden" r:id="rId13"/>
+    <sheet name="Synthèse ETPT" sheetId="10" r:id="rId4"/>
+    <sheet name="ETPT Format DDG DETAIL" sheetId="44" state="hidden" r:id="rId5"/>
+    <sheet name="codage tribunal" sheetId="12" state="hidden" r:id="rId6"/>
+    <sheet name="Juridictions" sheetId="17" state="hidden" r:id="rId7"/>
+    <sheet name="Table_Fonctions" sheetId="19" state="hidden" r:id="rId8"/>
+    <sheet name="ETPT_CA_JUR" sheetId="30" state="hidden" r:id="rId9"/>
+    <sheet name="ETPT_CA_JUR_DDG" sheetId="25" r:id="rId10"/>
+    <sheet name="ETPT_ATTACHES_JUSTICE" sheetId="41" state="hidden" r:id="rId11"/>
+    <sheet name="ETPT_ATTACHES_JUSTICE_DDG" sheetId="42" r:id="rId12"/>
+    <sheet name="ETPT_CA_JUR Corresp" sheetId="38" state="hidden" r:id="rId13"/>
+    <sheet name="ETPT_ATTACHES_JUSTICE Corresp" sheetId="43" state="hidden" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ETPT A-JUST'!$A$2:$DN$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ETPT Format DDG'!$A$2:$DT$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Table_Fonctions!$A$1:$F$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Table_Fonctions!$A$1:$F$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="337">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -3134,13 +3135,153 @@
       </rPr>
       <t>Temps ventilé sur la période A-JUST* = figurant dans l'onglet ETPT A-JUST</t>
     </r>
+  </si>
+  <si>
+    <t>Synthèse ETPT</t>
+  </si>
+  <si>
+    <t>Réf.</t>
+  </si>
+  <si>
+    <t>Nom/Prénom/Matricule</t>
+  </si>
+  <si>
+    <t>Date d'arrivée</t>
+  </si>
+  <si>
+    <t>Date de départ</t>
+  </si>
+  <si>
+    <t>Date de début du segment</t>
+  </si>
+  <si>
+    <t>Date de fin du segment</t>
+  </si>
+  <si>
+    <t>Nombre jour ouvré sur période total extaction</t>
+  </si>
+  <si>
+    <t>Nombre jour ouvré segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio Jour : 
+Nb jour ouvré segment /
+Nb jour ouvré total </t>
+  </si>
+  <si>
+    <t>Temps de travail en ETPT saisie</t>
+  </si>
+  <si>
+    <t>Valeur de l'ETPT sur période total d'extraction (ETPT saisi x Ratio Jour)</t>
+  </si>
+  <si>
+    <t>Indisponibilité saisie</t>
+  </si>
+  <si>
+    <t>Valeur de l'indisponibilité sur la période total d'extraction (Indisponibilité saisie en%/100 x Ratio Jour)</t>
+  </si>
+  <si>
+    <t>Nb jour ouvré CET sur toute la période d'extraction</t>
+  </si>
+  <si>
+    <t>Valeur de l'absentéisme</t>
+  </si>
+  <si>
+    <t>Valeur de l'action 99</t>
+  </si>
+  <si>
+    <t>ETPT effectif sur la période total (ETPT- action 99 + absentéisme) x Ratio Jour</t>
+  </si>
+  <si>
+    <t>#! FOR_EACH log ongletLogs</t>
+  </si>
+  <si>
+    <t>## log.id</t>
+  </si>
+  <si>
+    <t>## log.name</t>
+  </si>
+  <si>
+    <t>## log.category</t>
+  </si>
+  <si>
+    <t>## log.humanStart</t>
+  </si>
+  <si>
+    <t>## log.humanEnd</t>
+  </si>
+  <si>
+    <t>## log.main</t>
+  </si>
+  <si>
+    <t>## log.periodStart</t>
+  </si>
+  <si>
+    <t>## log.periodEnd</t>
+  </si>
+  <si>
+    <t>## log.nbOfWorkingDaysQuery</t>
+  </si>
+  <si>
+    <t>## log.workingDays</t>
+  </si>
+  <si>
+    <t>## log.dayRate</t>
+  </si>
+  <si>
+    <t>## log.filledEtp</t>
+  </si>
+  <si>
+    <t>## log.queryEtpValue</t>
+  </si>
+  <si>
+    <t>## log.totalIndispo</t>
+  </si>
+  <si>
+    <t>## log.queryIndispoValue</t>
+  </si>
+  <si>
+    <t>## log.cetDays</t>
+  </si>
+  <si>
+    <t>## log.abs</t>
+  </si>
+  <si>
+    <t>## log.action99</t>
+  </si>
+  <si>
+    <t>## log.effectifEtp</t>
+  </si>
+  <si>
+    <t>## log.logAccVentilation</t>
+  </si>
+  <si>
+    <t>## log.ctx</t>
+  </si>
+  <si>
+    <t>#! END_LOOP log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Détails de la ventilation (arrondi au millième) :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Synthèse ETPT</t>
+  </si>
+  <si>
+    <t>ETPT global sur la période (incluant absentéisme et action 99)</t>
+  </si>
+  <si>
+    <t>## log.etptGlobal</t>
+  </si>
+  <si>
+    <t>ETPT ventilé</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -3148,6 +3289,7 @@
     <numFmt numFmtId="168" formatCode="0.###;0.###;\-"/>
     <numFmt numFmtId="169" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="171" formatCode="0.###"/>
   </numFmts>
   <fonts count="57" x14ac:knownFonts="1">
     <font>
@@ -3546,7 +3688,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3658,6 +3800,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF7F02D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCB1EE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4018,7 +4178,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4503,6 +4663,39 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -4603,7 +4796,87 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{6FC886D6-2077-B34D-B1DF-739B068A66D1}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6BD57324-3FD5-D341-A299-730D14794802}"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="23">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCB1EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9948118533890809E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5583,7 +5856,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+      <selection activeCell="A13" sqref="A13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5603,11 +5876,11 @@
       <c r="B1" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="169" t="s">
+      <c r="C1" s="180" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
       <c r="F1" s="49"/>
       <c r="H1" s="26" t="s">
         <v>0</v>
@@ -5616,11 +5889,11 @@
     <row r="2" spans="1:8" s="53" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="50"/>
       <c r="B2" s="51"/>
-      <c r="C2" s="170" t="s">
+      <c r="C2" s="181" t="s">
         <v>106</v>
       </c>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
       <c r="F2" s="52"/>
       <c r="H2" s="26" t="s">
         <v>0</v>
@@ -5644,10 +5917,10 @@
       <c r="D4" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="174" t="s">
+      <c r="E4" s="185" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="175"/>
+      <c r="F4" s="186"/>
       <c r="G4" s="65"/>
       <c r="H4" s="26" t="s">
         <v>0</v>
@@ -5664,10 +5937,10 @@
       <c r="D5" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="176" t="s">
+      <c r="E5" s="187" t="s">
         <v>100</v>
       </c>
-      <c r="F5" s="177"/>
+      <c r="F5" s="188"/>
       <c r="G5" s="64"/>
       <c r="H5" s="26" t="s">
         <v>0</v>
@@ -5684,10 +5957,10 @@
       <c r="D6" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="178" t="s">
+      <c r="E6" s="189" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="179"/>
+      <c r="F6" s="190"/>
       <c r="G6" s="64"/>
       <c r="H6" s="26" t="s">
         <v>0</v>
@@ -5696,7 +5969,7 @@
     <row r="7" spans="1:8" s="26" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="54"/>
       <c r="B7" s="164" t="s">
-        <v>96</v>
+        <v>291</v>
       </c>
       <c r="C7" s="63" t="s">
         <v>283</v>
@@ -5704,10 +5977,10 @@
       <c r="D7" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="178" t="s">
+      <c r="E7" s="189" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="179"/>
+      <c r="F7" s="190"/>
       <c r="G7" s="64"/>
       <c r="H7" s="26" t="s">
         <v>0</v>
@@ -5718,16 +5991,16 @@
       <c r="B8" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="C8" s="167" t="s">
+      <c r="C8" s="178" t="s">
         <v>254</v>
       </c>
-      <c r="D8" s="167" t="s">
+      <c r="D8" s="178" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="180" t="s">
+      <c r="E8" s="191" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="181"/>
+      <c r="F8" s="192"/>
       <c r="G8" s="64"/>
       <c r="H8" s="26" t="s">
         <v>0</v>
@@ -5738,10 +6011,10 @@
       <c r="B9" s="165" t="s">
         <v>253</v>
       </c>
-      <c r="C9" s="168"/>
-      <c r="D9" s="168"/>
-      <c r="E9" s="168"/>
-      <c r="F9" s="168"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
       <c r="G9" s="64"/>
       <c r="H9" s="26" t="s">
         <v>0</v>
@@ -5761,11 +6034,11 @@
     <row r="11" spans="1:8" s="26" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="54"/>
       <c r="B11" s="66"/>
-      <c r="C11" s="173" t="s">
+      <c r="C11" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="173"/>
-      <c r="E11" s="173"/>
+      <c r="D11" s="184"/>
+      <c r="E11" s="184"/>
       <c r="F11" s="67"/>
       <c r="H11" s="26" t="s">
         <v>0</v>
@@ -5779,14 +6052,14 @@
       </c>
     </row>
     <row r="13" spans="1:8" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="171" t="s">
+      <c r="A13" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="171"/>
-      <c r="C13" s="171"/>
-      <c r="D13" s="171"/>
-      <c r="E13" s="171"/>
-      <c r="F13" s="172"/>
+      <c r="B13" s="182"/>
+      <c r="C13" s="182"/>
+      <c r="D13" s="182"/>
+      <c r="E13" s="182"/>
+      <c r="F13" s="183"/>
       <c r="H13" s="26" t="s">
         <v>0</v>
       </c>
@@ -5817,6 +6090,1496 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701921C7-025B-4F4F-A5C7-6D94075AC520}">
+  <sheetPr codeName="Feuil8">
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:AA17"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6" style="37" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="37" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" style="37" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="37" customWidth="1"/>
+    <col min="5" max="5" width="6.5" style="37" customWidth="1"/>
+    <col min="6" max="6" width="50" style="37" customWidth="1"/>
+    <col min="7" max="27" width="14" style="37" customWidth="1"/>
+    <col min="28" max="34" width="9.33203125" style="37" customWidth="1"/>
+    <col min="35" max="35" width="8.5" style="37" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.33203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14" style="37" customWidth="1"/>
+    <col min="38" max="58" width="9.33203125" style="37" customWidth="1"/>
+    <col min="59" max="59" width="4" style="37" customWidth="1"/>
+    <col min="60" max="16384" width="11" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+    </row>
+    <row r="2" spans="1:27" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2" s="44"/>
+      <c r="B2" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="95" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="99" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="100" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" s="99" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="99" t="s">
+        <v>273</v>
+      </c>
+      <c r="K2" s="99" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="99" t="s">
+        <v>274</v>
+      </c>
+      <c r="M2" s="99" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" s="100" t="s">
+        <v>80</v>
+      </c>
+      <c r="P2" s="99" t="s">
+        <v>275</v>
+      </c>
+      <c r="Q2" s="99" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="99" t="s">
+        <v>276</v>
+      </c>
+      <c r="S2" s="99" t="s">
+        <v>112</v>
+      </c>
+      <c r="T2" s="99" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="100" t="s">
+        <v>79</v>
+      </c>
+      <c r="V2" s="99" t="s">
+        <v>63</v>
+      </c>
+      <c r="W2" s="99" t="s">
+        <v>284</v>
+      </c>
+      <c r="X2" s="99" t="s">
+        <v>285</v>
+      </c>
+      <c r="Y2" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z2" s="99" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" s="100" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" s="42"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="150" t="s">
+        <v>266</v>
+      </c>
+      <c r="E3" s="96" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="96" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G3),"",IF(ETPT_CA_JUR!G3=0,"",ETPT_CA_JUR!G3)))</f>
+        <v/>
+      </c>
+      <c r="H3" s="137">
+        <f>ETPT_CA_JUR!H3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I3),"",IF(ETPT_CA_JUR!I3=0,"",ETPT_CA_JUR!I3)))</f>
+        <v/>
+      </c>
+      <c r="J3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J3),"",IF(ETPT_CA_JUR!J3=0,"",ETPT_CA_JUR!J3)))</f>
+        <v/>
+      </c>
+      <c r="K3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K3),"",IF(ETPT_CA_JUR!K3=0,"",ETPT_CA_JUR!K3)))</f>
+        <v/>
+      </c>
+      <c r="L3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L3),"",IF(ETPT_CA_JUR!L3=0,"",ETPT_CA_JUR!L3)))</f>
+        <v/>
+      </c>
+      <c r="M3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M3),"",IF(ETPT_CA_JUR!M3=0,"",ETPT_CA_JUR!M3)))</f>
+        <v/>
+      </c>
+      <c r="N3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N3),"",IF(ETPT_CA_JUR!N3=0,"",ETPT_CA_JUR!N3)))</f>
+        <v/>
+      </c>
+      <c r="O3" s="137">
+        <f>ETPT_CA_JUR!O3</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P3),"",IF(ETPT_CA_JUR!P3=0,"",ETPT_CA_JUR!P3)))</f>
+        <v/>
+      </c>
+      <c r="Q3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q3),"",IF(ETPT_CA_JUR!Q3=0,"",ETPT_CA_JUR!Q3)))</f>
+        <v/>
+      </c>
+      <c r="R3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R3),"",IF(ETPT_CA_JUR!R3=0,"",ETPT_CA_JUR!R3)))</f>
+        <v/>
+      </c>
+      <c r="S3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S3),"",IF(ETPT_CA_JUR!S3=0,"",ETPT_CA_JUR!S3)))</f>
+        <v/>
+      </c>
+      <c r="T3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T3),"",IF(ETPT_CA_JUR!T3=0,"",ETPT_CA_JUR!T3)))</f>
+        <v/>
+      </c>
+      <c r="U3" s="137">
+        <f>ETPT_CA_JUR!U3</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V3),"",IF(ETPT_CA_JUR!V3=0,"",ETPT_CA_JUR!V3)))</f>
+        <v/>
+      </c>
+      <c r="W3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W3),"",IF(ETPT_CA_JUR!W3=0,"",ETPT_CA_JUR!W3)))</f>
+        <v/>
+      </c>
+      <c r="X3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X3),"",IF(ETPT_CA_JUR!X3=0,"",ETPT_CA_JUR!X3)))</f>
+        <v/>
+      </c>
+      <c r="Y3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y3),"",IF(ETPT_CA_JUR!Y3=0,"",ETPT_CA_JUR!Y3)))</f>
+        <v/>
+      </c>
+      <c r="Z3" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z3),"",IF(ETPT_CA_JUR!Z3=0,"",ETPT_CA_JUR!Z3)))</f>
+        <v/>
+      </c>
+      <c r="AA3" s="137">
+        <f>ETPT_CA_JUR!AA3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" s="42"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="38" t="str">
+        <f>IF(ISBLANK($D$3),"",$D$3)</f>
+        <v>A</v>
+      </c>
+      <c r="E4" s="96" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="96" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G4),"",IF(ETPT_CA_JUR!G4=0,"",ETPT_CA_JUR!G4)))</f>
+        <v/>
+      </c>
+      <c r="H4" s="137">
+        <f>ETPT_CA_JUR!H4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I4),"",IF(ETPT_CA_JUR!I4=0,"",ETPT_CA_JUR!I4)))</f>
+        <v/>
+      </c>
+      <c r="J4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J4),"",IF(ETPT_CA_JUR!J4=0,"",ETPT_CA_JUR!J4)))</f>
+        <v/>
+      </c>
+      <c r="K4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K4),"",IF(ETPT_CA_JUR!K4=0,"",ETPT_CA_JUR!K4)))</f>
+        <v/>
+      </c>
+      <c r="L4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L4),"",IF(ETPT_CA_JUR!L4=0,"",ETPT_CA_JUR!L4)))</f>
+        <v/>
+      </c>
+      <c r="M4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M4),"",IF(ETPT_CA_JUR!M4=0,"",ETPT_CA_JUR!M4)))</f>
+        <v/>
+      </c>
+      <c r="N4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N4),"",IF(ETPT_CA_JUR!N4=0,"",ETPT_CA_JUR!N4)))</f>
+        <v/>
+      </c>
+      <c r="O4" s="137">
+        <f>ETPT_CA_JUR!O4</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P4),"",IF(ETPT_CA_JUR!P4=0,"",ETPT_CA_JUR!P4)))</f>
+        <v/>
+      </c>
+      <c r="Q4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q4),"",IF(ETPT_CA_JUR!Q4=0,"",ETPT_CA_JUR!Q4)))</f>
+        <v/>
+      </c>
+      <c r="R4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R4),"",IF(ETPT_CA_JUR!R4=0,"",ETPT_CA_JUR!R4)))</f>
+        <v/>
+      </c>
+      <c r="S4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S4),"",IF(ETPT_CA_JUR!S4=0,"",ETPT_CA_JUR!S4)))</f>
+        <v/>
+      </c>
+      <c r="T4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T4),"",IF(ETPT_CA_JUR!T4=0,"",ETPT_CA_JUR!T4)))</f>
+        <v/>
+      </c>
+      <c r="U4" s="137">
+        <f>ETPT_CA_JUR!U4</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V4),"",IF(ETPT_CA_JUR!V4=0,"",ETPT_CA_JUR!V4)))</f>
+        <v/>
+      </c>
+      <c r="W4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W4),"",IF(ETPT_CA_JUR!W4=0,"",ETPT_CA_JUR!W4)))</f>
+        <v/>
+      </c>
+      <c r="X4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X4),"",IF(ETPT_CA_JUR!X4=0,"",ETPT_CA_JUR!X4)))</f>
+        <v/>
+      </c>
+      <c r="Y4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y4),"",IF(ETPT_CA_JUR!Y4=0,"",ETPT_CA_JUR!Y4)))</f>
+        <v/>
+      </c>
+      <c r="Z4" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z4),"",IF(ETPT_CA_JUR!Z4=0,"",ETPT_CA_JUR!Z4)))</f>
+        <v/>
+      </c>
+      <c r="AA4" s="137">
+        <f>ETPT_CA_JUR!AA4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="42"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="38" t="str">
+        <f t="shared" ref="D5:D13" si="0">IF(ISBLANK($D$3),"",$D$3)</f>
+        <v>A</v>
+      </c>
+      <c r="E5" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="96" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G5),"",IF(ETPT_CA_JUR!G5=0,"",ETPT_CA_JUR!G5)))</f>
+        <v/>
+      </c>
+      <c r="H5" s="137">
+        <f>ETPT_CA_JUR!H5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I5),"",IF(ETPT_CA_JUR!I5=0,"",ETPT_CA_JUR!I5)))</f>
+        <v/>
+      </c>
+      <c r="J5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J5),"",IF(ETPT_CA_JUR!J5=0,"",ETPT_CA_JUR!J5)))</f>
+        <v/>
+      </c>
+      <c r="K5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K5),"",IF(ETPT_CA_JUR!K5=0,"",ETPT_CA_JUR!K5)))</f>
+        <v/>
+      </c>
+      <c r="L5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L5),"",IF(ETPT_CA_JUR!L5=0,"",ETPT_CA_JUR!L5)))</f>
+        <v/>
+      </c>
+      <c r="M5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M5),"",IF(ETPT_CA_JUR!M5=0,"",ETPT_CA_JUR!M5)))</f>
+        <v/>
+      </c>
+      <c r="N5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N5),"",IF(ETPT_CA_JUR!N5=0,"",ETPT_CA_JUR!N5)))</f>
+        <v/>
+      </c>
+      <c r="O5" s="137">
+        <f>ETPT_CA_JUR!O5</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P5),"",IF(ETPT_CA_JUR!P5=0,"",ETPT_CA_JUR!P5)))</f>
+        <v/>
+      </c>
+      <c r="Q5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q5),"",IF(ETPT_CA_JUR!Q5=0,"",ETPT_CA_JUR!Q5)))</f>
+        <v/>
+      </c>
+      <c r="R5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R5),"",IF(ETPT_CA_JUR!R5=0,"",ETPT_CA_JUR!R5)))</f>
+        <v/>
+      </c>
+      <c r="S5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S5),"",IF(ETPT_CA_JUR!S5=0,"",ETPT_CA_JUR!S5)))</f>
+        <v/>
+      </c>
+      <c r="T5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T5),"",IF(ETPT_CA_JUR!T5=0,"",ETPT_CA_JUR!T5)))</f>
+        <v/>
+      </c>
+      <c r="U5" s="137">
+        <f>ETPT_CA_JUR!U5</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V5),"",IF(ETPT_CA_JUR!V5=0,"",ETPT_CA_JUR!V5)))</f>
+        <v/>
+      </c>
+      <c r="W5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W5),"",IF(ETPT_CA_JUR!W5=0,"",ETPT_CA_JUR!W5)))</f>
+        <v/>
+      </c>
+      <c r="X5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X5),"",IF(ETPT_CA_JUR!X5=0,"",ETPT_CA_JUR!X5)))</f>
+        <v/>
+      </c>
+      <c r="Y5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y5),"",IF(ETPT_CA_JUR!Y5=0,"",ETPT_CA_JUR!Y5)))</f>
+        <v/>
+      </c>
+      <c r="Z5" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z5),"",IF(ETPT_CA_JUR!Z5=0,"",ETPT_CA_JUR!Z5)))</f>
+        <v/>
+      </c>
+      <c r="AA5" s="137">
+        <f>ETPT_CA_JUR!AA5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" s="42"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E6" s="96" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G6),"",IF(ETPT_CA_JUR!G6=0,"",ETPT_CA_JUR!G6)))</f>
+        <v/>
+      </c>
+      <c r="H6" s="137">
+        <f>ETPT_CA_JUR!H6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I6),"",IF(ETPT_CA_JUR!I6=0,"",ETPT_CA_JUR!I6)))</f>
+        <v/>
+      </c>
+      <c r="J6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J6),"",IF(ETPT_CA_JUR!J6=0,"",ETPT_CA_JUR!J6)))</f>
+        <v/>
+      </c>
+      <c r="K6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K6),"",IF(ETPT_CA_JUR!K6=0,"",ETPT_CA_JUR!K6)))</f>
+        <v/>
+      </c>
+      <c r="L6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L6),"",IF(ETPT_CA_JUR!L6=0,"",ETPT_CA_JUR!L6)))</f>
+        <v/>
+      </c>
+      <c r="M6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M6),"",IF(ETPT_CA_JUR!M6=0,"",ETPT_CA_JUR!M6)))</f>
+        <v/>
+      </c>
+      <c r="N6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N6),"",IF(ETPT_CA_JUR!N6=0,"",ETPT_CA_JUR!N6)))</f>
+        <v/>
+      </c>
+      <c r="O6" s="137">
+        <f>ETPT_CA_JUR!O6</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P6),"",IF(ETPT_CA_JUR!P6=0,"",ETPT_CA_JUR!P6)))</f>
+        <v/>
+      </c>
+      <c r="Q6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q6),"",IF(ETPT_CA_JUR!Q6=0,"",ETPT_CA_JUR!Q6)))</f>
+        <v/>
+      </c>
+      <c r="R6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R6),"",IF(ETPT_CA_JUR!R6=0,"",ETPT_CA_JUR!R6)))</f>
+        <v/>
+      </c>
+      <c r="S6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S6),"",IF(ETPT_CA_JUR!S6=0,"",ETPT_CA_JUR!S6)))</f>
+        <v/>
+      </c>
+      <c r="T6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T6),"",IF(ETPT_CA_JUR!T6=0,"",ETPT_CA_JUR!T6)))</f>
+        <v/>
+      </c>
+      <c r="U6" s="137">
+        <f>ETPT_CA_JUR!U6</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V6),"",IF(ETPT_CA_JUR!V6=0,"",ETPT_CA_JUR!V6)))</f>
+        <v/>
+      </c>
+      <c r="W6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W6),"",IF(ETPT_CA_JUR!W6=0,"",ETPT_CA_JUR!W6)))</f>
+        <v/>
+      </c>
+      <c r="X6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X6),"",IF(ETPT_CA_JUR!X6=0,"",ETPT_CA_JUR!X6)))</f>
+        <v/>
+      </c>
+      <c r="Y6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y6),"",IF(ETPT_CA_JUR!Y6=0,"",ETPT_CA_JUR!Y6)))</f>
+        <v/>
+      </c>
+      <c r="Z6" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z6),"",IF(ETPT_CA_JUR!Z6=0,"",ETPT_CA_JUR!Z6)))</f>
+        <v/>
+      </c>
+      <c r="AA6" s="137">
+        <f>ETPT_CA_JUR!AA6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="42"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E7" s="96" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G7),"",IF(ETPT_CA_JUR!G7=0,"",ETPT_CA_JUR!G7)))</f>
+        <v/>
+      </c>
+      <c r="H7" s="137">
+        <f>ETPT_CA_JUR!H7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I7),"",IF(ETPT_CA_JUR!I7=0,"",ETPT_CA_JUR!I7)))</f>
+        <v/>
+      </c>
+      <c r="J7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J7),"",IF(ETPT_CA_JUR!J7=0,"",ETPT_CA_JUR!J7)))</f>
+        <v/>
+      </c>
+      <c r="K7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K7),"",IF(ETPT_CA_JUR!K7=0,"",ETPT_CA_JUR!K7)))</f>
+        <v/>
+      </c>
+      <c r="L7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L7),"",IF(ETPT_CA_JUR!L7=0,"",ETPT_CA_JUR!L7)))</f>
+        <v/>
+      </c>
+      <c r="M7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M7),"",IF(ETPT_CA_JUR!M7=0,"",ETPT_CA_JUR!M7)))</f>
+        <v/>
+      </c>
+      <c r="N7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N7),"",IF(ETPT_CA_JUR!N7=0,"",ETPT_CA_JUR!N7)))</f>
+        <v/>
+      </c>
+      <c r="O7" s="137">
+        <f>ETPT_CA_JUR!O7</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P7),"",IF(ETPT_CA_JUR!P7=0,"",ETPT_CA_JUR!P7)))</f>
+        <v/>
+      </c>
+      <c r="Q7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q7),"",IF(ETPT_CA_JUR!Q7=0,"",ETPT_CA_JUR!Q7)))</f>
+        <v/>
+      </c>
+      <c r="R7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R7),"",IF(ETPT_CA_JUR!R7=0,"",ETPT_CA_JUR!R7)))</f>
+        <v/>
+      </c>
+      <c r="S7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S7),"",IF(ETPT_CA_JUR!S7=0,"",ETPT_CA_JUR!S7)))</f>
+        <v/>
+      </c>
+      <c r="T7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T7),"",IF(ETPT_CA_JUR!T7=0,"",ETPT_CA_JUR!T7)))</f>
+        <v/>
+      </c>
+      <c r="U7" s="137">
+        <f>ETPT_CA_JUR!U7</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V7),"",IF(ETPT_CA_JUR!V7=0,"",ETPT_CA_JUR!V7)))</f>
+        <v/>
+      </c>
+      <c r="W7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W7),"",IF(ETPT_CA_JUR!W7=0,"",ETPT_CA_JUR!W7)))</f>
+        <v/>
+      </c>
+      <c r="X7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X7),"",IF(ETPT_CA_JUR!X7=0,"",ETPT_CA_JUR!X7)))</f>
+        <v/>
+      </c>
+      <c r="Y7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y7),"",IF(ETPT_CA_JUR!Y7=0,"",ETPT_CA_JUR!Y7)))</f>
+        <v/>
+      </c>
+      <c r="Z7" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z7),"",IF(ETPT_CA_JUR!Z7=0,"",ETPT_CA_JUR!Z7)))</f>
+        <v/>
+      </c>
+      <c r="AA7" s="137">
+        <f>ETPT_CA_JUR!AA7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" s="42"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E8" s="96" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="96" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G8),"",IF(ETPT_CA_JUR!G8=0,"",ETPT_CA_JUR!G8)))</f>
+        <v/>
+      </c>
+      <c r="H8" s="137">
+        <f>ETPT_CA_JUR!H8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I8),"",IF(ETPT_CA_JUR!I8=0,"",ETPT_CA_JUR!I8)))</f>
+        <v/>
+      </c>
+      <c r="J8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J8),"",IF(ETPT_CA_JUR!J8=0,"",ETPT_CA_JUR!J8)))</f>
+        <v/>
+      </c>
+      <c r="K8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K8),"",IF(ETPT_CA_JUR!K8=0,"",ETPT_CA_JUR!K8)))</f>
+        <v/>
+      </c>
+      <c r="L8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L8),"",IF(ETPT_CA_JUR!L8=0,"",ETPT_CA_JUR!L8)))</f>
+        <v/>
+      </c>
+      <c r="M8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M8),"",IF(ETPT_CA_JUR!M8=0,"",ETPT_CA_JUR!M8)))</f>
+        <v/>
+      </c>
+      <c r="N8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N8),"",IF(ETPT_CA_JUR!N8=0,"",ETPT_CA_JUR!N8)))</f>
+        <v/>
+      </c>
+      <c r="O8" s="137">
+        <f>ETPT_CA_JUR!O8</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P8),"",IF(ETPT_CA_JUR!P8=0,"",ETPT_CA_JUR!P8)))</f>
+        <v/>
+      </c>
+      <c r="Q8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q8),"",IF(ETPT_CA_JUR!Q8=0,"",ETPT_CA_JUR!Q8)))</f>
+        <v/>
+      </c>
+      <c r="R8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R8),"",IF(ETPT_CA_JUR!R8=0,"",ETPT_CA_JUR!R8)))</f>
+        <v/>
+      </c>
+      <c r="S8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S8),"",IF(ETPT_CA_JUR!S8=0,"",ETPT_CA_JUR!S8)))</f>
+        <v/>
+      </c>
+      <c r="T8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T8),"",IF(ETPT_CA_JUR!T8=0,"",ETPT_CA_JUR!T8)))</f>
+        <v/>
+      </c>
+      <c r="U8" s="137">
+        <f>ETPT_CA_JUR!U8</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V8),"",IF(ETPT_CA_JUR!V8=0,"",ETPT_CA_JUR!V8)))</f>
+        <v/>
+      </c>
+      <c r="W8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W8),"",IF(ETPT_CA_JUR!W8=0,"",ETPT_CA_JUR!W8)))</f>
+        <v/>
+      </c>
+      <c r="X8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X8),"",IF(ETPT_CA_JUR!X8=0,"",ETPT_CA_JUR!X8)))</f>
+        <v/>
+      </c>
+      <c r="Y8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y8),"",IF(ETPT_CA_JUR!Y8=0,"",ETPT_CA_JUR!Y8)))</f>
+        <v/>
+      </c>
+      <c r="Z8" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z8),"",IF(ETPT_CA_JUR!Z8=0,"",ETPT_CA_JUR!Z8)))</f>
+        <v/>
+      </c>
+      <c r="AA8" s="137">
+        <f>ETPT_CA_JUR!AA8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" s="42"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E9" s="96" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="96" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G9),"",IF(ETPT_CA_JUR!G9=0,"",ETPT_CA_JUR!G9)))</f>
+        <v/>
+      </c>
+      <c r="H9" s="137">
+        <f>ETPT_CA_JUR!H9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I9),"",IF(ETPT_CA_JUR!I9=0,"",ETPT_CA_JUR!I9)))</f>
+        <v/>
+      </c>
+      <c r="J9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J9),"",IF(ETPT_CA_JUR!J9=0,"",ETPT_CA_JUR!J9)))</f>
+        <v/>
+      </c>
+      <c r="K9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K9),"",IF(ETPT_CA_JUR!K9=0,"",ETPT_CA_JUR!K9)))</f>
+        <v/>
+      </c>
+      <c r="L9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L9),"",IF(ETPT_CA_JUR!L9=0,"",ETPT_CA_JUR!L9)))</f>
+        <v/>
+      </c>
+      <c r="M9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M9),"",IF(ETPT_CA_JUR!M9=0,"",ETPT_CA_JUR!M9)))</f>
+        <v/>
+      </c>
+      <c r="N9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N9),"",IF(ETPT_CA_JUR!N9=0,"",ETPT_CA_JUR!N9)))</f>
+        <v/>
+      </c>
+      <c r="O9" s="137">
+        <f>ETPT_CA_JUR!O9</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P9),"",IF(ETPT_CA_JUR!P9=0,"",ETPT_CA_JUR!P9)))</f>
+        <v/>
+      </c>
+      <c r="Q9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q9),"",IF(ETPT_CA_JUR!Q9=0,"",ETPT_CA_JUR!Q9)))</f>
+        <v/>
+      </c>
+      <c r="R9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R9),"",IF(ETPT_CA_JUR!R9=0,"",ETPT_CA_JUR!R9)))</f>
+        <v/>
+      </c>
+      <c r="S9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S9),"",IF(ETPT_CA_JUR!S9=0,"",ETPT_CA_JUR!S9)))</f>
+        <v/>
+      </c>
+      <c r="T9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T9),"",IF(ETPT_CA_JUR!T9=0,"",ETPT_CA_JUR!T9)))</f>
+        <v/>
+      </c>
+      <c r="U9" s="137">
+        <f>ETPT_CA_JUR!U9</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V9),"",IF(ETPT_CA_JUR!V9=0,"",ETPT_CA_JUR!V9)))</f>
+        <v/>
+      </c>
+      <c r="W9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W9),"",IF(ETPT_CA_JUR!W9=0,"",ETPT_CA_JUR!W9)))</f>
+        <v/>
+      </c>
+      <c r="X9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X9),"",IF(ETPT_CA_JUR!X9=0,"",ETPT_CA_JUR!X9)))</f>
+        <v/>
+      </c>
+      <c r="Y9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y9),"",IF(ETPT_CA_JUR!Y9=0,"",ETPT_CA_JUR!Y9)))</f>
+        <v/>
+      </c>
+      <c r="Z9" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z9),"",IF(ETPT_CA_JUR!Z9=0,"",ETPT_CA_JUR!Z9)))</f>
+        <v/>
+      </c>
+      <c r="AA9" s="137">
+        <f>ETPT_CA_JUR!AA9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" s="42"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E10" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="96" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G10),"",IF(ETPT_CA_JUR!G10=0,"",ETPT_CA_JUR!G10)))</f>
+        <v/>
+      </c>
+      <c r="H10" s="137">
+        <f>ETPT_CA_JUR!H10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I10),"",IF(ETPT_CA_JUR!I10=0,"",ETPT_CA_JUR!I10)))</f>
+        <v/>
+      </c>
+      <c r="J10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J10),"",IF(ETPT_CA_JUR!J10=0,"",ETPT_CA_JUR!J10)))</f>
+        <v/>
+      </c>
+      <c r="K10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K10),"",IF(ETPT_CA_JUR!K10=0,"",ETPT_CA_JUR!K10)))</f>
+        <v/>
+      </c>
+      <c r="L10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L10),"",IF(ETPT_CA_JUR!L10=0,"",ETPT_CA_JUR!L10)))</f>
+        <v/>
+      </c>
+      <c r="M10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M10),"",IF(ETPT_CA_JUR!M10=0,"",ETPT_CA_JUR!M10)))</f>
+        <v/>
+      </c>
+      <c r="N10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N10),"",IF(ETPT_CA_JUR!N10=0,"",ETPT_CA_JUR!N10)))</f>
+        <v/>
+      </c>
+      <c r="O10" s="137">
+        <f>ETPT_CA_JUR!O10</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P10),"",IF(ETPT_CA_JUR!P10=0,"",ETPT_CA_JUR!P10)))</f>
+        <v/>
+      </c>
+      <c r="Q10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q10),"",IF(ETPT_CA_JUR!Q10=0,"",ETPT_CA_JUR!Q10)))</f>
+        <v/>
+      </c>
+      <c r="R10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R10),"",IF(ETPT_CA_JUR!R10=0,"",ETPT_CA_JUR!R10)))</f>
+        <v/>
+      </c>
+      <c r="S10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S10),"",IF(ETPT_CA_JUR!S10=0,"",ETPT_CA_JUR!S10)))</f>
+        <v/>
+      </c>
+      <c r="T10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T10),"",IF(ETPT_CA_JUR!T10=0,"",ETPT_CA_JUR!T10)))</f>
+        <v/>
+      </c>
+      <c r="U10" s="137">
+        <f>ETPT_CA_JUR!U10</f>
+        <v>0</v>
+      </c>
+      <c r="V10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V10),"",IF(ETPT_CA_JUR!V10=0,"",ETPT_CA_JUR!V10)))</f>
+        <v/>
+      </c>
+      <c r="W10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W10),"",IF(ETPT_CA_JUR!W10=0,"",ETPT_CA_JUR!W10)))</f>
+        <v/>
+      </c>
+      <c r="X10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X10),"",IF(ETPT_CA_JUR!X10=0,"",ETPT_CA_JUR!X10)))</f>
+        <v/>
+      </c>
+      <c r="Y10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y10),"",IF(ETPT_CA_JUR!Y10=0,"",ETPT_CA_JUR!Y10)))</f>
+        <v/>
+      </c>
+      <c r="Z10" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z10),"",IF(ETPT_CA_JUR!Z10=0,"",ETPT_CA_JUR!Z10)))</f>
+        <v/>
+      </c>
+      <c r="AA10" s="137">
+        <f>ETPT_CA_JUR!AA10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="42"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E11" s="96" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="96" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G11),"",IF(ETPT_CA_JUR!G11=0,"",ETPT_CA_JUR!G11)))</f>
+        <v/>
+      </c>
+      <c r="H11" s="137">
+        <f>ETPT_CA_JUR!H11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I11),"",IF(ETPT_CA_JUR!I11=0,"",ETPT_CA_JUR!I11)))</f>
+        <v/>
+      </c>
+      <c r="J11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J11),"",IF(ETPT_CA_JUR!J11=0,"",ETPT_CA_JUR!J11)))</f>
+        <v/>
+      </c>
+      <c r="K11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K11),"",IF(ETPT_CA_JUR!K11=0,"",ETPT_CA_JUR!K11)))</f>
+        <v/>
+      </c>
+      <c r="L11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L11),"",IF(ETPT_CA_JUR!L11=0,"",ETPT_CA_JUR!L11)))</f>
+        <v/>
+      </c>
+      <c r="M11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M11),"",IF(ETPT_CA_JUR!M11=0,"",ETPT_CA_JUR!M11)))</f>
+        <v/>
+      </c>
+      <c r="N11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N11),"",IF(ETPT_CA_JUR!N11=0,"",ETPT_CA_JUR!N11)))</f>
+        <v/>
+      </c>
+      <c r="O11" s="137">
+        <f>ETPT_CA_JUR!O11</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P11),"",IF(ETPT_CA_JUR!P11=0,"",ETPT_CA_JUR!P11)))</f>
+        <v/>
+      </c>
+      <c r="Q11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q11),"",IF(ETPT_CA_JUR!Q11=0,"",ETPT_CA_JUR!Q11)))</f>
+        <v/>
+      </c>
+      <c r="R11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R11),"",IF(ETPT_CA_JUR!R11=0,"",ETPT_CA_JUR!R11)))</f>
+        <v/>
+      </c>
+      <c r="S11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S11),"",IF(ETPT_CA_JUR!S11=0,"",ETPT_CA_JUR!S11)))</f>
+        <v/>
+      </c>
+      <c r="T11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T11),"",IF(ETPT_CA_JUR!T11=0,"",ETPT_CA_JUR!T11)))</f>
+        <v/>
+      </c>
+      <c r="U11" s="137">
+        <f>ETPT_CA_JUR!U11</f>
+        <v>0</v>
+      </c>
+      <c r="V11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V11),"",IF(ETPT_CA_JUR!V11=0,"",ETPT_CA_JUR!V11)))</f>
+        <v/>
+      </c>
+      <c r="W11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W11),"",IF(ETPT_CA_JUR!W11=0,"",ETPT_CA_JUR!W11)))</f>
+        <v/>
+      </c>
+      <c r="X11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X11),"",IF(ETPT_CA_JUR!X11=0,"",ETPT_CA_JUR!X11)))</f>
+        <v/>
+      </c>
+      <c r="Y11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y11),"",IF(ETPT_CA_JUR!Y11=0,"",ETPT_CA_JUR!Y11)))</f>
+        <v/>
+      </c>
+      <c r="Z11" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z11),"",IF(ETPT_CA_JUR!Z11=0,"",ETPT_CA_JUR!Z11)))</f>
+        <v/>
+      </c>
+      <c r="AA11" s="137">
+        <f>ETPT_CA_JUR!AA11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="40"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E12" s="96" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G12),"",IF(ETPT_CA_JUR!G12=0,"",ETPT_CA_JUR!G12)))</f>
+        <v/>
+      </c>
+      <c r="H12" s="137">
+        <f>ETPT_CA_JUR!H12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I12),"",IF(ETPT_CA_JUR!I12=0,"",ETPT_CA_JUR!I12)))</f>
+        <v/>
+      </c>
+      <c r="J12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J12),"",IF(ETPT_CA_JUR!J12=0,"",ETPT_CA_JUR!J12)))</f>
+        <v/>
+      </c>
+      <c r="K12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K12),"",IF(ETPT_CA_JUR!K12=0,"",ETPT_CA_JUR!K12)))</f>
+        <v/>
+      </c>
+      <c r="L12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L12),"",IF(ETPT_CA_JUR!L12=0,"",ETPT_CA_JUR!L12)))</f>
+        <v/>
+      </c>
+      <c r="M12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M12),"",IF(ETPT_CA_JUR!M12=0,"",ETPT_CA_JUR!M12)))</f>
+        <v/>
+      </c>
+      <c r="N12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N12),"",IF(ETPT_CA_JUR!N12=0,"",ETPT_CA_JUR!N12)))</f>
+        <v/>
+      </c>
+      <c r="O12" s="137">
+        <f>ETPT_CA_JUR!O12</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P12),"",IF(ETPT_CA_JUR!P12=0,"",ETPT_CA_JUR!P12)))</f>
+        <v/>
+      </c>
+      <c r="Q12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q12),"",IF(ETPT_CA_JUR!Q12=0,"",ETPT_CA_JUR!Q12)))</f>
+        <v/>
+      </c>
+      <c r="R12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R12),"",IF(ETPT_CA_JUR!R12=0,"",ETPT_CA_JUR!R12)))</f>
+        <v/>
+      </c>
+      <c r="S12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S12),"",IF(ETPT_CA_JUR!S12=0,"",ETPT_CA_JUR!S12)))</f>
+        <v/>
+      </c>
+      <c r="T12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T12),"",IF(ETPT_CA_JUR!T12=0,"",ETPT_CA_JUR!T12)))</f>
+        <v/>
+      </c>
+      <c r="U12" s="137">
+        <f>ETPT_CA_JUR!U12</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V12),"",IF(ETPT_CA_JUR!V12=0,"",ETPT_CA_JUR!V12)))</f>
+        <v/>
+      </c>
+      <c r="W12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W12),"",IF(ETPT_CA_JUR!W12=0,"",ETPT_CA_JUR!W12)))</f>
+        <v/>
+      </c>
+      <c r="X12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X12),"",IF(ETPT_CA_JUR!X12=0,"",ETPT_CA_JUR!X12)))</f>
+        <v/>
+      </c>
+      <c r="Y12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y12),"",IF(ETPT_CA_JUR!Y12=0,"",ETPT_CA_JUR!Y12)))</f>
+        <v/>
+      </c>
+      <c r="Z12" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z12),"",IF(ETPT_CA_JUR!Z12=0,"",ETPT_CA_JUR!Z12)))</f>
+        <v/>
+      </c>
+      <c r="AA12" s="137">
+        <f>ETPT_CA_JUR!AA12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="D13" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>A</v>
+      </c>
+      <c r="E13" s="96" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="96" t="s">
+        <v>115</v>
+      </c>
+      <c r="G13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G13),"",IF(ETPT_CA_JUR!G13=0,"",ETPT_CA_JUR!G13)))</f>
+        <v/>
+      </c>
+      <c r="H13" s="137">
+        <f>ETPT_CA_JUR!H13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I13),"",IF(ETPT_CA_JUR!I13=0,"",ETPT_CA_JUR!I13)))</f>
+        <v/>
+      </c>
+      <c r="J13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J13),"",IF(ETPT_CA_JUR!J13=0,"",ETPT_CA_JUR!J13)))</f>
+        <v/>
+      </c>
+      <c r="K13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K13),"",IF(ETPT_CA_JUR!K13=0,"",ETPT_CA_JUR!K13)))</f>
+        <v/>
+      </c>
+      <c r="L13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L13),"",IF(ETPT_CA_JUR!L13=0,"",ETPT_CA_JUR!L13)))</f>
+        <v/>
+      </c>
+      <c r="M13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M13),"",IF(ETPT_CA_JUR!M13=0,"",ETPT_CA_JUR!M13)))</f>
+        <v/>
+      </c>
+      <c r="N13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N13),"",IF(ETPT_CA_JUR!N13=0,"",ETPT_CA_JUR!N13)))</f>
+        <v/>
+      </c>
+      <c r="O13" s="137">
+        <f>ETPT_CA_JUR!O13</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P13),"",IF(ETPT_CA_JUR!P13=0,"",ETPT_CA_JUR!P13)))</f>
+        <v/>
+      </c>
+      <c r="Q13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q13),"",IF(ETPT_CA_JUR!Q13=0,"",ETPT_CA_JUR!Q13)))</f>
+        <v/>
+      </c>
+      <c r="R13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R13),"",IF(ETPT_CA_JUR!R13=0,"",ETPT_CA_JUR!R13)))</f>
+        <v/>
+      </c>
+      <c r="S13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S13),"",IF(ETPT_CA_JUR!S13=0,"",ETPT_CA_JUR!S13)))</f>
+        <v/>
+      </c>
+      <c r="T13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T13),"",IF(ETPT_CA_JUR!T13=0,"",ETPT_CA_JUR!T13)))</f>
+        <v/>
+      </c>
+      <c r="U13" s="137">
+        <f>ETPT_CA_JUR!U13</f>
+        <v>0</v>
+      </c>
+      <c r="V13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V13),"",IF(ETPT_CA_JUR!V13=0,"",ETPT_CA_JUR!V13)))</f>
+        <v/>
+      </c>
+      <c r="W13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W13),"",IF(ETPT_CA_JUR!W13=0,"",ETPT_CA_JUR!W13)))</f>
+        <v/>
+      </c>
+      <c r="X13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X13),"",IF(ETPT_CA_JUR!X13=0,"",ETPT_CA_JUR!X13)))</f>
+        <v/>
+      </c>
+      <c r="Y13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y13),"",IF(ETPT_CA_JUR!Y13=0,"",ETPT_CA_JUR!Y13)))</f>
+        <v/>
+      </c>
+      <c r="Z13" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z13),"",IF(ETPT_CA_JUR!Z13=0,"",ETPT_CA_JUR!Z13)))</f>
+        <v/>
+      </c>
+      <c r="AA13" s="137">
+        <f>ETPT_CA_JUR!AA13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="D14" s="38" t="str">
+        <f>IF(ISBLANK($D$3),"",$D$3)</f>
+        <v>A</v>
+      </c>
+      <c r="E14" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G14),"",IF(ETPT_CA_JUR!G14=0,"",ETPT_CA_JUR!G14)))</f>
+        <v/>
+      </c>
+      <c r="H14" s="137">
+        <f>ETPT_CA_JUR!H14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I14),"",IF(ETPT_CA_JUR!I14=0,"",ETPT_CA_JUR!I14)))</f>
+        <v/>
+      </c>
+      <c r="J14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J14),"",IF(ETPT_CA_JUR!J14=0,"",ETPT_CA_JUR!J14)))</f>
+        <v/>
+      </c>
+      <c r="K14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K14),"",IF(ETPT_CA_JUR!K14=0,"",ETPT_CA_JUR!K14)))</f>
+        <v/>
+      </c>
+      <c r="L14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L14),"",IF(ETPT_CA_JUR!L14=0,"",ETPT_CA_JUR!L14)))</f>
+        <v/>
+      </c>
+      <c r="M14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M14),"",IF(ETPT_CA_JUR!M14=0,"",ETPT_CA_JUR!M14)))</f>
+        <v/>
+      </c>
+      <c r="N14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N14),"",IF(ETPT_CA_JUR!N14=0,"",ETPT_CA_JUR!N14)))</f>
+        <v/>
+      </c>
+      <c r="O14" s="137">
+        <f>ETPT_CA_JUR!O14</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P14),"",IF(ETPT_CA_JUR!P14=0,"",ETPT_CA_JUR!P14)))</f>
+        <v/>
+      </c>
+      <c r="Q14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q14),"",IF(ETPT_CA_JUR!Q14=0,"",ETPT_CA_JUR!Q14)))</f>
+        <v/>
+      </c>
+      <c r="R14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R14),"",IF(ETPT_CA_JUR!R14=0,"",ETPT_CA_JUR!R14)))</f>
+        <v/>
+      </c>
+      <c r="S14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S14),"",IF(ETPT_CA_JUR!S14=0,"",ETPT_CA_JUR!S14)))</f>
+        <v/>
+      </c>
+      <c r="T14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T14),"",IF(ETPT_CA_JUR!T14=0,"",ETPT_CA_JUR!T14)))</f>
+        <v/>
+      </c>
+      <c r="U14" s="137">
+        <f>ETPT_CA_JUR!U14</f>
+        <v>0</v>
+      </c>
+      <c r="V14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V14),"",IF(ETPT_CA_JUR!V14=0,"",ETPT_CA_JUR!V14)))</f>
+        <v/>
+      </c>
+      <c r="W14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W14),"",IF(ETPT_CA_JUR!W14=0,"",ETPT_CA_JUR!W14)))</f>
+        <v/>
+      </c>
+      <c r="X14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X14),"",IF(ETPT_CA_JUR!X14=0,"",ETPT_CA_JUR!X14)))</f>
+        <v/>
+      </c>
+      <c r="Y14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y14),"",IF(ETPT_CA_JUR!Y14=0,"",ETPT_CA_JUR!Y14)))</f>
+        <v/>
+      </c>
+      <c r="Z14" s="136" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z14),"",IF(ETPT_CA_JUR!Z14=0,"",ETPT_CA_JUR!Z14)))</f>
+        <v/>
+      </c>
+      <c r="AA14" s="137">
+        <f>ETPT_CA_JUR!AA14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="D15" s="38"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="98" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="137">
+        <f>ETPT_CA_JUR!G15</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="137">
+        <f>ETPT_CA_JUR!H15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="137">
+        <f>ETPT_CA_JUR!I15</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="137">
+        <f>ETPT_CA_JUR!J15</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="137">
+        <f>ETPT_CA_JUR!K15</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="137">
+        <f>ETPT_CA_JUR!L15</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="137">
+        <f>ETPT_CA_JUR!M15</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="137">
+        <f>ETPT_CA_JUR!N15</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="137">
+        <f>ETPT_CA_JUR!O15</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="137">
+        <f>ETPT_CA_JUR!P15</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="137">
+        <f>ETPT_CA_JUR!Q15</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="137">
+        <f>ETPT_CA_JUR!R15</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="137">
+        <f>ETPT_CA_JUR!S15</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="137">
+        <f>ETPT_CA_JUR!T15</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="137">
+        <f>ETPT_CA_JUR!U15</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="137">
+        <f>ETPT_CA_JUR!V15</f>
+        <v>0</v>
+      </c>
+      <c r="W15" s="137">
+        <f>ETPT_CA_JUR!W15</f>
+        <v>0</v>
+      </c>
+      <c r="X15" s="137">
+        <f>ETPT_CA_JUR!X15</f>
+        <v>0</v>
+      </c>
+      <c r="Y15" s="137">
+        <f>ETPT_CA_JUR!Y15</f>
+        <v>0</v>
+      </c>
+      <c r="Z15" s="137">
+        <f>ETPT_CA_JUR!Z15</f>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="137">
+        <f>ETPT_CA_JUR!AA15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="138"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="138"/>
+      <c r="J16" s="138"/>
+      <c r="K16" s="138"/>
+      <c r="L16" s="138"/>
+      <c r="M16" s="138"/>
+      <c r="N16" s="138"/>
+      <c r="O16" s="138"/>
+      <c r="P16" s="138"/>
+      <c r="Q16" s="138"/>
+      <c r="R16" s="138"/>
+      <c r="S16" s="138"/>
+      <c r="T16" s="138"/>
+      <c r="U16" s="138"/>
+      <c r="V16" s="138"/>
+      <c r="W16" s="138"/>
+      <c r="X16" s="138"/>
+      <c r="Y16" s="138"/>
+      <c r="Z16" s="138"/>
+      <c r="AA16" s="138"/>
+    </row>
+    <row r="17" spans="1:27" ht="24" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17" s="135"/>
+      <c r="E17" s="135"/>
+      <c r="F17" s="151" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="140" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G17),"",IF(ETPT_CA_JUR!G17=0,"",ETPT_CA_JUR!G17)))</f>
+        <v/>
+      </c>
+      <c r="H17" s="139"/>
+      <c r="I17" s="202" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="203"/>
+      <c r="K17" s="203"/>
+      <c r="L17" s="203"/>
+      <c r="M17" s="204"/>
+      <c r="N17" s="140" t="str">
+        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N17),"",IF(ETPT_CA_JUR!N17=0,"",ETPT_CA_JUR!N17)))</f>
+        <v/>
+      </c>
+      <c r="O17" s="139"/>
+      <c r="P17" s="139"/>
+      <c r="Q17" s="139"/>
+      <c r="R17" s="139"/>
+      <c r="S17" s="139"/>
+      <c r="T17" s="139"/>
+      <c r="U17" s="139"/>
+      <c r="V17" s="139"/>
+      <c r="W17" s="139"/>
+      <c r="X17" s="139"/>
+      <c r="Y17" s="139"/>
+      <c r="Z17" s="139"/>
+      <c r="AA17" s="139"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I17:M17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB554CC5-4631-9C4D-9EF1-39CD273D3537}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -6533,7 +8296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AA5FE4-5D9A-904C-8E7D-D70A5B5F8254}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -7118,7 +8881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA9DAE4-6E6E-634B-B61F-BD7DA00BF20E}">
   <dimension ref="A1:U17"/>
   <sheetViews>
@@ -7133,13 +8896,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="194" t="s">
+      <c r="A1" s="205" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="194"/>
-      <c r="C1" s="194"/>
-      <c r="D1" s="194"/>
-      <c r="E1" s="194"/>
+      <c r="B1" s="205"/>
+      <c r="C1" s="205"/>
+      <c r="D1" s="205"/>
+      <c r="E1" s="205"/>
       <c r="F1" s="153"/>
       <c r="G1" s="154"/>
       <c r="H1" s="154"/>
@@ -7885,7 +9648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A2E841C-99B1-2944-9963-E2DDCA0EE564}">
   <dimension ref="A1:Q144"/>
   <sheetViews>
@@ -7900,12 +9663,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="195" t="s">
+      <c r="A1" s="206" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="195"/>
-      <c r="C1" s="195"/>
-      <c r="D1" s="195"/>
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
       <c r="E1" s="120"/>
       <c r="F1" s="119"/>
       <c r="G1" s="119"/>
@@ -7955,7 +9718,7 @@
       <c r="O2" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="196" t="s">
+      <c r="P2" s="207" t="s">
         <v>138</v>
       </c>
     </row>
@@ -7995,7 +9758,7 @@
       <c r="O3" s="105" t="s">
         <v>145</v>
       </c>
-      <c r="P3" s="196"/>
+      <c r="P3" s="207"/>
     </row>
     <row r="4" spans="1:16" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="106" t="s">
@@ -8043,7 +9806,7 @@
       <c r="O4" s="108" t="s">
         <v>282</v>
       </c>
-      <c r="P4" s="196"/>
+      <c r="P4" s="207"/>
     </row>
     <row r="5" spans="1:16" ht="252" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="109"/>
@@ -8929,22 +10692,22 @@
       <c r="A1" s="131"/>
       <c r="B1" s="131"/>
       <c r="C1" s="131"/>
-      <c r="D1" s="182" t="s">
+      <c r="D1" s="193" t="s">
         <v>286</v>
       </c>
-      <c r="E1" s="182"/>
-      <c r="F1" s="182"/>
-      <c r="G1" s="182"/>
-      <c r="H1" s="182"/>
-      <c r="I1" s="182"/>
-      <c r="J1" s="182"/>
-      <c r="K1" s="182"/>
-      <c r="L1" s="182"/>
-      <c r="M1" s="182"/>
-      <c r="N1" s="182"/>
-      <c r="O1" s="182"/>
-      <c r="P1" s="182"/>
-      <c r="Q1" s="182"/>
+      <c r="E1" s="193"/>
+      <c r="F1" s="193"/>
+      <c r="G1" s="193"/>
+      <c r="H1" s="193"/>
+      <c r="I1" s="193"/>
+      <c r="J1" s="193"/>
+      <c r="K1" s="193"/>
+      <c r="L1" s="193"/>
+      <c r="M1" s="193"/>
+      <c r="N1" s="193"/>
+      <c r="O1" s="193"/>
+      <c r="P1" s="193"/>
+      <c r="Q1" s="193"/>
       <c r="R1" s="132" t="s">
         <v>130</v>
       </c>
@@ -8986,8 +10749,8 @@
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="11" priority="2" stopIfTrue="1">
-      <formula>AND(OR($R1&lt;&gt;"-",$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
+    <cfRule type="expression" dxfId="22" priority="2">
+      <formula>AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9004,7 +10767,7 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AE18" sqref="AE18"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9031,7 +10794,7 @@
         <v>96</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>82</v>
+        <v>333</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -9085,28 +10848,28 @@
       <c r="D4" s="75"/>
       <c r="E4" s="75"/>
       <c r="F4" s="75"/>
-      <c r="G4" s="183" t="s">
+      <c r="G4" s="194" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="184"/>
-      <c r="K4" s="184"/>
-      <c r="L4" s="185"/>
-      <c r="M4" s="186"/>
-      <c r="N4" s="187" t="s">
+      <c r="H4" s="195"/>
+      <c r="I4" s="195"/>
+      <c r="J4" s="195"/>
+      <c r="K4" s="195"/>
+      <c r="L4" s="196"/>
+      <c r="M4" s="197"/>
+      <c r="N4" s="198" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="185"/>
-      <c r="P4" s="185"/>
-      <c r="Q4" s="185"/>
-      <c r="R4" s="185"/>
-      <c r="S4" s="185"/>
-      <c r="T4" s="188"/>
-      <c r="U4" s="183" t="s">
+      <c r="O4" s="196"/>
+      <c r="P4" s="196"/>
+      <c r="Q4" s="196"/>
+      <c r="R4" s="196"/>
+      <c r="S4" s="196"/>
+      <c r="T4" s="199"/>
+      <c r="U4" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="186"/>
+      <c r="V4" s="197"/>
       <c r="W4" s="82"/>
       <c r="X4" t="s">
         <v>0</v>
@@ -9304,57 +11067,57 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="10" priority="20">
+    <cfRule type="expression" dxfId="21" priority="20">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:F6 C7:V151">
-    <cfRule type="expression" dxfId="9" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="8" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="7" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="17" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L6)&lt;&gt;_xlfn.NUMBERVALUE($L7),_xlfn.NUMBERVALUE($S6)&lt;&gt;_xlfn.NUMBERVALUE($S7),_xlfn.NUMBERVALUE($U6)&lt;&gt;_xlfn.NUMBERVALUE($U7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="17" priority="6">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="5" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:V6">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="2" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9364,6 +11127,240 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ECF8FA8-E8EA-D647-9FEC-F590B68508F3}">
+  <dimension ref="A1:W3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="17.83203125" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="19" max="20" width="19" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" customWidth="1"/>
+    <col min="22" max="22" width="255.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="112" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>295</v>
+      </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="167" t="s">
+        <v>296</v>
+      </c>
+      <c r="H1" s="167" t="s">
+        <v>297</v>
+      </c>
+      <c r="I1" s="168" t="s">
+        <v>298</v>
+      </c>
+      <c r="J1" s="168" t="s">
+        <v>299</v>
+      </c>
+      <c r="K1" s="168" t="s">
+        <v>300</v>
+      </c>
+      <c r="L1" s="169" t="s">
+        <v>301</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>302</v>
+      </c>
+      <c r="N1" s="169" t="s">
+        <v>303</v>
+      </c>
+      <c r="O1" s="170" t="s">
+        <v>304</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q1" s="170" t="s">
+        <v>306</v>
+      </c>
+      <c r="R1" s="170" t="s">
+        <v>307</v>
+      </c>
+      <c r="S1" s="167" t="s">
+        <v>308</v>
+      </c>
+      <c r="T1" s="167" t="s">
+        <v>334</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="V1" s="172" t="s">
+        <v>332</v>
+      </c>
+      <c r="W1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="171" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" s="171" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" s="171" t="s">
+        <v>312</v>
+      </c>
+      <c r="D2" s="171" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" s="171" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2" s="171" t="s">
+        <v>315</v>
+      </c>
+      <c r="G2" s="171" t="s">
+        <v>316</v>
+      </c>
+      <c r="H2" s="171" t="s">
+        <v>317</v>
+      </c>
+      <c r="I2" s="176" t="s">
+        <v>318</v>
+      </c>
+      <c r="J2" s="176" t="s">
+        <v>319</v>
+      </c>
+      <c r="K2" s="174" t="s">
+        <v>320</v>
+      </c>
+      <c r="L2" s="174" t="s">
+        <v>321</v>
+      </c>
+      <c r="M2" s="175" t="s">
+        <v>322</v>
+      </c>
+      <c r="N2" s="177" t="s">
+        <v>323</v>
+      </c>
+      <c r="O2" s="174" t="s">
+        <v>324</v>
+      </c>
+      <c r="P2" s="174" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q2" s="174" t="s">
+        <v>326</v>
+      </c>
+      <c r="R2" s="174" t="s">
+        <v>327</v>
+      </c>
+      <c r="S2" s="174" t="s">
+        <v>328</v>
+      </c>
+      <c r="T2" s="174" t="s">
+        <v>335</v>
+      </c>
+      <c r="U2" s="174" t="s">
+        <v>329</v>
+      </c>
+      <c r="V2" s="173" t="s">
+        <v>330</v>
+      </c>
+      <c r="W2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:B1">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>AND(OR($I1&lt;&gt;"-",#REF!&lt;&gt;0,#REF!&lt;&gt;0,ISBLANK($M1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:F2">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+      <formula>$F2="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:N2">
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>$F2="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:K2">
+    <cfRule type="expression" dxfId="7" priority="6">
+      <formula>1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2">
+    <cfRule type="expression" dxfId="6" priority="8">
+      <formula>1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:V2">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$F2="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:R2">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S2:T2">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0AF7A98-8726-2B45-9E0D-08F39416C73F}">
   <sheetPr codeName="Feuil19"/>
   <dimension ref="L1:L19"/>
@@ -9474,7 +11471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDB0A74-92BE-614C-B933-4270BECA0D39}">
   <sheetPr codeName="Feuil12"/>
   <dimension ref="A1:M21"/>
@@ -9637,7 +11634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40175DB0-40DB-6046-B965-F2F52476B1A1}">
   <sheetPr codeName="Feuil14">
     <pageSetUpPr fitToPage="1"/>
@@ -9749,7 +11746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C2B6A9-5FC7-3A43-BF37-0B81E3F33F51}">
   <sheetPr codeName="Feuil16">
     <tabColor rgb="FF01A94F"/>
@@ -11205,13 +13202,13 @@
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("Fonction recodée",'ETPT A-JUST'!2:2,0)),{"Fonctionnaire CTECH placé ADD";"Fonctionnaire CTECH placé SUB"}))</f>
         <v>#N/A</v>
       </c>
-      <c r="I17" s="189" t="s">
+      <c r="I17" s="200" t="s">
         <v>119</v>
       </c>
-      <c r="J17" s="189"/>
-      <c r="K17" s="189"/>
-      <c r="L17" s="189"/>
-      <c r="M17" s="190"/>
+      <c r="J17" s="200"/>
+      <c r="K17" s="200"/>
+      <c r="L17" s="200"/>
+      <c r="M17" s="201"/>
       <c r="N17" s="73" t="e" cm="1">
         <f t="array" ref="N17">SUM(SUMIFS(
 INDEX( 'ETPT A-JUST'!$A:$ZZ,,MATCH("14. TOTAL INDISPONIBILITÉ",'ETPT A-JUST'!2:2,0)),
@@ -11226,1494 +13223,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701921C7-025B-4F4F-A5C7-6D94075AC520}">
-  <sheetPr codeName="Feuil8">
-    <tabColor rgb="FFC00000"/>
-  </sheetPr>
-  <dimension ref="A1:AA17"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6" style="37" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" style="37" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" style="37" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="37" customWidth="1"/>
-    <col min="5" max="5" width="6.5" style="37" customWidth="1"/>
-    <col min="6" max="6" width="50" style="37" customWidth="1"/>
-    <col min="7" max="27" width="14" style="37" customWidth="1"/>
-    <col min="28" max="34" width="9.33203125" style="37" customWidth="1"/>
-    <col min="35" max="35" width="8.5" style="37" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14" style="37" customWidth="1"/>
-    <col min="38" max="58" width="9.33203125" style="37" customWidth="1"/>
-    <col min="59" max="59" width="4" style="37" customWidth="1"/>
-    <col min="60" max="16384" width="11" style="37"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:27" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-    </row>
-    <row r="2" spans="1:27" ht="36" x14ac:dyDescent="0.2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="95" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="95" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="99" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="100" t="s">
-        <v>81</v>
-      </c>
-      <c r="I2" s="99" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="99" t="s">
-        <v>273</v>
-      </c>
-      <c r="K2" s="99" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" s="99" t="s">
-        <v>274</v>
-      </c>
-      <c r="M2" s="99" t="s">
-        <v>110</v>
-      </c>
-      <c r="N2" s="99" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="100" t="s">
-        <v>80</v>
-      </c>
-      <c r="P2" s="99" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q2" s="99" t="s">
-        <v>65</v>
-      </c>
-      <c r="R2" s="99" t="s">
-        <v>276</v>
-      </c>
-      <c r="S2" s="99" t="s">
-        <v>112</v>
-      </c>
-      <c r="T2" s="99" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="100" t="s">
-        <v>79</v>
-      </c>
-      <c r="V2" s="99" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" s="99" t="s">
-        <v>284</v>
-      </c>
-      <c r="X2" s="99" t="s">
-        <v>285</v>
-      </c>
-      <c r="Y2" s="99" t="s">
-        <v>61</v>
-      </c>
-      <c r="Z2" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA2" s="100" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A3" s="42"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="150" t="s">
-        <v>266</v>
-      </c>
-      <c r="E3" s="96" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" s="96" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G3),"",IF(ETPT_CA_JUR!G3=0,"",ETPT_CA_JUR!G3)))</f>
-        <v/>
-      </c>
-      <c r="H3" s="137">
-        <f>ETPT_CA_JUR!H3</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I3),"",IF(ETPT_CA_JUR!I3=0,"",ETPT_CA_JUR!I3)))</f>
-        <v/>
-      </c>
-      <c r="J3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J3),"",IF(ETPT_CA_JUR!J3=0,"",ETPT_CA_JUR!J3)))</f>
-        <v/>
-      </c>
-      <c r="K3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K3),"",IF(ETPT_CA_JUR!K3=0,"",ETPT_CA_JUR!K3)))</f>
-        <v/>
-      </c>
-      <c r="L3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L3),"",IF(ETPT_CA_JUR!L3=0,"",ETPT_CA_JUR!L3)))</f>
-        <v/>
-      </c>
-      <c r="M3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M3),"",IF(ETPT_CA_JUR!M3=0,"",ETPT_CA_JUR!M3)))</f>
-        <v/>
-      </c>
-      <c r="N3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N3),"",IF(ETPT_CA_JUR!N3=0,"",ETPT_CA_JUR!N3)))</f>
-        <v/>
-      </c>
-      <c r="O3" s="137">
-        <f>ETPT_CA_JUR!O3</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P3),"",IF(ETPT_CA_JUR!P3=0,"",ETPT_CA_JUR!P3)))</f>
-        <v/>
-      </c>
-      <c r="Q3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q3),"",IF(ETPT_CA_JUR!Q3=0,"",ETPT_CA_JUR!Q3)))</f>
-        <v/>
-      </c>
-      <c r="R3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R3),"",IF(ETPT_CA_JUR!R3=0,"",ETPT_CA_JUR!R3)))</f>
-        <v/>
-      </c>
-      <c r="S3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S3),"",IF(ETPT_CA_JUR!S3=0,"",ETPT_CA_JUR!S3)))</f>
-        <v/>
-      </c>
-      <c r="T3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T3),"",IF(ETPT_CA_JUR!T3=0,"",ETPT_CA_JUR!T3)))</f>
-        <v/>
-      </c>
-      <c r="U3" s="137">
-        <f>ETPT_CA_JUR!U3</f>
-        <v>0</v>
-      </c>
-      <c r="V3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V3),"",IF(ETPT_CA_JUR!V3=0,"",ETPT_CA_JUR!V3)))</f>
-        <v/>
-      </c>
-      <c r="W3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W3),"",IF(ETPT_CA_JUR!W3=0,"",ETPT_CA_JUR!W3)))</f>
-        <v/>
-      </c>
-      <c r="X3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X3),"",IF(ETPT_CA_JUR!X3=0,"",ETPT_CA_JUR!X3)))</f>
-        <v/>
-      </c>
-      <c r="Y3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y3),"",IF(ETPT_CA_JUR!Y3=0,"",ETPT_CA_JUR!Y3)))</f>
-        <v/>
-      </c>
-      <c r="Z3" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z3),"",IF(ETPT_CA_JUR!Z3=0,"",ETPT_CA_JUR!Z3)))</f>
-        <v/>
-      </c>
-      <c r="AA3" s="137">
-        <f>ETPT_CA_JUR!AA3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A4" s="42"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="38" t="str">
-        <f>IF(ISBLANK($D$3),"",$D$3)</f>
-        <v>A</v>
-      </c>
-      <c r="E4" s="96" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G4),"",IF(ETPT_CA_JUR!G4=0,"",ETPT_CA_JUR!G4)))</f>
-        <v/>
-      </c>
-      <c r="H4" s="137">
-        <f>ETPT_CA_JUR!H4</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I4),"",IF(ETPT_CA_JUR!I4=0,"",ETPT_CA_JUR!I4)))</f>
-        <v/>
-      </c>
-      <c r="J4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J4),"",IF(ETPT_CA_JUR!J4=0,"",ETPT_CA_JUR!J4)))</f>
-        <v/>
-      </c>
-      <c r="K4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K4),"",IF(ETPT_CA_JUR!K4=0,"",ETPT_CA_JUR!K4)))</f>
-        <v/>
-      </c>
-      <c r="L4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L4),"",IF(ETPT_CA_JUR!L4=0,"",ETPT_CA_JUR!L4)))</f>
-        <v/>
-      </c>
-      <c r="M4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M4),"",IF(ETPT_CA_JUR!M4=0,"",ETPT_CA_JUR!M4)))</f>
-        <v/>
-      </c>
-      <c r="N4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N4),"",IF(ETPT_CA_JUR!N4=0,"",ETPT_CA_JUR!N4)))</f>
-        <v/>
-      </c>
-      <c r="O4" s="137">
-        <f>ETPT_CA_JUR!O4</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P4),"",IF(ETPT_CA_JUR!P4=0,"",ETPT_CA_JUR!P4)))</f>
-        <v/>
-      </c>
-      <c r="Q4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q4),"",IF(ETPT_CA_JUR!Q4=0,"",ETPT_CA_JUR!Q4)))</f>
-        <v/>
-      </c>
-      <c r="R4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R4),"",IF(ETPT_CA_JUR!R4=0,"",ETPT_CA_JUR!R4)))</f>
-        <v/>
-      </c>
-      <c r="S4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S4),"",IF(ETPT_CA_JUR!S4=0,"",ETPT_CA_JUR!S4)))</f>
-        <v/>
-      </c>
-      <c r="T4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T4),"",IF(ETPT_CA_JUR!T4=0,"",ETPT_CA_JUR!T4)))</f>
-        <v/>
-      </c>
-      <c r="U4" s="137">
-        <f>ETPT_CA_JUR!U4</f>
-        <v>0</v>
-      </c>
-      <c r="V4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V4),"",IF(ETPT_CA_JUR!V4=0,"",ETPT_CA_JUR!V4)))</f>
-        <v/>
-      </c>
-      <c r="W4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W4),"",IF(ETPT_CA_JUR!W4=0,"",ETPT_CA_JUR!W4)))</f>
-        <v/>
-      </c>
-      <c r="X4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X4),"",IF(ETPT_CA_JUR!X4=0,"",ETPT_CA_JUR!X4)))</f>
-        <v/>
-      </c>
-      <c r="Y4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y4),"",IF(ETPT_CA_JUR!Y4=0,"",ETPT_CA_JUR!Y4)))</f>
-        <v/>
-      </c>
-      <c r="Z4" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z4),"",IF(ETPT_CA_JUR!Z4=0,"",ETPT_CA_JUR!Z4)))</f>
-        <v/>
-      </c>
-      <c r="AA4" s="137">
-        <f>ETPT_CA_JUR!AA4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A5" s="42"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="38" t="str">
-        <f t="shared" ref="D5:D13" si="0">IF(ISBLANK($D$3),"",$D$3)</f>
-        <v>A</v>
-      </c>
-      <c r="E5" s="96" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="96" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G5),"",IF(ETPT_CA_JUR!G5=0,"",ETPT_CA_JUR!G5)))</f>
-        <v/>
-      </c>
-      <c r="H5" s="137">
-        <f>ETPT_CA_JUR!H5</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I5),"",IF(ETPT_CA_JUR!I5=0,"",ETPT_CA_JUR!I5)))</f>
-        <v/>
-      </c>
-      <c r="J5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J5),"",IF(ETPT_CA_JUR!J5=0,"",ETPT_CA_JUR!J5)))</f>
-        <v/>
-      </c>
-      <c r="K5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K5),"",IF(ETPT_CA_JUR!K5=0,"",ETPT_CA_JUR!K5)))</f>
-        <v/>
-      </c>
-      <c r="L5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L5),"",IF(ETPT_CA_JUR!L5=0,"",ETPT_CA_JUR!L5)))</f>
-        <v/>
-      </c>
-      <c r="M5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M5),"",IF(ETPT_CA_JUR!M5=0,"",ETPT_CA_JUR!M5)))</f>
-        <v/>
-      </c>
-      <c r="N5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N5),"",IF(ETPT_CA_JUR!N5=0,"",ETPT_CA_JUR!N5)))</f>
-        <v/>
-      </c>
-      <c r="O5" s="137">
-        <f>ETPT_CA_JUR!O5</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P5),"",IF(ETPT_CA_JUR!P5=0,"",ETPT_CA_JUR!P5)))</f>
-        <v/>
-      </c>
-      <c r="Q5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q5),"",IF(ETPT_CA_JUR!Q5=0,"",ETPT_CA_JUR!Q5)))</f>
-        <v/>
-      </c>
-      <c r="R5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R5),"",IF(ETPT_CA_JUR!R5=0,"",ETPT_CA_JUR!R5)))</f>
-        <v/>
-      </c>
-      <c r="S5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S5),"",IF(ETPT_CA_JUR!S5=0,"",ETPT_CA_JUR!S5)))</f>
-        <v/>
-      </c>
-      <c r="T5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T5),"",IF(ETPT_CA_JUR!T5=0,"",ETPT_CA_JUR!T5)))</f>
-        <v/>
-      </c>
-      <c r="U5" s="137">
-        <f>ETPT_CA_JUR!U5</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V5),"",IF(ETPT_CA_JUR!V5=0,"",ETPT_CA_JUR!V5)))</f>
-        <v/>
-      </c>
-      <c r="W5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W5),"",IF(ETPT_CA_JUR!W5=0,"",ETPT_CA_JUR!W5)))</f>
-        <v/>
-      </c>
-      <c r="X5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X5),"",IF(ETPT_CA_JUR!X5=0,"",ETPT_CA_JUR!X5)))</f>
-        <v/>
-      </c>
-      <c r="Y5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y5),"",IF(ETPT_CA_JUR!Y5=0,"",ETPT_CA_JUR!Y5)))</f>
-        <v/>
-      </c>
-      <c r="Z5" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z5),"",IF(ETPT_CA_JUR!Z5=0,"",ETPT_CA_JUR!Z5)))</f>
-        <v/>
-      </c>
-      <c r="AA5" s="137">
-        <f>ETPT_CA_JUR!AA5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="42"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="E6" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="96" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G6),"",IF(ETPT_CA_JUR!G6=0,"",ETPT_CA_JUR!G6)))</f>
-        <v/>
-      </c>
-      <c r="H6" s="137">
-        <f>ETPT_CA_JUR!H6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I6),"",IF(ETPT_CA_JUR!I6=0,"",ETPT_CA_JUR!I6)))</f>
-        <v/>
-      </c>
-      <c r="J6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J6),"",IF(ETPT_CA_JUR!J6=0,"",ETPT_CA_JUR!J6)))</f>
-        <v/>
-      </c>
-      <c r="K6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K6),"",IF(ETPT_CA_JUR!K6=0,"",ETPT_CA_JUR!K6)))</f>
-        <v/>
-      </c>
-      <c r="L6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L6),"",IF(ETPT_CA_JUR!L6=0,"",ETPT_CA_JUR!L6)))</f>
-        <v/>
-      </c>
-      <c r="M6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M6),"",IF(ETPT_CA_JUR!M6=0,"",ETPT_CA_JUR!M6)))</f>
-        <v/>
-      </c>
-      <c r="N6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N6),"",IF(ETPT_CA_JUR!N6=0,"",ETPT_CA_JUR!N6)))</f>
-        <v/>
-      </c>
-      <c r="O6" s="137">
-        <f>ETPT_CA_JUR!O6</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P6),"",IF(ETPT_CA_JUR!P6=0,"",ETPT_CA_JUR!P6)))</f>
-        <v/>
-      </c>
-      <c r="Q6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q6),"",IF(ETPT_CA_JUR!Q6=0,"",ETPT_CA_JUR!Q6)))</f>
-        <v/>
-      </c>
-      <c r="R6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R6),"",IF(ETPT_CA_JUR!R6=0,"",ETPT_CA_JUR!R6)))</f>
-        <v/>
-      </c>
-      <c r="S6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S6),"",IF(ETPT_CA_JUR!S6=0,"",ETPT_CA_JUR!S6)))</f>
-        <v/>
-      </c>
-      <c r="T6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T6),"",IF(ETPT_CA_JUR!T6=0,"",ETPT_CA_JUR!T6)))</f>
-        <v/>
-      </c>
-      <c r="U6" s="137">
-        <f>ETPT_CA_JUR!U6</f>
-        <v>0</v>
-      </c>
-      <c r="V6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V6),"",IF(ETPT_CA_JUR!V6=0,"",ETPT_CA_JUR!V6)))</f>
-        <v/>
-      </c>
-      <c r="W6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W6),"",IF(ETPT_CA_JUR!W6=0,"",ETPT_CA_JUR!W6)))</f>
-        <v/>
-      </c>
-      <c r="X6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X6),"",IF(ETPT_CA_JUR!X6=0,"",ETPT_CA_JUR!X6)))</f>
-        <v/>
-      </c>
-      <c r="Y6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y6),"",IF(ETPT_CA_JUR!Y6=0,"",ETPT_CA_JUR!Y6)))</f>
-        <v/>
-      </c>
-      <c r="Z6" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z6),"",IF(ETPT_CA_JUR!Z6=0,"",ETPT_CA_JUR!Z6)))</f>
-        <v/>
-      </c>
-      <c r="AA6" s="137">
-        <f>ETPT_CA_JUR!AA6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A7" s="42"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="E7" s="96" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="96" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G7),"",IF(ETPT_CA_JUR!G7=0,"",ETPT_CA_JUR!G7)))</f>
-        <v/>
-      </c>
-      <c r="H7" s="137">
-        <f>ETPT_CA_JUR!H7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I7),"",IF(ETPT_CA_JUR!I7=0,"",ETPT_CA_JUR!I7)))</f>
-        <v/>
-      </c>
-      <c r="J7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J7),"",IF(ETPT_CA_JUR!J7=0,"",ETPT_CA_JUR!J7)))</f>
-        <v/>
-      </c>
-      <c r="K7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K7),"",IF(ETPT_CA_JUR!K7=0,"",ETPT_CA_JUR!K7)))</f>
-        <v/>
-      </c>
-      <c r="L7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L7),"",IF(ETPT_CA_JUR!L7=0,"",ETPT_CA_JUR!L7)))</f>
-        <v/>
-      </c>
-      <c r="M7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M7),"",IF(ETPT_CA_JUR!M7=0,"",ETPT_CA_JUR!M7)))</f>
-        <v/>
-      </c>
-      <c r="N7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N7),"",IF(ETPT_CA_JUR!N7=0,"",ETPT_CA_JUR!N7)))</f>
-        <v/>
-      </c>
-      <c r="O7" s="137">
-        <f>ETPT_CA_JUR!O7</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P7),"",IF(ETPT_CA_JUR!P7=0,"",ETPT_CA_JUR!P7)))</f>
-        <v/>
-      </c>
-      <c r="Q7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q7),"",IF(ETPT_CA_JUR!Q7=0,"",ETPT_CA_JUR!Q7)))</f>
-        <v/>
-      </c>
-      <c r="R7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R7),"",IF(ETPT_CA_JUR!R7=0,"",ETPT_CA_JUR!R7)))</f>
-        <v/>
-      </c>
-      <c r="S7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S7),"",IF(ETPT_CA_JUR!S7=0,"",ETPT_CA_JUR!S7)))</f>
-        <v/>
-      </c>
-      <c r="T7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T7),"",IF(ETPT_CA_JUR!T7=0,"",ETPT_CA_JUR!T7)))</f>
-        <v/>
-      </c>
-      <c r="U7" s="137">
-        <f>ETPT_CA_JUR!U7</f>
-        <v>0</v>
-      </c>
-      <c r="V7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V7),"",IF(ETPT_CA_JUR!V7=0,"",ETPT_CA_JUR!V7)))</f>
-        <v/>
-      </c>
-      <c r="W7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W7),"",IF(ETPT_CA_JUR!W7=0,"",ETPT_CA_JUR!W7)))</f>
-        <v/>
-      </c>
-      <c r="X7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X7),"",IF(ETPT_CA_JUR!X7=0,"",ETPT_CA_JUR!X7)))</f>
-        <v/>
-      </c>
-      <c r="Y7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y7),"",IF(ETPT_CA_JUR!Y7=0,"",ETPT_CA_JUR!Y7)))</f>
-        <v/>
-      </c>
-      <c r="Z7" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z7),"",IF(ETPT_CA_JUR!Z7=0,"",ETPT_CA_JUR!Z7)))</f>
-        <v/>
-      </c>
-      <c r="AA7" s="137">
-        <f>ETPT_CA_JUR!AA7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="E8" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="96" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G8),"",IF(ETPT_CA_JUR!G8=0,"",ETPT_CA_JUR!G8)))</f>
-        <v/>
-      </c>
-      <c r="H8" s="137">
-        <f>ETPT_CA_JUR!H8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I8),"",IF(ETPT_CA_JUR!I8=0,"",ETPT_CA_JUR!I8)))</f>
-        <v/>
-      </c>
-      <c r="J8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J8),"",IF(ETPT_CA_JUR!J8=0,"",ETPT_CA_JUR!J8)))</f>
-        <v/>
-      </c>
-      <c r="K8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K8),"",IF(ETPT_CA_JUR!K8=0,"",ETPT_CA_JUR!K8)))</f>
-        <v/>
-      </c>
-      <c r="L8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L8),"",IF(ETPT_CA_JUR!L8=0,"",ETPT_CA_JUR!L8)))</f>
-        <v/>
-      </c>
-      <c r="M8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M8),"",IF(ETPT_CA_JUR!M8=0,"",ETPT_CA_JUR!M8)))</f>
-        <v/>
-      </c>
-      <c r="N8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N8),"",IF(ETPT_CA_JUR!N8=0,"",ETPT_CA_JUR!N8)))</f>
-        <v/>
-      </c>
-      <c r="O8" s="137">
-        <f>ETPT_CA_JUR!O8</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P8),"",IF(ETPT_CA_JUR!P8=0,"",ETPT_CA_JUR!P8)))</f>
-        <v/>
-      </c>
-      <c r="Q8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q8),"",IF(ETPT_CA_JUR!Q8=0,"",ETPT_CA_JUR!Q8)))</f>
-        <v/>
-      </c>
-      <c r="R8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R8),"",IF(ETPT_CA_JUR!R8=0,"",ETPT_CA_JUR!R8)))</f>
-        <v/>
-      </c>
-      <c r="S8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S8),"",IF(ETPT_CA_JUR!S8=0,"",ETPT_CA_JUR!S8)))</f>
-        <v/>
-      </c>
-      <c r="T8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T8),"",IF(ETPT_CA_JUR!T8=0,"",ETPT_CA_JUR!T8)))</f>
-        <v/>
-      </c>
-      <c r="U8" s="137">
-        <f>ETPT_CA_JUR!U8</f>
-        <v>0</v>
-      </c>
-      <c r="V8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V8),"",IF(ETPT_CA_JUR!V8=0,"",ETPT_CA_JUR!V8)))</f>
-        <v/>
-      </c>
-      <c r="W8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W8),"",IF(ETPT_CA_JUR!W8=0,"",ETPT_CA_JUR!W8)))</f>
-        <v/>
-      </c>
-      <c r="X8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X8),"",IF(ETPT_CA_JUR!X8=0,"",ETPT_CA_JUR!X8)))</f>
-        <v/>
-      </c>
-      <c r="Y8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y8),"",IF(ETPT_CA_JUR!Y8=0,"",ETPT_CA_JUR!Y8)))</f>
-        <v/>
-      </c>
-      <c r="Z8" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z8),"",IF(ETPT_CA_JUR!Z8=0,"",ETPT_CA_JUR!Z8)))</f>
-        <v/>
-      </c>
-      <c r="AA8" s="137">
-        <f>ETPT_CA_JUR!AA8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="E9" s="96" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="96" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G9),"",IF(ETPT_CA_JUR!G9=0,"",ETPT_CA_JUR!G9)))</f>
-        <v/>
-      </c>
-      <c r="H9" s="137">
-        <f>ETPT_CA_JUR!H9</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I9),"",IF(ETPT_CA_JUR!I9=0,"",ETPT_CA_JUR!I9)))</f>
-        <v/>
-      </c>
-      <c r="J9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J9),"",IF(ETPT_CA_JUR!J9=0,"",ETPT_CA_JUR!J9)))</f>
-        <v/>
-      </c>
-      <c r="K9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K9),"",IF(ETPT_CA_JUR!K9=0,"",ETPT_CA_JUR!K9)))</f>
-        <v/>
-      </c>
-      <c r="L9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L9),"",IF(ETPT_CA_JUR!L9=0,"",ETPT_CA_JUR!L9)))</f>
-        <v/>
-      </c>
-      <c r="M9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M9),"",IF(ETPT_CA_JUR!M9=0,"",ETPT_CA_JUR!M9)))</f>
-        <v/>
-      </c>
-      <c r="N9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N9),"",IF(ETPT_CA_JUR!N9=0,"",ETPT_CA_JUR!N9)))</f>
-        <v/>
-      </c>
-      <c r="O9" s="137">
-        <f>ETPT_CA_JUR!O9</f>
-        <v>0</v>
-      </c>
-      <c r="P9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P9),"",IF(ETPT_CA_JUR!P9=0,"",ETPT_CA_JUR!P9)))</f>
-        <v/>
-      </c>
-      <c r="Q9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q9),"",IF(ETPT_CA_JUR!Q9=0,"",ETPT_CA_JUR!Q9)))</f>
-        <v/>
-      </c>
-      <c r="R9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R9),"",IF(ETPT_CA_JUR!R9=0,"",ETPT_CA_JUR!R9)))</f>
-        <v/>
-      </c>
-      <c r="S9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S9),"",IF(ETPT_CA_JUR!S9=0,"",ETPT_CA_JUR!S9)))</f>
-        <v/>
-      </c>
-      <c r="T9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T9),"",IF(ETPT_CA_JUR!T9=0,"",ETPT_CA_JUR!T9)))</f>
-        <v/>
-      </c>
-      <c r="U9" s="137">
-        <f>ETPT_CA_JUR!U9</f>
-        <v>0</v>
-      </c>
-      <c r="V9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V9),"",IF(ETPT_CA_JUR!V9=0,"",ETPT_CA_JUR!V9)))</f>
-        <v/>
-      </c>
-      <c r="W9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W9),"",IF(ETPT_CA_JUR!W9=0,"",ETPT_CA_JUR!W9)))</f>
-        <v/>
-      </c>
-      <c r="X9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X9),"",IF(ETPT_CA_JUR!X9=0,"",ETPT_CA_JUR!X9)))</f>
-        <v/>
-      </c>
-      <c r="Y9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y9),"",IF(ETPT_CA_JUR!Y9=0,"",ETPT_CA_JUR!Y9)))</f>
-        <v/>
-      </c>
-      <c r="Z9" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z9),"",IF(ETPT_CA_JUR!Z9=0,"",ETPT_CA_JUR!Z9)))</f>
-        <v/>
-      </c>
-      <c r="AA9" s="137">
-        <f>ETPT_CA_JUR!AA9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="E10" s="96" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="96" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G10),"",IF(ETPT_CA_JUR!G10=0,"",ETPT_CA_JUR!G10)))</f>
-        <v/>
-      </c>
-      <c r="H10" s="137">
-        <f>ETPT_CA_JUR!H10</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I10),"",IF(ETPT_CA_JUR!I10=0,"",ETPT_CA_JUR!I10)))</f>
-        <v/>
-      </c>
-      <c r="J10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J10),"",IF(ETPT_CA_JUR!J10=0,"",ETPT_CA_JUR!J10)))</f>
-        <v/>
-      </c>
-      <c r="K10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K10),"",IF(ETPT_CA_JUR!K10=0,"",ETPT_CA_JUR!K10)))</f>
-        <v/>
-      </c>
-      <c r="L10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L10),"",IF(ETPT_CA_JUR!L10=0,"",ETPT_CA_JUR!L10)))</f>
-        <v/>
-      </c>
-      <c r="M10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M10),"",IF(ETPT_CA_JUR!M10=0,"",ETPT_CA_JUR!M10)))</f>
-        <v/>
-      </c>
-      <c r="N10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N10),"",IF(ETPT_CA_JUR!N10=0,"",ETPT_CA_JUR!N10)))</f>
-        <v/>
-      </c>
-      <c r="O10" s="137">
-        <f>ETPT_CA_JUR!O10</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P10),"",IF(ETPT_CA_JUR!P10=0,"",ETPT_CA_JUR!P10)))</f>
-        <v/>
-      </c>
-      <c r="Q10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q10),"",IF(ETPT_CA_JUR!Q10=0,"",ETPT_CA_JUR!Q10)))</f>
-        <v/>
-      </c>
-      <c r="R10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R10),"",IF(ETPT_CA_JUR!R10=0,"",ETPT_CA_JUR!R10)))</f>
-        <v/>
-      </c>
-      <c r="S10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S10),"",IF(ETPT_CA_JUR!S10=0,"",ETPT_CA_JUR!S10)))</f>
-        <v/>
-      </c>
-      <c r="T10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T10),"",IF(ETPT_CA_JUR!T10=0,"",ETPT_CA_JUR!T10)))</f>
-        <v/>
-      </c>
-      <c r="U10" s="137">
-        <f>ETPT_CA_JUR!U10</f>
-        <v>0</v>
-      </c>
-      <c r="V10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V10),"",IF(ETPT_CA_JUR!V10=0,"",ETPT_CA_JUR!V10)))</f>
-        <v/>
-      </c>
-      <c r="W10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W10),"",IF(ETPT_CA_JUR!W10=0,"",ETPT_CA_JUR!W10)))</f>
-        <v/>
-      </c>
-      <c r="X10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X10),"",IF(ETPT_CA_JUR!X10=0,"",ETPT_CA_JUR!X10)))</f>
-        <v/>
-      </c>
-      <c r="Y10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y10),"",IF(ETPT_CA_JUR!Y10=0,"",ETPT_CA_JUR!Y10)))</f>
-        <v/>
-      </c>
-      <c r="Z10" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z10),"",IF(ETPT_CA_JUR!Z10=0,"",ETPT_CA_JUR!Z10)))</f>
-        <v/>
-      </c>
-      <c r="AA10" s="137">
-        <f>ETPT_CA_JUR!AA10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A11" s="42"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="E11" s="96" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="96" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G11),"",IF(ETPT_CA_JUR!G11=0,"",ETPT_CA_JUR!G11)))</f>
-        <v/>
-      </c>
-      <c r="H11" s="137">
-        <f>ETPT_CA_JUR!H11</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I11),"",IF(ETPT_CA_JUR!I11=0,"",ETPT_CA_JUR!I11)))</f>
-        <v/>
-      </c>
-      <c r="J11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J11),"",IF(ETPT_CA_JUR!J11=0,"",ETPT_CA_JUR!J11)))</f>
-        <v/>
-      </c>
-      <c r="K11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K11),"",IF(ETPT_CA_JUR!K11=0,"",ETPT_CA_JUR!K11)))</f>
-        <v/>
-      </c>
-      <c r="L11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L11),"",IF(ETPT_CA_JUR!L11=0,"",ETPT_CA_JUR!L11)))</f>
-        <v/>
-      </c>
-      <c r="M11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M11),"",IF(ETPT_CA_JUR!M11=0,"",ETPT_CA_JUR!M11)))</f>
-        <v/>
-      </c>
-      <c r="N11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N11),"",IF(ETPT_CA_JUR!N11=0,"",ETPT_CA_JUR!N11)))</f>
-        <v/>
-      </c>
-      <c r="O11" s="137">
-        <f>ETPT_CA_JUR!O11</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P11),"",IF(ETPT_CA_JUR!P11=0,"",ETPT_CA_JUR!P11)))</f>
-        <v/>
-      </c>
-      <c r="Q11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q11),"",IF(ETPT_CA_JUR!Q11=0,"",ETPT_CA_JUR!Q11)))</f>
-        <v/>
-      </c>
-      <c r="R11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R11),"",IF(ETPT_CA_JUR!R11=0,"",ETPT_CA_JUR!R11)))</f>
-        <v/>
-      </c>
-      <c r="S11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S11),"",IF(ETPT_CA_JUR!S11=0,"",ETPT_CA_JUR!S11)))</f>
-        <v/>
-      </c>
-      <c r="T11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T11),"",IF(ETPT_CA_JUR!T11=0,"",ETPT_CA_JUR!T11)))</f>
-        <v/>
-      </c>
-      <c r="U11" s="137">
-        <f>ETPT_CA_JUR!U11</f>
-        <v>0</v>
-      </c>
-      <c r="V11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V11),"",IF(ETPT_CA_JUR!V11=0,"",ETPT_CA_JUR!V11)))</f>
-        <v/>
-      </c>
-      <c r="W11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W11),"",IF(ETPT_CA_JUR!W11=0,"",ETPT_CA_JUR!W11)))</f>
-        <v/>
-      </c>
-      <c r="X11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X11),"",IF(ETPT_CA_JUR!X11=0,"",ETPT_CA_JUR!X11)))</f>
-        <v/>
-      </c>
-      <c r="Y11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y11),"",IF(ETPT_CA_JUR!Y11=0,"",ETPT_CA_JUR!Y11)))</f>
-        <v/>
-      </c>
-      <c r="Z11" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z11),"",IF(ETPT_CA_JUR!Z11=0,"",ETPT_CA_JUR!Z11)))</f>
-        <v/>
-      </c>
-      <c r="AA11" s="137">
-        <f>ETPT_CA_JUR!AA11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="E12" s="96" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="96" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G12),"",IF(ETPT_CA_JUR!G12=0,"",ETPT_CA_JUR!G12)))</f>
-        <v/>
-      </c>
-      <c r="H12" s="137">
-        <f>ETPT_CA_JUR!H12</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I12),"",IF(ETPT_CA_JUR!I12=0,"",ETPT_CA_JUR!I12)))</f>
-        <v/>
-      </c>
-      <c r="J12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J12),"",IF(ETPT_CA_JUR!J12=0,"",ETPT_CA_JUR!J12)))</f>
-        <v/>
-      </c>
-      <c r="K12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K12),"",IF(ETPT_CA_JUR!K12=0,"",ETPT_CA_JUR!K12)))</f>
-        <v/>
-      </c>
-      <c r="L12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L12),"",IF(ETPT_CA_JUR!L12=0,"",ETPT_CA_JUR!L12)))</f>
-        <v/>
-      </c>
-      <c r="M12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M12),"",IF(ETPT_CA_JUR!M12=0,"",ETPT_CA_JUR!M12)))</f>
-        <v/>
-      </c>
-      <c r="N12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N12),"",IF(ETPT_CA_JUR!N12=0,"",ETPT_CA_JUR!N12)))</f>
-        <v/>
-      </c>
-      <c r="O12" s="137">
-        <f>ETPT_CA_JUR!O12</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P12),"",IF(ETPT_CA_JUR!P12=0,"",ETPT_CA_JUR!P12)))</f>
-        <v/>
-      </c>
-      <c r="Q12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q12),"",IF(ETPT_CA_JUR!Q12=0,"",ETPT_CA_JUR!Q12)))</f>
-        <v/>
-      </c>
-      <c r="R12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R12),"",IF(ETPT_CA_JUR!R12=0,"",ETPT_CA_JUR!R12)))</f>
-        <v/>
-      </c>
-      <c r="S12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S12),"",IF(ETPT_CA_JUR!S12=0,"",ETPT_CA_JUR!S12)))</f>
-        <v/>
-      </c>
-      <c r="T12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T12),"",IF(ETPT_CA_JUR!T12=0,"",ETPT_CA_JUR!T12)))</f>
-        <v/>
-      </c>
-      <c r="U12" s="137">
-        <f>ETPT_CA_JUR!U12</f>
-        <v>0</v>
-      </c>
-      <c r="V12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V12),"",IF(ETPT_CA_JUR!V12=0,"",ETPT_CA_JUR!V12)))</f>
-        <v/>
-      </c>
-      <c r="W12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W12),"",IF(ETPT_CA_JUR!W12=0,"",ETPT_CA_JUR!W12)))</f>
-        <v/>
-      </c>
-      <c r="X12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X12),"",IF(ETPT_CA_JUR!X12=0,"",ETPT_CA_JUR!X12)))</f>
-        <v/>
-      </c>
-      <c r="Y12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y12),"",IF(ETPT_CA_JUR!Y12=0,"",ETPT_CA_JUR!Y12)))</f>
-        <v/>
-      </c>
-      <c r="Z12" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z12),"",IF(ETPT_CA_JUR!Z12=0,"",ETPT_CA_JUR!Z12)))</f>
-        <v/>
-      </c>
-      <c r="AA12" s="137">
-        <f>ETPT_CA_JUR!AA12</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D13" s="38" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="E13" s="96" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="96" t="s">
-        <v>115</v>
-      </c>
-      <c r="G13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G13),"",IF(ETPT_CA_JUR!G13=0,"",ETPT_CA_JUR!G13)))</f>
-        <v/>
-      </c>
-      <c r="H13" s="137">
-        <f>ETPT_CA_JUR!H13</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I13),"",IF(ETPT_CA_JUR!I13=0,"",ETPT_CA_JUR!I13)))</f>
-        <v/>
-      </c>
-      <c r="J13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J13),"",IF(ETPT_CA_JUR!J13=0,"",ETPT_CA_JUR!J13)))</f>
-        <v/>
-      </c>
-      <c r="K13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K13),"",IF(ETPT_CA_JUR!K13=0,"",ETPT_CA_JUR!K13)))</f>
-        <v/>
-      </c>
-      <c r="L13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L13),"",IF(ETPT_CA_JUR!L13=0,"",ETPT_CA_JUR!L13)))</f>
-        <v/>
-      </c>
-      <c r="M13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M13),"",IF(ETPT_CA_JUR!M13=0,"",ETPT_CA_JUR!M13)))</f>
-        <v/>
-      </c>
-      <c r="N13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N13),"",IF(ETPT_CA_JUR!N13=0,"",ETPT_CA_JUR!N13)))</f>
-        <v/>
-      </c>
-      <c r="O13" s="137">
-        <f>ETPT_CA_JUR!O13</f>
-        <v>0</v>
-      </c>
-      <c r="P13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P13),"",IF(ETPT_CA_JUR!P13=0,"",ETPT_CA_JUR!P13)))</f>
-        <v/>
-      </c>
-      <c r="Q13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q13),"",IF(ETPT_CA_JUR!Q13=0,"",ETPT_CA_JUR!Q13)))</f>
-        <v/>
-      </c>
-      <c r="R13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R13),"",IF(ETPT_CA_JUR!R13=0,"",ETPT_CA_JUR!R13)))</f>
-        <v/>
-      </c>
-      <c r="S13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S13),"",IF(ETPT_CA_JUR!S13=0,"",ETPT_CA_JUR!S13)))</f>
-        <v/>
-      </c>
-      <c r="T13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T13),"",IF(ETPT_CA_JUR!T13=0,"",ETPT_CA_JUR!T13)))</f>
-        <v/>
-      </c>
-      <c r="U13" s="137">
-        <f>ETPT_CA_JUR!U13</f>
-        <v>0</v>
-      </c>
-      <c r="V13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V13),"",IF(ETPT_CA_JUR!V13=0,"",ETPT_CA_JUR!V13)))</f>
-        <v/>
-      </c>
-      <c r="W13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W13),"",IF(ETPT_CA_JUR!W13=0,"",ETPT_CA_JUR!W13)))</f>
-        <v/>
-      </c>
-      <c r="X13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X13),"",IF(ETPT_CA_JUR!X13=0,"",ETPT_CA_JUR!X13)))</f>
-        <v/>
-      </c>
-      <c r="Y13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y13),"",IF(ETPT_CA_JUR!Y13=0,"",ETPT_CA_JUR!Y13)))</f>
-        <v/>
-      </c>
-      <c r="Z13" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z13),"",IF(ETPT_CA_JUR!Z13=0,"",ETPT_CA_JUR!Z13)))</f>
-        <v/>
-      </c>
-      <c r="AA13" s="137">
-        <f>ETPT_CA_JUR!AA13</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D14" s="38" t="str">
-        <f>IF(ISBLANK($D$3),"",$D$3)</f>
-        <v>A</v>
-      </c>
-      <c r="E14" s="96" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="96" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G14),"",IF(ETPT_CA_JUR!G14=0,"",ETPT_CA_JUR!G14)))</f>
-        <v/>
-      </c>
-      <c r="H14" s="137">
-        <f>ETPT_CA_JUR!H14</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!I14),"",IF(ETPT_CA_JUR!I14=0,"",ETPT_CA_JUR!I14)))</f>
-        <v/>
-      </c>
-      <c r="J14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!J14),"",IF(ETPT_CA_JUR!J14=0,"",ETPT_CA_JUR!J14)))</f>
-        <v/>
-      </c>
-      <c r="K14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!K14),"",IF(ETPT_CA_JUR!K14=0,"",ETPT_CA_JUR!K14)))</f>
-        <v/>
-      </c>
-      <c r="L14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!L14),"",IF(ETPT_CA_JUR!L14=0,"",ETPT_CA_JUR!L14)))</f>
-        <v/>
-      </c>
-      <c r="M14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!M14),"",IF(ETPT_CA_JUR!M14=0,"",ETPT_CA_JUR!M14)))</f>
-        <v/>
-      </c>
-      <c r="N14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N14),"",IF(ETPT_CA_JUR!N14=0,"",ETPT_CA_JUR!N14)))</f>
-        <v/>
-      </c>
-      <c r="O14" s="137">
-        <f>ETPT_CA_JUR!O14</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!P14),"",IF(ETPT_CA_JUR!P14=0,"",ETPT_CA_JUR!P14)))</f>
-        <v/>
-      </c>
-      <c r="Q14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Q14),"",IF(ETPT_CA_JUR!Q14=0,"",ETPT_CA_JUR!Q14)))</f>
-        <v/>
-      </c>
-      <c r="R14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!R14),"",IF(ETPT_CA_JUR!R14=0,"",ETPT_CA_JUR!R14)))</f>
-        <v/>
-      </c>
-      <c r="S14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!S14),"",IF(ETPT_CA_JUR!S14=0,"",ETPT_CA_JUR!S14)))</f>
-        <v/>
-      </c>
-      <c r="T14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!T14),"",IF(ETPT_CA_JUR!T14=0,"",ETPT_CA_JUR!T14)))</f>
-        <v/>
-      </c>
-      <c r="U14" s="137">
-        <f>ETPT_CA_JUR!U14</f>
-        <v>0</v>
-      </c>
-      <c r="V14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!V14),"",IF(ETPT_CA_JUR!V14=0,"",ETPT_CA_JUR!V14)))</f>
-        <v/>
-      </c>
-      <c r="W14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!W14),"",IF(ETPT_CA_JUR!W14=0,"",ETPT_CA_JUR!W14)))</f>
-        <v/>
-      </c>
-      <c r="X14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!X14),"",IF(ETPT_CA_JUR!X14=0,"",ETPT_CA_JUR!X14)))</f>
-        <v/>
-      </c>
-      <c r="Y14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Y14),"",IF(ETPT_CA_JUR!Y14=0,"",ETPT_CA_JUR!Y14)))</f>
-        <v/>
-      </c>
-      <c r="Z14" s="136" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!Z14),"",IF(ETPT_CA_JUR!Z14=0,"",ETPT_CA_JUR!Z14)))</f>
-        <v/>
-      </c>
-      <c r="AA14" s="137">
-        <f>ETPT_CA_JUR!AA14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D15" s="38"/>
-      <c r="E15" s="97"/>
-      <c r="F15" s="98" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="137">
-        <f>ETPT_CA_JUR!G15</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="137">
-        <f>ETPT_CA_JUR!H15</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="137">
-        <f>ETPT_CA_JUR!I15</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="137">
-        <f>ETPT_CA_JUR!J15</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="137">
-        <f>ETPT_CA_JUR!K15</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="137">
-        <f>ETPT_CA_JUR!L15</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="137">
-        <f>ETPT_CA_JUR!M15</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="137">
-        <f>ETPT_CA_JUR!N15</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="137">
-        <f>ETPT_CA_JUR!O15</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="137">
-        <f>ETPT_CA_JUR!P15</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="137">
-        <f>ETPT_CA_JUR!Q15</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="137">
-        <f>ETPT_CA_JUR!R15</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="137">
-        <f>ETPT_CA_JUR!S15</f>
-        <v>0</v>
-      </c>
-      <c r="T15" s="137">
-        <f>ETPT_CA_JUR!T15</f>
-        <v>0</v>
-      </c>
-      <c r="U15" s="137">
-        <f>ETPT_CA_JUR!U15</f>
-        <v>0</v>
-      </c>
-      <c r="V15" s="137">
-        <f>ETPT_CA_JUR!V15</f>
-        <v>0</v>
-      </c>
-      <c r="W15" s="137">
-        <f>ETPT_CA_JUR!W15</f>
-        <v>0</v>
-      </c>
-      <c r="X15" s="137">
-        <f>ETPT_CA_JUR!X15</f>
-        <v>0</v>
-      </c>
-      <c r="Y15" s="137">
-        <f>ETPT_CA_JUR!Y15</f>
-        <v>0</v>
-      </c>
-      <c r="Z15" s="137">
-        <f>ETPT_CA_JUR!Z15</f>
-        <v>0</v>
-      </c>
-      <c r="AA15" s="137">
-        <f>ETPT_CA_JUR!AA15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="D16" s="134"/>
-      <c r="E16" s="134"/>
-      <c r="F16" s="134"/>
-      <c r="G16" s="138"/>
-      <c r="H16" s="138"/>
-      <c r="I16" s="138"/>
-      <c r="J16" s="138"/>
-      <c r="K16" s="138"/>
-      <c r="L16" s="138"/>
-      <c r="M16" s="138"/>
-      <c r="N16" s="138"/>
-      <c r="O16" s="138"/>
-      <c r="P16" s="138"/>
-      <c r="Q16" s="138"/>
-      <c r="R16" s="138"/>
-      <c r="S16" s="138"/>
-      <c r="T16" s="138"/>
-      <c r="U16" s="138"/>
-      <c r="V16" s="138"/>
-      <c r="W16" s="138"/>
-      <c r="X16" s="138"/>
-      <c r="Y16" s="138"/>
-      <c r="Z16" s="138"/>
-      <c r="AA16" s="138"/>
-    </row>
-    <row r="17" spans="1:27" ht="24" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17"/>
-      <c r="C17"/>
-      <c r="D17" s="135"/>
-      <c r="E17" s="135"/>
-      <c r="F17" s="151" t="s">
-        <v>118</v>
-      </c>
-      <c r="G17" s="140" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!G17),"",IF(ETPT_CA_JUR!G17=0,"",ETPT_CA_JUR!G17)))</f>
-        <v/>
-      </c>
-      <c r="H17" s="139"/>
-      <c r="I17" s="191" t="s">
-        <v>119</v>
-      </c>
-      <c r="J17" s="192"/>
-      <c r="K17" s="192"/>
-      <c r="L17" s="192"/>
-      <c r="M17" s="193"/>
-      <c r="N17" s="140" t="str">
-        <f>IF(ISBLANK($D$3),"",IF(ISERROR(ETPT_CA_JUR!N17),"",IF(ETPT_CA_JUR!N17=0,"",ETPT_CA_JUR!N17)))</f>
-        <v/>
-      </c>
-      <c r="O17" s="139"/>
-      <c r="P17" s="139"/>
-      <c r="Q17" s="139"/>
-      <c r="R17" s="139"/>
-      <c r="S17" s="139"/>
-      <c r="T17" s="139"/>
-      <c r="U17" s="139"/>
-      <c r="V17" s="139"/>
-      <c r="W17" s="139"/>
-      <c r="X17" s="139"/>
-      <c r="Y17" s="139"/>
-      <c r="Z17" s="139"/>
-      <c r="AA17" s="139"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I17:M17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed column attachés de justice pole social
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FF5B65-4CCB-0146-B631-893451DE7F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D538FE4D-8930-3241-8D4E-243D5280FA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30240" windowHeight="17680" activeTab="10" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Table_Fonctions" sheetId="19" state="hidden" r:id="rId8"/>
     <sheet name="ETPT_CA_ATTJ" sheetId="30" state="hidden" r:id="rId9"/>
     <sheet name="ETPT_CA_ATTJ_DDG" sheetId="25" r:id="rId10"/>
-    <sheet name="ETPT_ATTACHES_JUSTICE" sheetId="41" state="hidden" r:id="rId11"/>
+    <sheet name="ETPT_ATTACHES_JUSTICE" sheetId="41" r:id="rId11"/>
     <sheet name="ETPT_ATTACHES_JUSTICE_DDG" sheetId="42" r:id="rId12"/>
     <sheet name="ETPT_CA_JUR Corresp" sheetId="38" state="hidden" r:id="rId13"/>
     <sheet name="ETPT_ATTACHES_JUSTICE Corresp" sheetId="43" state="hidden" r:id="rId14"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="341">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -4829,16 +4829,6 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
@@ -5032,6 +5022,16 @@
       <font>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5886,7 +5886,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:F13"/>
     </sheetView>
   </sheetViews>
@@ -7615,20 +7615,20 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="73.83203125" customWidth="1"/>
-    <col min="4" max="16" width="23.6640625" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+    <col min="4" max="15" width="23.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="74" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="74" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>120</v>
       </c>
@@ -7649,9 +7649,8 @@
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="108" t="s">
         <v>32</v>
       </c>
@@ -7686,23 +7685,20 @@
         <v>334</v>
       </c>
       <c r="L2" s="99" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M2" s="99" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N2" s="99" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="O2" s="99" t="s">
-        <v>339</v>
-      </c>
-      <c r="P2" s="99" t="s">
         <v>335</v>
       </c>
-      <c r="Q2" s="128"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P2" s="128"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="117" t="s">
         <v>129</v>
       </c>
@@ -7794,12 +7790,12 @@
       </c>
       <c r="J3" s="207"/>
       <c r="K3" s="207"/>
-      <c r="Q3" s="114">
-        <f>_xlfn.AGGREGATE(9,6,D3:P3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P3" s="114">
+        <f>_xlfn.AGGREGATE(9,6,D3:O3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="117" t="s">
         <v>190</v>
       </c>
@@ -7879,12 +7875,12 @@
       </c>
       <c r="J4" s="207"/>
       <c r="K4" s="207"/>
-      <c r="Q4" s="114">
-        <f>_xlfn.AGGREGATE(9,6,D4:P4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P4" s="114">
+        <f>_xlfn.AGGREGATE(9,6,D4:O4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="117" t="s">
         <v>191</v>
       </c>
@@ -7922,12 +7918,12 @@
       </c>
       <c r="J5" s="207"/>
       <c r="K5" s="207"/>
-      <c r="Q5" s="114">
-        <f>_xlfn.AGGREGATE(9,6,D5:P5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P5" s="114">
+        <f>_xlfn.AGGREGATE(9,6,D5:O5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="117" t="s">
         <v>192</v>
       </c>
@@ -8061,12 +8057,12 @@
       </c>
       <c r="J6" s="207"/>
       <c r="K6" s="207"/>
-      <c r="Q6" s="114">
-        <f>_xlfn.AGGREGATE(9,6,D6:P6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P6" s="114">
+        <f>_xlfn.AGGREGATE(9,6,D6:O6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="117" t="s">
         <v>193</v>
       </c>
@@ -8104,12 +8100,12 @@
       </c>
       <c r="J7" s="207"/>
       <c r="K7" s="207"/>
-      <c r="Q7" s="114">
-        <f>_xlfn.AGGREGATE(9,6,D7:P7)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P7" s="114">
+        <f>_xlfn.AGGREGATE(9,6,D7:O7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="117" t="s">
         <v>194</v>
       </c>
@@ -8147,12 +8143,12 @@
       </c>
       <c r="J8" s="207"/>
       <c r="K8" s="207"/>
-      <c r="Q8" s="114">
-        <f>_xlfn.AGGREGATE(9,6,D8:P8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P8" s="114">
+        <f>_xlfn.AGGREGATE(9,6,D8:O8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="117" t="s">
         <v>195</v>
       </c>
@@ -8202,12 +8198,12 @@
       </c>
       <c r="J9" s="207"/>
       <c r="K9" s="207"/>
-      <c r="Q9" s="114">
-        <f>_xlfn.AGGREGATE(9,6,D9:P9)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P9" s="114">
+        <f>_xlfn.AGGREGATE(9,6,D9:O9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="117" t="s">
         <v>196</v>
       </c>
@@ -8245,12 +8241,12 @@
       </c>
       <c r="J10" s="207"/>
       <c r="K10" s="207"/>
-      <c r="Q10" s="114">
-        <f>_xlfn.AGGREGATE(9,6,D10:P10)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P10" s="114">
+        <f>_xlfn.AGGREGATE(9,6,D10:O10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C11" s="115" t="s">
         <v>37</v>
       </c>
@@ -8259,7 +8255,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="114">
-        <f t="shared" ref="E11:P11" si="0">_xlfn.AGGREGATE(9,6,E3:E10)</f>
+        <f t="shared" ref="E11:O11" si="0">_xlfn.AGGREGATE(9,6,E3:E10)</f>
         <v>0</v>
       </c>
       <c r="F11" s="114">
@@ -8303,11 +8299,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="114">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="114">
-        <f>_xlfn.AGGREGATE(9,6,Q3:Q10)</f>
+        <f>_xlfn.AGGREGATE(9,6,P3:P10)</f>
         <v>0</v>
       </c>
     </row>
@@ -8325,15 +8317,17 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="59.83203125" customWidth="1"/>
-    <col min="4" max="16" width="20.1640625" customWidth="1"/>
+    <col min="4" max="11" width="20.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" hidden="1" customWidth="1"/>
+    <col min="13" max="16" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="87" customHeight="1" x14ac:dyDescent="0.25">
@@ -8442,27 +8436,27 @@
       <c r="J3" s="135"/>
       <c r="K3" s="135"/>
       <c r="L3" s="135" t="str">
+        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!#REF!),"",IF(ETPT_ATTACHES_JUSTICE!#REF!=0,"",ETPT_ATTACHES_JUSTICE!#REF!))</f>
+        <v/>
+      </c>
+      <c r="M3" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!L3),"",IF(ETPT_ATTACHES_JUSTICE!L3=0,"",ETPT_ATTACHES_JUSTICE!L3))</f>
         <v/>
       </c>
-      <c r="M3" s="135" t="str">
+      <c r="N3" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!M3),"",IF(ETPT_ATTACHES_JUSTICE!M3=0,"",ETPT_ATTACHES_JUSTICE!M3))</f>
         <v/>
       </c>
-      <c r="N3" s="135" t="str">
+      <c r="O3" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!N3),"",IF(ETPT_ATTACHES_JUSTICE!N3=0,"",ETPT_ATTACHES_JUSTICE!N3))</f>
         <v/>
       </c>
-      <c r="O3" s="135" t="str">
+      <c r="P3" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!O3),"",IF(ETPT_ATTACHES_JUSTICE!O3=0,"",ETPT_ATTACHES_JUSTICE!O3))</f>
         <v/>
       </c>
-      <c r="P3" s="135" t="str">
-        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!P3),"",IF(ETPT_ATTACHES_JUSTICE!P3=0,"",ETPT_ATTACHES_JUSTICE!P3))</f>
-        <v/>
-      </c>
       <c r="Q3" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q3</f>
+        <f>ETPT_ATTACHES_JUSTICE!P3</f>
         <v>0</v>
       </c>
     </row>
@@ -8498,27 +8492,27 @@
       <c r="J4" s="135"/>
       <c r="K4" s="135"/>
       <c r="L4" s="135" t="str">
+        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!#REF!),"",IF(ETPT_ATTACHES_JUSTICE!#REF!=0,"",ETPT_ATTACHES_JUSTICE!#REF!))</f>
+        <v/>
+      </c>
+      <c r="M4" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!L4),"",IF(ETPT_ATTACHES_JUSTICE!L4=0,"",ETPT_ATTACHES_JUSTICE!L4))</f>
         <v/>
       </c>
-      <c r="M4" s="135" t="str">
+      <c r="N4" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!M4),"",IF(ETPT_ATTACHES_JUSTICE!M4=0,"",ETPT_ATTACHES_JUSTICE!M4))</f>
         <v/>
       </c>
-      <c r="N4" s="135" t="str">
+      <c r="O4" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!N4),"",IF(ETPT_ATTACHES_JUSTICE!N4=0,"",ETPT_ATTACHES_JUSTICE!N4))</f>
         <v/>
       </c>
-      <c r="O4" s="135" t="str">
+      <c r="P4" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!O4),"",IF(ETPT_ATTACHES_JUSTICE!O4=0,"",ETPT_ATTACHES_JUSTICE!O4))</f>
         <v/>
       </c>
-      <c r="P4" s="135" t="str">
-        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!P4),"",IF(ETPT_ATTACHES_JUSTICE!P4=0,"",ETPT_ATTACHES_JUSTICE!P4))</f>
-        <v/>
-      </c>
       <c r="Q4" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q4</f>
+        <f>ETPT_ATTACHES_JUSTICE!P4</f>
         <v>0</v>
       </c>
     </row>
@@ -8554,27 +8548,27 @@
       <c r="J5" s="135"/>
       <c r="K5" s="135"/>
       <c r="L5" s="135" t="str">
+        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!#REF!),"",IF(ETPT_ATTACHES_JUSTICE!#REF!=0,"",ETPT_ATTACHES_JUSTICE!#REF!))</f>
+        <v/>
+      </c>
+      <c r="M5" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!L5),"",IF(ETPT_ATTACHES_JUSTICE!L5=0,"",ETPT_ATTACHES_JUSTICE!L5))</f>
         <v/>
       </c>
-      <c r="M5" s="135" t="str">
+      <c r="N5" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!M5),"",IF(ETPT_ATTACHES_JUSTICE!M5=0,"",ETPT_ATTACHES_JUSTICE!M5))</f>
         <v/>
       </c>
-      <c r="N5" s="135" t="str">
+      <c r="O5" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!N5),"",IF(ETPT_ATTACHES_JUSTICE!N5=0,"",ETPT_ATTACHES_JUSTICE!N5))</f>
         <v/>
       </c>
-      <c r="O5" s="135" t="str">
+      <c r="P5" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!O5),"",IF(ETPT_ATTACHES_JUSTICE!O5=0,"",ETPT_ATTACHES_JUSTICE!O5))</f>
         <v/>
       </c>
-      <c r="P5" s="135" t="str">
-        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!P5),"",IF(ETPT_ATTACHES_JUSTICE!P5=0,"",ETPT_ATTACHES_JUSTICE!P5))</f>
-        <v/>
-      </c>
       <c r="Q5" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q5</f>
+        <f>ETPT_ATTACHES_JUSTICE!P5</f>
         <v>0</v>
       </c>
     </row>
@@ -8610,27 +8604,27 @@
       <c r="J6" s="135"/>
       <c r="K6" s="135"/>
       <c r="L6" s="135" t="str">
+        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!#REF!),"",IF(ETPT_ATTACHES_JUSTICE!#REF!=0,"",ETPT_ATTACHES_JUSTICE!#REF!))</f>
+        <v/>
+      </c>
+      <c r="M6" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!L6),"",IF(ETPT_ATTACHES_JUSTICE!L6=0,"",ETPT_ATTACHES_JUSTICE!L6))</f>
         <v/>
       </c>
-      <c r="M6" s="135" t="str">
+      <c r="N6" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!M6),"",IF(ETPT_ATTACHES_JUSTICE!M6=0,"",ETPT_ATTACHES_JUSTICE!M6))</f>
         <v/>
       </c>
-      <c r="N6" s="135" t="str">
+      <c r="O6" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!N6),"",IF(ETPT_ATTACHES_JUSTICE!N6=0,"",ETPT_ATTACHES_JUSTICE!N6))</f>
         <v/>
       </c>
-      <c r="O6" s="135" t="str">
+      <c r="P6" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!O6),"",IF(ETPT_ATTACHES_JUSTICE!O6=0,"",ETPT_ATTACHES_JUSTICE!O6))</f>
         <v/>
       </c>
-      <c r="P6" s="135" t="str">
-        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!P6),"",IF(ETPT_ATTACHES_JUSTICE!P6=0,"",ETPT_ATTACHES_JUSTICE!P6))</f>
-        <v/>
-      </c>
       <c r="Q6" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q6</f>
+        <f>ETPT_ATTACHES_JUSTICE!P6</f>
         <v>0</v>
       </c>
     </row>
@@ -8666,27 +8660,27 @@
       <c r="J7" s="135"/>
       <c r="K7" s="135"/>
       <c r="L7" s="135" t="str">
+        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!#REF!),"",IF(ETPT_ATTACHES_JUSTICE!#REF!=0,"",ETPT_ATTACHES_JUSTICE!#REF!))</f>
+        <v/>
+      </c>
+      <c r="M7" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!L7),"",IF(ETPT_ATTACHES_JUSTICE!L7=0,"",ETPT_ATTACHES_JUSTICE!L7))</f>
         <v/>
       </c>
-      <c r="M7" s="135" t="str">
+      <c r="N7" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!M7),"",IF(ETPT_ATTACHES_JUSTICE!M7=0,"",ETPT_ATTACHES_JUSTICE!M7))</f>
         <v/>
       </c>
-      <c r="N7" s="135" t="str">
+      <c r="O7" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!N7),"",IF(ETPT_ATTACHES_JUSTICE!N7=0,"",ETPT_ATTACHES_JUSTICE!N7))</f>
         <v/>
       </c>
-      <c r="O7" s="135" t="str">
+      <c r="P7" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!O7),"",IF(ETPT_ATTACHES_JUSTICE!O7=0,"",ETPT_ATTACHES_JUSTICE!O7))</f>
         <v/>
       </c>
-      <c r="P7" s="135" t="str">
-        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!P7),"",IF(ETPT_ATTACHES_JUSTICE!P7=0,"",ETPT_ATTACHES_JUSTICE!P7))</f>
-        <v/>
-      </c>
       <c r="Q7" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q7</f>
+        <f>ETPT_ATTACHES_JUSTICE!P7</f>
         <v>0</v>
       </c>
     </row>
@@ -8722,27 +8716,27 @@
       <c r="J8" s="135"/>
       <c r="K8" s="135"/>
       <c r="L8" s="135" t="str">
+        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!#REF!),"",IF(ETPT_ATTACHES_JUSTICE!#REF!=0,"",ETPT_ATTACHES_JUSTICE!#REF!))</f>
+        <v/>
+      </c>
+      <c r="M8" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!L8),"",IF(ETPT_ATTACHES_JUSTICE!L8=0,"",ETPT_ATTACHES_JUSTICE!L8))</f>
         <v/>
       </c>
-      <c r="M8" s="135" t="str">
+      <c r="N8" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!M8),"",IF(ETPT_ATTACHES_JUSTICE!M8=0,"",ETPT_ATTACHES_JUSTICE!M8))</f>
         <v/>
       </c>
-      <c r="N8" s="135" t="str">
+      <c r="O8" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!N8),"",IF(ETPT_ATTACHES_JUSTICE!N8=0,"",ETPT_ATTACHES_JUSTICE!N8))</f>
         <v/>
       </c>
-      <c r="O8" s="135" t="str">
+      <c r="P8" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!O8),"",IF(ETPT_ATTACHES_JUSTICE!O8=0,"",ETPT_ATTACHES_JUSTICE!O8))</f>
         <v/>
       </c>
-      <c r="P8" s="135" t="str">
-        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!P8),"",IF(ETPT_ATTACHES_JUSTICE!P8=0,"",ETPT_ATTACHES_JUSTICE!P8))</f>
-        <v/>
-      </c>
       <c r="Q8" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q8</f>
+        <f>ETPT_ATTACHES_JUSTICE!P8</f>
         <v>0</v>
       </c>
     </row>
@@ -8778,27 +8772,27 @@
       <c r="J9" s="135"/>
       <c r="K9" s="135"/>
       <c r="L9" s="135" t="str">
+        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!#REF!),"",IF(ETPT_ATTACHES_JUSTICE!#REF!=0,"",ETPT_ATTACHES_JUSTICE!#REF!))</f>
+        <v/>
+      </c>
+      <c r="M9" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!L9),"",IF(ETPT_ATTACHES_JUSTICE!L9=0,"",ETPT_ATTACHES_JUSTICE!L9))</f>
         <v/>
       </c>
-      <c r="M9" s="135" t="str">
+      <c r="N9" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!M9),"",IF(ETPT_ATTACHES_JUSTICE!M9=0,"",ETPT_ATTACHES_JUSTICE!M9))</f>
         <v/>
       </c>
-      <c r="N9" s="135" t="str">
+      <c r="O9" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!N9),"",IF(ETPT_ATTACHES_JUSTICE!N9=0,"",ETPT_ATTACHES_JUSTICE!N9))</f>
         <v/>
       </c>
-      <c r="O9" s="135" t="str">
+      <c r="P9" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!O9),"",IF(ETPT_ATTACHES_JUSTICE!O9=0,"",ETPT_ATTACHES_JUSTICE!O9))</f>
         <v/>
       </c>
-      <c r="P9" s="135" t="str">
-        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!P9),"",IF(ETPT_ATTACHES_JUSTICE!P9=0,"",ETPT_ATTACHES_JUSTICE!P9))</f>
-        <v/>
-      </c>
       <c r="Q9" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q9</f>
+        <f>ETPT_ATTACHES_JUSTICE!P9</f>
         <v>0</v>
       </c>
     </row>
@@ -8834,27 +8828,27 @@
       <c r="J10" s="135"/>
       <c r="K10" s="135"/>
       <c r="L10" s="135" t="str">
+        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!#REF!),"",IF(ETPT_ATTACHES_JUSTICE!#REF!=0,"",ETPT_ATTACHES_JUSTICE!#REF!))</f>
+        <v/>
+      </c>
+      <c r="M10" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!L10),"",IF(ETPT_ATTACHES_JUSTICE!L10=0,"",ETPT_ATTACHES_JUSTICE!L10))</f>
         <v/>
       </c>
-      <c r="M10" s="135" t="str">
+      <c r="N10" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!M10),"",IF(ETPT_ATTACHES_JUSTICE!M10=0,"",ETPT_ATTACHES_JUSTICE!M10))</f>
         <v/>
       </c>
-      <c r="N10" s="135" t="str">
+      <c r="O10" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!N10),"",IF(ETPT_ATTACHES_JUSTICE!N10=0,"",ETPT_ATTACHES_JUSTICE!N10))</f>
         <v/>
       </c>
-      <c r="O10" s="135" t="str">
+      <c r="P10" s="135" t="str">
         <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!O10),"",IF(ETPT_ATTACHES_JUSTICE!O10=0,"",ETPT_ATTACHES_JUSTICE!O10))</f>
         <v/>
       </c>
-      <c r="P10" s="135" t="str">
-        <f>IF(ISERROR(ETPT_ATTACHES_JUSTICE!P10),"",IF(ETPT_ATTACHES_JUSTICE!P10=0,"",ETPT_ATTACHES_JUSTICE!P10))</f>
-        <v/>
-      </c>
       <c r="Q10" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q10</f>
+        <f>ETPT_ATTACHES_JUSTICE!P10</f>
         <v>0</v>
       </c>
     </row>
@@ -8896,28 +8890,28 @@
         <f>ETPT_ATTACHES_JUSTICE!K11</f>
         <v>0</v>
       </c>
-      <c r="L11" s="141">
+      <c r="L11" s="141" t="e">
+        <f>ETPT_ATTACHES_JUSTICE!#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M11" s="141">
         <f>ETPT_ATTACHES_JUSTICE!L11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="141">
+      <c r="N11" s="141">
         <f>ETPT_ATTACHES_JUSTICE!M11</f>
         <v>0</v>
       </c>
-      <c r="N11" s="141">
+      <c r="O11" s="141">
         <f>ETPT_ATTACHES_JUSTICE!N11</f>
         <v>0</v>
       </c>
-      <c r="O11" s="141">
+      <c r="P11" s="141">
         <f>ETPT_ATTACHES_JUSTICE!O11</f>
         <v>0</v>
       </c>
-      <c r="P11" s="141">
+      <c r="Q11" s="141">
         <f>ETPT_ATTACHES_JUSTICE!P11</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="141">
-        <f>ETPT_ATTACHES_JUSTICE!Q11</f>
         <v>0</v>
       </c>
     </row>
@@ -10796,7 +10790,7 @@
     <mergeCell ref="D1:Q1"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:EZ2 A3:FB1048576">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="2" stopIfTrue="1">
       <formula>OR(AND(OR($R1&lt;&gt;0,$S1&lt;&gt;0,$T1&lt;&gt;0,ISBLANK($P1)),ROW()&gt;2,$A1&lt;&gt;""),LEFT($I1,3)="JA ")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11114,57 +11108,57 @@
     <mergeCell ref="U4:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:F4">
-    <cfRule type="expression" dxfId="22" priority="20">
+    <cfRule type="expression" dxfId="21" priority="20">
       <formula>IF(LEFT($A$3,2)&lt;&gt;"TJ",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:F6 C7:V151">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1048576">
-    <cfRule type="expression" dxfId="20" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",OR(ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0,ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:F7">
-    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="17" stopIfTrue="1">
       <formula>OR(_xlfn.NUMBERVALUE($L6)&lt;&gt;_xlfn.NUMBERVALUE($L7),_xlfn.NUMBERVALUE($S6)&lt;&gt;_xlfn.NUMBERVALUE($S7),_xlfn.NUMBERVALUE($U6)&lt;&gt;_xlfn.NUMBERVALUE($U7))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:M1048576">
-    <cfRule type="expression" dxfId="18" priority="6">
+    <cfRule type="expression" dxfId="17" priority="6">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",ROUND(_xlfn.NUMBERVALUE($L1)-_xlfn.NUMBERVALUE($L2)-_xlfn.NUMBERVALUE($L3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:M7">
-    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($L7)&lt;&gt;_xlfn.NUMBERVALUE($L6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:V6">
-    <cfRule type="expression" dxfId="16" priority="7">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>AND(ISBLANK($C6)=FALSE,ISBLANK($E6)=TRUE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:T1048576">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",ROUND(_xlfn.NUMBERVALUE($S1)-_xlfn.NUMBERVALUE($S2)-_xlfn.NUMBERVALUE($S3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:T7">
-    <cfRule type="expression" dxfId="14" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>_xlfn.NUMBERVALUE($S7)&lt;&gt;_xlfn.NUMBERVALUE($S6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:V1048576">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>AND($D1="7. TOTAL CONTENTIEUX DES MINEURS",ROUND(_xlfn.NUMBERVALUE($U1)-_xlfn.NUMBERVALUE($U2)-_xlfn.NUMBERVALUE($U3),3)&lt;&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U7:V7">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>_xlfn.NUMBERVALUE($U7)&lt;&gt;_xlfn.NUMBERVALUE($U6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11349,57 +11343,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B1">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>AND(OR($I1&lt;&gt;"-",#REF!&lt;&gt;0,#REF!&lt;&gt;0,ISBLANK($M1)),ROW()&gt;2,$A1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:F2">
-    <cfRule type="expression" dxfId="10" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:N2">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:K2">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2">
-    <cfRule type="expression" dxfId="5" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:V2">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$F2="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:R2">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:T2">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>1=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11801,7 +11795,7 @@
   <dimension ref="A1:BF17"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="topRight" activeCell="AA11" sqref="AA11"/>
     </sheetView>

</xml_diff>

<commit_message>
chore: update template4CA.xlsx with dropdown changes
</commit_message>
<xml_diff>
--- a/front/src/assets/template4CA.xlsx
+++ b/front/src/assets/template4CA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinum-327809/Documents/a-just-dev/a-just/front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61E7D98-56A3-8046-80D8-C4C288796DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACA34D7-F6DA-E64A-8D56-65E7DB338BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="30220" windowHeight="15320" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="30220" windowHeight="15320" activeTab="11" xr2:uid="{50CB0F02-73D8-432D-BA19-0D33B1FE1838}"/>
   </bookViews>
   <sheets>
     <sheet name="ACCUEIL" sheetId="33" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="339">
   <si>
     <t>#! END_ROW</t>
   </si>
@@ -2719,9 +2719,6 @@
   </si>
   <si>
     <t>Contractuels A J Prox et A VIF au Parquet</t>
-  </si>
-  <si>
-    <t>Juristes assistants au parquet</t>
   </si>
   <si>
     <t>A</t>
@@ -5883,7 +5880,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:F13"/>
     </sheetView>
   </sheetViews>
@@ -5997,10 +5994,10 @@
     <row r="7" spans="1:8" s="26" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="54"/>
       <c r="B7" s="163" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D7" s="63" t="s">
         <v>97</v>
@@ -6206,13 +6203,13 @@
         <v>70</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K2" s="99" t="s">
         <v>68</v>
       </c>
       <c r="L2" s="99" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M2" s="99" t="s">
         <v>110</v>
@@ -6224,13 +6221,13 @@
         <v>80</v>
       </c>
       <c r="P2" s="99" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q2" s="99" t="s">
         <v>65</v>
       </c>
       <c r="R2" s="99" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="S2" s="99" t="s">
         <v>112</v>
@@ -6245,10 +6242,10 @@
         <v>63</v>
       </c>
       <c r="W2" s="99" t="s">
+        <v>276</v>
+      </c>
+      <c r="X2" s="99" t="s">
         <v>277</v>
-      </c>
-      <c r="X2" s="99" t="s">
-        <v>278</v>
       </c>
       <c r="Y2" s="99" t="s">
         <v>61</v>
@@ -6265,7 +6262,7 @@
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="149" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E3" s="96" t="s">
         <v>59</v>
@@ -7634,7 +7631,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -7664,34 +7661,34 @@
         <v>257</v>
       </c>
       <c r="F2" s="99" t="s">
+        <v>329</v>
+      </c>
+      <c r="G2" s="99" t="s">
         <v>330</v>
       </c>
-      <c r="G2" s="99" t="s">
+      <c r="H2" s="99" t="s">
         <v>331</v>
       </c>
-      <c r="H2" s="99" t="s">
+      <c r="I2" s="99" t="s">
+        <v>338</v>
+      </c>
+      <c r="J2" s="99" t="s">
         <v>332</v>
       </c>
-      <c r="I2" s="99" t="s">
-        <v>339</v>
-      </c>
-      <c r="J2" s="99" t="s">
+      <c r="K2" s="99" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="99" t="s">
+      <c r="L2" s="99" t="s">
+        <v>335</v>
+      </c>
+      <c r="M2" s="99" t="s">
+        <v>336</v>
+      </c>
+      <c r="N2" s="99" t="s">
+        <v>337</v>
+      </c>
+      <c r="O2" s="99" t="s">
         <v>334</v>
-      </c>
-      <c r="L2" s="99" t="s">
-        <v>336</v>
-      </c>
-      <c r="M2" s="99" t="s">
-        <v>337</v>
-      </c>
-      <c r="N2" s="99" t="s">
-        <v>338</v>
-      </c>
-      <c r="O2" s="99" t="s">
-        <v>335</v>
       </c>
       <c r="P2" s="128"/>
     </row>
@@ -8314,8 +8311,8 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8362,34 +8359,34 @@
         <v>257</v>
       </c>
       <c r="F2" s="99" t="s">
+        <v>329</v>
+      </c>
+      <c r="G2" s="99" t="s">
         <v>330</v>
       </c>
-      <c r="G2" s="99" t="s">
+      <c r="H2" s="209" t="s">
         <v>331</v>
       </c>
-      <c r="H2" s="209" t="s">
+      <c r="I2" s="99" t="s">
+        <v>338</v>
+      </c>
+      <c r="J2" s="99" t="s">
         <v>332</v>
       </c>
-      <c r="I2" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="J2" s="99" t="s">
+      <c r="K2" s="209" t="s">
         <v>333</v>
       </c>
-      <c r="K2" s="209" t="s">
+      <c r="L2" s="209" t="s">
+        <v>335</v>
+      </c>
+      <c r="M2" s="209" t="s">
+        <v>336</v>
+      </c>
+      <c r="N2" s="209" t="s">
+        <v>337</v>
+      </c>
+      <c r="O2" s="99" t="s">
         <v>334</v>
-      </c>
-      <c r="L2" s="209" t="s">
-        <v>336</v>
-      </c>
-      <c r="M2" s="209" t="s">
-        <v>337</v>
-      </c>
-      <c r="N2" s="209" t="s">
-        <v>338</v>
-      </c>
-      <c r="O2" s="99" t="s">
-        <v>335</v>
       </c>
       <c r="P2" s="129" t="s">
         <v>138</v>
@@ -8928,13 +8925,13 @@
         <v>70</v>
       </c>
       <c r="J2" s="72" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K2" s="72" t="s">
         <v>68</v>
       </c>
       <c r="L2" s="72" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M2" s="72" t="s">
         <v>110</v>
@@ -8944,13 +8941,13 @@
       </c>
       <c r="O2" s="151"/>
       <c r="P2" s="72" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q2" s="72" t="s">
         <v>65</v>
       </c>
       <c r="R2" s="72" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="S2" s="72" t="s">
         <v>112</v>
@@ -8974,7 +8971,7 @@
         <v>58</v>
       </c>
       <c r="G3" s="74" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H3" s="71" t="e">
         <f>SUMIF(#REF!,#REF!,$G3:G3)</f>
@@ -9024,7 +9021,7 @@
         <v>56</v>
       </c>
       <c r="G4" s="74" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H4" s="71" t="e">
         <f>SUMIF(#REF!,#REF!,$G4:G4)</f>
@@ -9042,7 +9039,7 @@
       </c>
       <c r="M4" s="154"/>
       <c r="N4" s="74" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="O4" s="71" t="e">
         <f>SUMIF(#REF!,#REF!,$G4:N4)</f>
@@ -9059,7 +9056,7 @@
       </c>
       <c r="S4" s="154"/>
       <c r="T4" s="74" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="U4" s="71" t="e">
         <f>SUMIF(#REF!,#REF!,$G4:T4)</f>
@@ -9406,7 +9403,7 @@
         <v>232</v>
       </c>
       <c r="N12" s="74" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="O12" s="71" t="e">
         <f>SUMIF(#REF!,#REF!,$G12:N12)</f>
@@ -9425,7 +9422,7 @@
         <v>236</v>
       </c>
       <c r="T12" s="74" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="U12" s="71" t="e">
         <f>SUMIF(#REF!,#REF!,$G12:T12)</f>
@@ -9469,7 +9466,7 @@
       <c r="R13" s="159"/>
       <c r="S13" s="159"/>
       <c r="T13" s="74" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="U13" s="71" t="e">
         <f>SUMIF(#REF!,#REF!,$G13:T13)</f>
@@ -9614,13 +9611,13 @@
         <v>118</v>
       </c>
       <c r="G17" s="74" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M17" s="143" t="s">
         <v>119</v>
       </c>
       <c r="N17" s="74" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -9766,7 +9763,7 @@
         <v>150</v>
       </c>
       <c r="H4" s="108" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I4" s="108" t="s">
         <v>148</v>
@@ -9775,19 +9772,19 @@
         <v>149</v>
       </c>
       <c r="K4" s="108" t="s">
+        <v>270</v>
+      </c>
+      <c r="L4" s="108" t="s">
         <v>271</v>
       </c>
-      <c r="L4" s="108" t="s">
+      <c r="M4" s="108" t="s">
         <v>272</v>
       </c>
-      <c r="M4" s="108" t="s">
+      <c r="N4" s="108" t="s">
         <v>273</v>
       </c>
-      <c r="N4" s="108" t="s">
+      <c r="O4" s="108" t="s">
         <v>274</v>
-      </c>
-      <c r="O4" s="108" t="s">
-        <v>275</v>
       </c>
       <c r="P4" s="206"/>
     </row>
@@ -10676,7 +10673,7 @@
       <c r="B1" s="130"/>
       <c r="C1" s="130"/>
       <c r="D1" s="192" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E1" s="192"/>
       <c r="F1" s="192"/>
@@ -10778,7 +10775,7 @@
         <v>96</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -11141,142 +11138,142 @@
   <sheetData>
     <row r="1" spans="1:23" ht="112" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>285</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>286</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>132</v>
       </c>
       <c r="D1" s="22" t="s">
+        <v>286</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>287</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>288</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="166" t="s">
+        <v>288</v>
+      </c>
+      <c r="H1" s="166" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="166" t="s">
+      <c r="I1" s="167" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="167" t="s">
+      <c r="J1" s="167" t="s">
         <v>291</v>
       </c>
-      <c r="J1" s="167" t="s">
+      <c r="K1" s="167" t="s">
         <v>292</v>
       </c>
-      <c r="K1" s="167" t="s">
+      <c r="L1" s="168" t="s">
         <v>293</v>
       </c>
-      <c r="L1" s="168" t="s">
+      <c r="M1" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="N1" s="168" t="s">
         <v>295</v>
       </c>
-      <c r="N1" s="168" t="s">
+      <c r="O1" s="169" t="s">
         <v>296</v>
       </c>
-      <c r="O1" s="169" t="s">
+      <c r="P1" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="Q1" s="169" t="s">
         <v>298</v>
       </c>
-      <c r="Q1" s="169" t="s">
+      <c r="R1" s="169" t="s">
         <v>299</v>
       </c>
-      <c r="R1" s="169" t="s">
+      <c r="S1" s="166" t="s">
         <v>300</v>
       </c>
-      <c r="S1" s="166" t="s">
+      <c r="T1" s="166" t="s">
+        <v>326</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="V1" s="171" t="s">
+        <v>324</v>
+      </c>
+      <c r="W1" t="s">
         <v>301</v>
-      </c>
-      <c r="T1" s="166" t="s">
-        <v>327</v>
-      </c>
-      <c r="U1" s="22" t="s">
-        <v>329</v>
-      </c>
-      <c r="V1" s="171" t="s">
-        <v>325</v>
-      </c>
-      <c r="W1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="170" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="170" t="s">
         <v>303</v>
       </c>
-      <c r="B2" s="170" t="s">
+      <c r="C2" s="170" t="s">
         <v>304</v>
       </c>
-      <c r="C2" s="170" t="s">
+      <c r="D2" s="170" t="s">
         <v>305</v>
       </c>
-      <c r="D2" s="170" t="s">
+      <c r="E2" s="170" t="s">
         <v>306</v>
       </c>
-      <c r="E2" s="170" t="s">
+      <c r="F2" s="170" t="s">
         <v>307</v>
       </c>
-      <c r="F2" s="170" t="s">
+      <c r="G2" s="170" t="s">
         <v>308</v>
       </c>
-      <c r="G2" s="170" t="s">
+      <c r="H2" s="170" t="s">
         <v>309</v>
       </c>
-      <c r="H2" s="170" t="s">
+      <c r="I2" s="175" t="s">
         <v>310</v>
       </c>
-      <c r="I2" s="175" t="s">
+      <c r="J2" s="175" t="s">
         <v>311</v>
       </c>
-      <c r="J2" s="175" t="s">
+      <c r="K2" s="173" t="s">
         <v>312</v>
       </c>
-      <c r="K2" s="173" t="s">
+      <c r="L2" s="173" t="s">
         <v>313</v>
       </c>
-      <c r="L2" s="173" t="s">
+      <c r="M2" s="174" t="s">
         <v>314</v>
       </c>
-      <c r="M2" s="174" t="s">
+      <c r="N2" s="176" t="s">
         <v>315</v>
       </c>
-      <c r="N2" s="176" t="s">
+      <c r="O2" s="173" t="s">
         <v>316</v>
       </c>
-      <c r="O2" s="173" t="s">
+      <c r="P2" s="173" t="s">
         <v>317</v>
       </c>
-      <c r="P2" s="173" t="s">
+      <c r="Q2" s="173" t="s">
         <v>318</v>
       </c>
-      <c r="Q2" s="173" t="s">
+      <c r="R2" s="173" t="s">
         <v>319</v>
       </c>
-      <c r="R2" s="173" t="s">
+      <c r="S2" s="173" t="s">
         <v>320</v>
       </c>
-      <c r="S2" s="173" t="s">
+      <c r="T2" s="173" t="s">
+        <v>327</v>
+      </c>
+      <c r="U2" s="173" t="s">
         <v>321</v>
       </c>
-      <c r="T2" s="173" t="s">
-        <v>328</v>
-      </c>
-      <c r="U2" s="173" t="s">
+      <c r="V2" s="172" t="s">
         <v>322</v>
       </c>
-      <c r="V2" s="172" t="s">
+      <c r="W2" t="s">
         <v>323</v>
-      </c>
-      <c r="W2" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
@@ -11904,7 +11901,7 @@
       <c r="B3" s="41"/>
       <c r="C3" s="41"/>
       <c r="D3" s="45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E3" s="96" t="s">
         <v>59</v>

</xml_diff>